<commit_message>
Added notes and subjects like Note:site, Note:edition, Subject:culturalContext, Subject:lithology etc. DM-137
</commit_message>
<xml_diff>
--- a/WebContent/files/xls_standard_input_template.xlsx
+++ b/WebContent/files/xls_standard_input_template.xlsx
@@ -9,14 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
     <sheet name="Select-a-header values" sheetId="14" r:id="rId2"/>
     <sheet name="CV values" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -34,13 +34,13 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>COLLECTION RECORD ONLY</t>
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Q1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
             <sz val="9"/>
             <color indexed="81"/>
             <rFont val="Tahoma"/>
-            <charset val="1"/>
+            <family val="2"/>
           </rPr>
           <t>COLLECTION RECORD ONLY</t>
         </r>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="641" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="633">
   <si>
     <t>text</t>
   </si>
@@ -2036,13 +2036,37 @@
   </si>
   <si>
     <t>CLR image file name</t>
+  </si>
+  <si>
+    <t>Subject:culturalContext</t>
+  </si>
+  <si>
+    <t>Subject:lithology</t>
+  </si>
+  <si>
+    <t>Subject:series</t>
+  </si>
+  <si>
+    <t>Subject:cruise</t>
+  </si>
+  <si>
+    <t>Note:site</t>
+  </si>
+  <si>
+    <t>Note:edition</t>
+  </si>
+  <si>
+    <t>Note:funding</t>
+  </si>
+  <si>
+    <t>Note:related publications</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="32" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2260,11 +2284,17 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="9"/>
-      <color indexed="81"/>
-      <name val="Tahoma"/>
-      <charset val="1"/>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="38">
@@ -2661,7 +2691,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2699,10 +2729,13 @@
     <xf numFmtId="49" fontId="16" fillId="36" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="36" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="13" fillId="37" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="49" fontId="14" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3103,10 +3136,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V1"/>
+  <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3119,21 +3152,20 @@
     <col min="6" max="6" width="19.7109375" style="3" customWidth="1"/>
     <col min="7" max="7" width="23.85546875" style="3" customWidth="1"/>
     <col min="8" max="8" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="30.5703125" style="3" customWidth="1"/>
-    <col min="10" max="10" width="22" style="3" customWidth="1"/>
-    <col min="11" max="11" width="51.5703125" style="3" customWidth="1"/>
-    <col min="12" max="13" width="45.140625" style="3" customWidth="1"/>
-    <col min="14" max="14" width="45.5703125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="14.85546875" style="3" customWidth="1"/>
-    <col min="16" max="16" width="15.140625" style="3" customWidth="1"/>
-    <col min="17" max="17" width="19.85546875" style="3" customWidth="1"/>
-    <col min="18" max="19" width="39.140625" style="3" customWidth="1"/>
-    <col min="20" max="20" width="42.85546875" style="3" customWidth="1"/>
-    <col min="21" max="21" width="44.5703125" style="3" customWidth="1"/>
-    <col min="22" max="22" width="84.28515625" style="3" customWidth="1"/>
+    <col min="9" max="9" width="22" style="3" customWidth="1"/>
+    <col min="10" max="10" width="51.5703125" style="3" customWidth="1"/>
+    <col min="11" max="12" width="45.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="45.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" style="3" customWidth="1"/>
+    <col min="17" max="18" width="39.140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="42.85546875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="44.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3152,52 +3184,49 @@
       <c r="F1" s="16" t="s">
         <v>502</v>
       </c>
-      <c r="G1" s="18" t="s">
+      <c r="G1" s="17" t="s">
         <v>624</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="I1" s="17" t="s">
-        <v>349</v>
+      <c r="I1" s="15" t="s">
+        <v>8</v>
       </c>
       <c r="J1" s="15" t="s">
-        <v>8</v>
-      </c>
-      <c r="K1" s="15" t="s">
         <v>517</v>
       </c>
+      <c r="K1" s="16" t="s">
+        <v>518</v>
+      </c>
       <c r="L1" s="16" t="s">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="M1" s="16" t="s">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="N1" s="16" t="s">
-        <v>520</v>
+        <v>6</v>
       </c>
       <c r="O1" s="16" t="s">
-        <v>6</v>
-      </c>
-      <c r="P1" s="16" t="s">
         <v>7</v>
       </c>
-      <c r="Q1" s="18" t="s">
+      <c r="P1" s="17" t="s">
         <v>623</v>
       </c>
+      <c r="Q1" s="16" t="s">
+        <v>521</v>
+      </c>
       <c r="R1" s="16" t="s">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="S1" s="16" t="s">
-        <v>522</v>
+        <v>523</v>
       </c>
       <c r="T1" s="16" t="s">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="U1" s="16" t="s">
-        <v>524</v>
-      </c>
-      <c r="V1" s="16" t="s">
         <v>525</v>
       </c>
     </row>
@@ -3219,17 +3248,16 @@
       <formula>NOT(ISERROR(SEARCH("    \Sub-component",B1)))</formula>
     </cfRule>
   </conditionalFormatting>
-  <dataValidations count="3">
+  <dataValidations count="2">
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list" sqref="B1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="J1"/>
-    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a value from the drop-down list" sqref="I1"/>
+    <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="I1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="14">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
@@ -3252,67 +3280,61 @@
           <x14:formula1>
             <xm:f>'Select-a-header values'!$A$1:$A$7</xm:f>
           </x14:formula1>
-          <xm:sqref>K1</xm:sqref>
+          <xm:sqref>J1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'CV values'!$D$2:$D$60</xm:f>
           </x14:formula1>
-          <xm:sqref>J2:J1048576</xm:sqref>
+          <xm:sqref>I2:I1048576</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$C$1:$C$185</xm:f>
           </x14:formula1>
-          <xm:sqref>M1</xm:sqref>
+          <xm:sqref>L1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
             <xm:f>'Select-a-header values'!$D$1:$D$6</xm:f>
           </x14:formula1>
-          <xm:sqref>N1</xm:sqref>
+          <xm:sqref>M1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$E$1:$E$31</xm:f>
+            <xm:f>'Select-a-header values'!$G$1:$G$13</xm:f>
+          </x14:formula1>
+          <xm:sqref>S1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
+          <x14:formula1>
+            <xm:f>'Select-a-header values'!$H$1:$H$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>T1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
+          <x14:formula1>
+            <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
+          </x14:formula1>
+          <xm:sqref>U1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
+          <x14:formula1>
+            <xm:f>'Select-a-header values'!$B$1:$B$233</xm:f>
+          </x14:formula1>
+          <xm:sqref>K1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
+          <x14:formula1>
+            <xm:f>'Select-a-header values'!$F$1:$F$20</xm:f>
           </x14:formula1>
           <xm:sqref>R1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$G$1:$G$13</xm:f>
+            <xm:f>'Select-a-header values'!$E$1:$E$29</xm:f>
           </x14:formula1>
-          <xm:sqref>T1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$H$1:$H$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>U1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$I$1:$I$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>V1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a value from the drop-down list">
-          <x14:formula1>
-            <xm:f>'CV values'!$E$2:$E$5</xm:f>
-          </x14:formula1>
-          <xm:sqref>I2:I1048576</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$B$1:$B$233</xm:f>
-          </x14:formula1>
-          <xm:sqref>L1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
-            <xm:f>'Select-a-header values'!$F$1:$F$20</xm:f>
-          </x14:formula1>
-          <xm:sqref>S1</xm:sqref>
+          <xm:sqref>Q1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3324,8 +3346,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R333"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3502,8 +3524,8 @@
       <c r="F6" s="11" t="s">
         <v>12</v>
       </c>
-      <c r="G6" s="11" t="s">
-        <v>337</v>
+      <c r="G6" s="18" t="s">
+        <v>628</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>456</v>
@@ -3528,8 +3550,8 @@
       <c r="F7" s="11" t="s">
         <v>454</v>
       </c>
-      <c r="G7" s="12" t="s">
-        <v>451</v>
+      <c r="G7" s="21" t="s">
+        <v>625</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>458</v>
@@ -3551,8 +3573,8 @@
       <c r="F8" s="11" t="s">
         <v>493</v>
       </c>
-      <c r="G8" s="12" t="s">
-        <v>455</v>
+      <c r="G8" s="11" t="s">
+        <v>337</v>
       </c>
       <c r="H8" s="11"/>
       <c r="I8" s="11" t="s">
@@ -3566,14 +3588,14 @@
       <c r="C9" s="14" t="s">
         <v>535</v>
       </c>
-      <c r="E9" s="11" t="s">
-        <v>349</v>
+      <c r="E9" s="18" t="s">
+        <v>630</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>503</v>
       </c>
-      <c r="G9" s="11" t="s">
-        <v>335</v>
+      <c r="G9" s="12" t="s">
+        <v>451</v>
       </c>
       <c r="H9" s="11"/>
       <c r="I9" s="11" t="s">
@@ -3594,7 +3616,7 @@
         <v>14</v>
       </c>
       <c r="G10" s="12" t="s">
-        <v>459</v>
+        <v>455</v>
       </c>
       <c r="H10" s="11"/>
       <c r="I10" s="11" t="s">
@@ -3608,14 +3630,14 @@
       <c r="C11" s="14" t="s">
         <v>537</v>
       </c>
-      <c r="E11" s="11" t="s">
-        <v>461</v>
+      <c r="E11" s="18" t="s">
+        <v>631</v>
       </c>
       <c r="F11" s="11" t="s">
         <v>494</v>
       </c>
-      <c r="G11" s="12" t="s">
-        <v>512</v>
+      <c r="G11" s="21" t="s">
+        <v>626</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
@@ -3630,13 +3652,13 @@
         <v>38</v>
       </c>
       <c r="E12" s="11" t="s">
-        <v>339</v>
+        <v>461</v>
       </c>
       <c r="F12" s="11" t="s">
         <v>15</v>
       </c>
       <c r="G12" s="11" t="s">
-        <v>334</v>
+        <v>335</v>
       </c>
       <c r="H12" s="11"/>
       <c r="I12" s="11" t="s">
@@ -3651,13 +3673,13 @@
         <v>538</v>
       </c>
       <c r="E13" s="11" t="s">
-        <v>462</v>
+        <v>339</v>
       </c>
       <c r="F13" s="11" t="s">
         <v>495</v>
       </c>
       <c r="G13" s="12" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
@@ -3670,10 +3692,13 @@
         <v>539</v>
       </c>
       <c r="E14" s="11" t="s">
-        <v>505</v>
+        <v>462</v>
       </c>
       <c r="F14" s="11" t="s">
         <v>5</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>512</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -3684,10 +3709,13 @@
         <v>540</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>506</v>
+        <v>505</v>
       </c>
       <c r="F15" s="11" t="s">
         <v>16</v>
+      </c>
+      <c r="G15" s="21" t="s">
+        <v>627</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -3698,13 +3726,16 @@
         <v>541</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>507</v>
+        <v>506</v>
       </c>
       <c r="F16" s="11" t="s">
         <v>496</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G16" s="11" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>37</v>
       </c>
@@ -3712,13 +3743,16 @@
         <v>542</v>
       </c>
       <c r="E17" s="11" t="s">
-        <v>463</v>
+        <v>507</v>
       </c>
       <c r="F17" s="11" t="s">
         <v>17</v>
       </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="G17" s="12" t="s">
+        <v>460</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>40</v>
       </c>
@@ -3726,13 +3760,13 @@
         <v>29</v>
       </c>
       <c r="E18" s="11" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
       <c r="F18" s="11" t="s">
         <v>516</v>
       </c>
     </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>41</v>
       </c>
@@ -3740,38 +3774,38 @@
         <v>56</v>
       </c>
       <c r="E19" s="11" t="s">
-        <v>508</v>
+        <v>464</v>
       </c>
       <c r="F19" s="11" t="s">
         <v>504</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>45</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="12" t="s">
-        <v>484</v>
+      <c r="E20" s="11" t="s">
+        <v>508</v>
       </c>
       <c r="F20" s="11" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>31</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>543</v>
       </c>
-      <c r="E21" s="11" t="s">
-        <v>351</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E21" s="12" t="s">
+        <v>484</v>
+      </c>
+    </row>
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>24</v>
       </c>
@@ -3779,10 +3813,10 @@
         <v>51</v>
       </c>
       <c r="E22" s="11" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.25">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
         <v>42</v>
       </c>
@@ -3790,10 +3824,10 @@
         <v>53</v>
       </c>
       <c r="E23" s="11" t="s">
-        <v>352</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.25">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
         <v>43</v>
       </c>
@@ -3801,10 +3835,10 @@
         <v>49</v>
       </c>
       <c r="E24" s="11" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
         <v>39</v>
       </c>
@@ -3812,21 +3846,21 @@
         <v>58</v>
       </c>
       <c r="E25" s="11" t="s">
-        <v>354</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
         <v>28</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="11" t="s">
-        <v>465</v>
-      </c>
-    </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E26" s="18" t="s">
+        <v>632</v>
+      </c>
+    </row>
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
         <v>55</v>
       </c>
@@ -3834,10 +3868,10 @@
         <v>59</v>
       </c>
       <c r="E27" s="11" t="s">
-        <v>355</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.25">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>46</v>
       </c>
@@ -3845,21 +3879,21 @@
         <v>544</v>
       </c>
       <c r="E28" s="11" t="s">
-        <v>356</v>
-      </c>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.25">
+        <v>465</v>
+      </c>
+    </row>
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>54</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>545</v>
       </c>
-      <c r="E29" s="11" t="s">
-        <v>509</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="E29" s="18" t="s">
+        <v>629</v>
+      </c>
+    </row>
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>50</v>
       </c>
@@ -3867,10 +3901,10 @@
         <v>77</v>
       </c>
       <c r="E30" s="11" t="s">
-        <v>357</v>
-      </c>
-    </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.25">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>52</v>
       </c>
@@ -3878,34 +3912,43 @@
         <v>67</v>
       </c>
       <c r="E31" s="11" t="s">
-        <v>466</v>
-      </c>
-    </row>
-    <row r="32" spans="2:6" x14ac:dyDescent="0.25">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>48</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="33" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E32" s="11" t="s">
+        <v>509</v>
+      </c>
+    </row>
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
         <v>57</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="34" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E33" s="11" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
         <v>61</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>546</v>
       </c>
-    </row>
-    <row r="35" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E34" s="11" t="s">
+        <v>466</v>
+      </c>
+    </row>
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
         <v>60</v>
       </c>
@@ -3913,31 +3956,34 @@
         <v>547</v>
       </c>
     </row>
-    <row r="36" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
         <v>68</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>548</v>
       </c>
-    </row>
-    <row r="37" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E36" s="20"/>
+    </row>
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
         <v>106</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>111</v>
       </c>
-    </row>
-    <row r="38" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E37" s="18"/>
+    </row>
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
         <v>63</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>549</v>
       </c>
-    </row>
-    <row r="39" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="E38" s="19"/>
+    </row>
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
         <v>76</v>
       </c>
@@ -3945,7 +3991,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
         <v>65</v>
       </c>
@@ -3953,7 +3999,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
         <v>75</v>
       </c>
@@ -3961,7 +4007,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="42" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
         <v>66</v>
       </c>
@@ -3969,7 +4015,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="43" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
         <v>83</v>
       </c>
@@ -3977,7 +4023,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="44" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
         <v>79</v>
       </c>
@@ -3985,7 +4031,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="45" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
         <v>70</v>
       </c>
@@ -3993,7 +4039,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="46" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
         <v>69</v>
       </c>
@@ -4001,7 +4047,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="47" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
         <v>71</v>
       </c>
@@ -4009,7 +4055,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
         <v>110</v>
       </c>
@@ -5702,6 +5748,9 @@
       <c r="C333"/>
     </row>
   </sheetData>
+  <sortState ref="G2:G17">
+    <sortCondition ref="G2"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
@@ -5712,7 +5761,7 @@
   <dimension ref="A1:F63"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added the Subject Import tool to import subjects and names from Excel source. DM-136
</commit_message>
<xml_diff>
--- a/WebContent/files/xls_standard_input_template.xlsx
+++ b/WebContent/files/xls_standard_input_template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MSD\DOMM\Excel standard input\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="16700" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
     <sheet name="Select-a-header values" sheetId="14" r:id="rId2"/>
     <sheet name="CV values" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -26,7 +26,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="650">
   <si>
     <t>text</t>
   </si>
@@ -2060,13 +2060,64 @@
   </si>
   <si>
     <t>Note:related publications</t>
+  </si>
+  <si>
+    <t>subject type</t>
+  </si>
+  <si>
+    <t>anatomy</t>
+  </si>
+  <si>
+    <t>common name</t>
+  </si>
+  <si>
+    <t>conference name</t>
+  </si>
+  <si>
+    <t>corporate name</t>
+  </si>
+  <si>
+    <t>cruise</t>
+  </si>
+  <si>
+    <t>culturalContext</t>
+  </si>
+  <si>
+    <t>family name</t>
+  </si>
+  <si>
+    <t>genre</t>
+  </si>
+  <si>
+    <t>geographic</t>
+  </si>
+  <si>
+    <t>lithology</t>
+  </si>
+  <si>
+    <t>occupation</t>
+  </si>
+  <si>
+    <t>personal name</t>
+  </si>
+  <si>
+    <t>scientific name</t>
+  </si>
+  <si>
+    <t>series</t>
+  </si>
+  <si>
+    <t>temporal</t>
+  </si>
+  <si>
+    <t>topic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="35" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2292,6 +2343,22 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2638,7 +2705,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="51">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2690,6 +2757,8 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2737,7 +2806,7 @@
     <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="51">
+  <cellStyles count="53">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2766,11 +2835,13 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="48"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -2892,7 +2963,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2927,7 +2998,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3142,30 +3213,30 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" style="3" customWidth="1"/>
-    <col min="10" max="10" width="51.5703125" style="3" customWidth="1"/>
-    <col min="11" max="12" width="45.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="45.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" style="3" customWidth="1"/>
-    <col min="17" max="18" width="39.140625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="42.85546875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="44.5703125" style="3" customWidth="1"/>
-    <col min="21" max="21" width="84.28515625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="51.5" style="3" customWidth="1"/>
+    <col min="11" max="12" width="45.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="45.5" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" style="3" customWidth="1"/>
+    <col min="17" max="18" width="39.1640625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="42.83203125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="44.5" style="3" customWidth="1"/>
+    <col min="21" max="21" width="84.33203125" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="22.5" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3253,8 +3324,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="I1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
@@ -3338,6 +3409,9 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
   </extLst>
 </worksheet>
 </file>
@@ -3346,21 +3420,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="G1" sqref="G1:G1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="41.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="43.7109375" style="14" customWidth="1"/>
-    <col min="6" max="18" width="38.5703125" style="14"/>
-    <col min="19" max="16384" width="38.5703125" style="11"/>
+    <col min="1" max="1" width="21.1640625" style="14" customWidth="1"/>
+    <col min="2" max="3" width="41.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="43.6640625" style="14" customWidth="1"/>
+    <col min="6" max="18" width="38.5" style="14"/>
+    <col min="19" max="16384" width="38.5" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="14" t="s">
         <v>517</v>
       </c>
@@ -3389,7 +3463,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -3418,7 +3492,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="14" t="s">
         <v>445</v>
       </c>
@@ -3447,7 +3521,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="14" t="s">
         <v>447</v>
       </c>
@@ -3476,7 +3550,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
         <v>449</v>
       </c>
@@ -3505,7 +3579,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="14" t="s">
         <v>453</v>
       </c>
@@ -3534,7 +3608,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="14" t="s">
         <v>457</v>
       </c>
@@ -3560,7 +3634,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="B8" s="14" t="s">
         <v>27</v>
       </c>
@@ -3581,7 +3655,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
@@ -3602,7 +3676,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="B10" s="14" t="s">
         <v>32</v>
       </c>
@@ -3623,7 +3697,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
@@ -3644,7 +3718,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="B12" s="14" t="s">
         <v>20</v>
       </c>
@@ -3665,7 +3739,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="B13" s="14" t="s">
         <v>22</v>
       </c>
@@ -3684,7 +3758,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="B14" s="14" t="s">
         <v>35</v>
       </c>
@@ -3701,7 +3775,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="B15" s="14" t="s">
         <v>33</v>
       </c>
@@ -3718,7 +3792,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="B16" s="14" t="s">
         <v>36</v>
       </c>
@@ -3735,7 +3809,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:7">
       <c r="B17" s="14" t="s">
         <v>37</v>
       </c>
@@ -3752,7 +3826,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:7">
       <c r="B18" s="14" t="s">
         <v>40</v>
       </c>
@@ -3766,7 +3840,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7">
       <c r="B19" s="14" t="s">
         <v>41</v>
       </c>
@@ -3780,7 +3854,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7">
       <c r="B20" s="14" t="s">
         <v>45</v>
       </c>
@@ -3794,7 +3868,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7">
       <c r="B21" s="14" t="s">
         <v>31</v>
       </c>
@@ -3805,7 +3879,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7">
       <c r="B22" s="14" t="s">
         <v>24</v>
       </c>
@@ -3816,7 +3890,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7">
       <c r="B23" s="14" t="s">
         <v>42</v>
       </c>
@@ -3827,7 +3901,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7">
       <c r="B24" s="14" t="s">
         <v>43</v>
       </c>
@@ -3838,7 +3912,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7">
       <c r="B25" s="14" t="s">
         <v>39</v>
       </c>
@@ -3849,7 +3923,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7">
       <c r="B26" s="14" t="s">
         <v>28</v>
       </c>
@@ -3860,7 +3934,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7">
       <c r="B27" s="14" t="s">
         <v>55</v>
       </c>
@@ -3871,7 +3945,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7">
       <c r="B28" s="14" t="s">
         <v>46</v>
       </c>
@@ -3882,7 +3956,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7">
       <c r="B29" s="14" t="s">
         <v>54</v>
       </c>
@@ -3893,7 +3967,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7">
       <c r="B30" s="14" t="s">
         <v>50</v>
       </c>
@@ -3904,7 +3978,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7">
       <c r="B31" s="14" t="s">
         <v>52</v>
       </c>
@@ -3915,7 +3989,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7">
       <c r="B32" s="14" t="s">
         <v>48</v>
       </c>
@@ -3926,7 +4000,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5">
       <c r="B33" s="14" t="s">
         <v>57</v>
       </c>
@@ -3937,7 +4011,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5">
       <c r="B34" s="14" t="s">
         <v>61</v>
       </c>
@@ -3948,7 +4022,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5">
       <c r="B35" s="14" t="s">
         <v>60</v>
       </c>
@@ -3956,7 +4030,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5">
       <c r="B36" s="14" t="s">
         <v>68</v>
       </c>
@@ -3965,7 +4039,7 @@
       </c>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5">
       <c r="B37" s="14" t="s">
         <v>106</v>
       </c>
@@ -3974,7 +4048,7 @@
       </c>
       <c r="E37" s="18"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5">
       <c r="B38" s="14" t="s">
         <v>63</v>
       </c>
@@ -3983,7 +4057,7 @@
       </c>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5">
       <c r="B39" s="14" t="s">
         <v>76</v>
       </c>
@@ -3991,7 +4065,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5">
       <c r="B40" s="14" t="s">
         <v>65</v>
       </c>
@@ -3999,7 +4073,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5">
       <c r="B41" s="14" t="s">
         <v>75</v>
       </c>
@@ -4007,7 +4081,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5">
       <c r="B42" s="14" t="s">
         <v>66</v>
       </c>
@@ -4015,7 +4089,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5">
       <c r="B43" s="14" t="s">
         <v>83</v>
       </c>
@@ -4023,7 +4097,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:5">
       <c r="B44" s="14" t="s">
         <v>79</v>
       </c>
@@ -4031,7 +4105,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:5">
       <c r="B45" s="14" t="s">
         <v>70</v>
       </c>
@@ -4039,7 +4113,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5">
       <c r="B46" s="14" t="s">
         <v>69</v>
       </c>
@@ -4047,7 +4121,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5">
       <c r="B47" s="14" t="s">
         <v>71</v>
       </c>
@@ -4055,7 +4129,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5">
       <c r="B48" s="14" t="s">
         <v>110</v>
       </c>
@@ -4063,7 +4137,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3">
       <c r="B49" s="14" t="s">
         <v>81</v>
       </c>
@@ -4071,7 +4145,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3">
       <c r="B50" s="14" t="s">
         <v>72</v>
       </c>
@@ -4079,7 +4153,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3">
       <c r="B51" s="14" t="s">
         <v>73</v>
       </c>
@@ -4087,7 +4161,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3">
       <c r="B52" s="14" t="s">
         <v>64</v>
       </c>
@@ -4095,7 +4169,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3">
       <c r="B53" s="14" t="s">
         <v>74</v>
       </c>
@@ -4103,7 +4177,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3">
       <c r="B54" s="14" t="s">
         <v>82</v>
       </c>
@@ -4111,7 +4185,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3">
       <c r="B55" s="14" t="s">
         <v>101</v>
       </c>
@@ -4119,7 +4193,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3">
       <c r="B56" s="14" t="s">
         <v>102</v>
       </c>
@@ -4127,7 +4201,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3">
       <c r="B57" s="14" t="s">
         <v>107</v>
       </c>
@@ -4135,7 +4209,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3">
       <c r="B58" s="14" t="s">
         <v>104</v>
       </c>
@@ -4143,7 +4217,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3">
       <c r="B59" s="14" t="s">
         <v>467</v>
       </c>
@@ -4151,7 +4225,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3">
       <c r="B60" s="14" t="s">
         <v>90</v>
       </c>
@@ -4159,7 +4233,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3">
       <c r="B61" s="14" t="s">
         <v>92</v>
       </c>
@@ -4167,7 +4241,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3">
       <c r="B62" s="14" t="s">
         <v>99</v>
       </c>
@@ -4175,7 +4249,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3">
       <c r="B63" s="14" t="s">
         <v>98</v>
       </c>
@@ -4183,7 +4257,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3">
       <c r="B64" s="14" t="s">
         <v>103</v>
       </c>
@@ -4191,7 +4265,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3">
       <c r="B65" s="14" t="s">
         <v>87</v>
       </c>
@@ -4199,7 +4273,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3">
       <c r="B66" s="14" t="s">
         <v>100</v>
       </c>
@@ -4207,7 +4281,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3">
       <c r="B67" s="14" t="s">
         <v>89</v>
       </c>
@@ -4215,7 +4289,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3">
       <c r="B68" s="14" t="s">
         <v>96</v>
       </c>
@@ -4223,7 +4297,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3">
       <c r="B69" s="14" t="s">
         <v>109</v>
       </c>
@@ -4231,7 +4305,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3">
       <c r="B70" s="14" t="s">
         <v>117</v>
       </c>
@@ -4239,7 +4313,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3">
       <c r="B71" s="14" t="s">
         <v>129</v>
       </c>
@@ -4247,7 +4321,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3">
       <c r="B72" s="14" t="s">
         <v>132</v>
       </c>
@@ -4255,7 +4329,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3">
       <c r="B73" s="14" t="s">
         <v>131</v>
       </c>
@@ -4263,7 +4337,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3">
       <c r="B74" s="14" t="s">
         <v>133</v>
       </c>
@@ -4271,7 +4345,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3">
       <c r="B75" s="14" t="s">
         <v>114</v>
       </c>
@@ -4279,7 +4353,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3">
       <c r="B76" s="14" t="s">
         <v>116</v>
       </c>
@@ -4287,7 +4361,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3">
       <c r="B77" s="14" t="s">
         <v>120</v>
       </c>
@@ -4295,7 +4369,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3">
       <c r="B78" s="14" t="s">
         <v>121</v>
       </c>
@@ -4303,7 +4377,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3">
       <c r="B79" s="14" t="s">
         <v>125</v>
       </c>
@@ -4311,7 +4385,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3">
       <c r="B80" s="14" t="s">
         <v>124</v>
       </c>
@@ -4319,7 +4393,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3">
       <c r="B81" s="14" t="s">
         <v>115</v>
       </c>
@@ -4327,7 +4401,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3">
       <c r="B82" s="14" t="s">
         <v>127</v>
       </c>
@@ -4335,7 +4409,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3">
       <c r="B83" s="14" t="s">
         <v>118</v>
       </c>
@@ -4343,7 +4417,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3">
       <c r="B84" s="14" t="s">
         <v>123</v>
       </c>
@@ -4351,7 +4425,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3">
       <c r="B85" s="14" t="s">
         <v>134</v>
       </c>
@@ -4359,7 +4433,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3">
       <c r="B86" s="14" t="s">
         <v>137</v>
       </c>
@@ -4367,7 +4441,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3">
       <c r="B87" s="14" t="s">
         <v>135</v>
       </c>
@@ -4375,7 +4449,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3">
       <c r="B88" s="14" t="s">
         <v>136</v>
       </c>
@@ -4383,7 +4457,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3">
       <c r="B89" s="14" t="s">
         <v>139</v>
       </c>
@@ -4391,7 +4465,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3">
       <c r="B90" s="14" t="s">
         <v>140</v>
       </c>
@@ -4399,7 +4473,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3">
       <c r="B91" s="14" t="s">
         <v>142</v>
       </c>
@@ -4407,7 +4481,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3">
       <c r="B92" s="14" t="s">
         <v>141</v>
       </c>
@@ -4415,7 +4489,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3">
       <c r="B93" s="14" t="s">
         <v>138</v>
       </c>
@@ -4423,7 +4497,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3">
       <c r="B94" s="14" t="s">
         <v>144</v>
       </c>
@@ -4431,7 +4505,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3">
       <c r="B95" s="14" t="s">
         <v>146</v>
       </c>
@@ -4439,7 +4513,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3">
       <c r="B96" s="14" t="s">
         <v>147</v>
       </c>
@@ -4447,7 +4521,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3">
       <c r="B97" s="14" t="s">
         <v>469</v>
       </c>
@@ -4455,7 +4529,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3">
       <c r="B98" s="14" t="s">
         <v>150</v>
       </c>
@@ -4463,7 +4537,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3">
       <c r="B99" s="14" t="s">
         <v>152</v>
       </c>
@@ -4471,7 +4545,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3">
       <c r="B100" s="14" t="s">
         <v>148</v>
       </c>
@@ -4479,7 +4553,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3">
       <c r="B101" s="14" t="s">
         <v>151</v>
       </c>
@@ -4487,7 +4561,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3">
       <c r="B102" s="14" t="s">
         <v>156</v>
       </c>
@@ -4495,7 +4569,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3">
       <c r="B103" s="14" t="s">
         <v>153</v>
       </c>
@@ -4503,7 +4577,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3">
       <c r="B104" s="14" t="s">
         <v>160</v>
       </c>
@@ -4511,7 +4585,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3">
       <c r="B105" s="14" t="s">
         <v>162</v>
       </c>
@@ -4519,7 +4593,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3">
       <c r="B106" s="14" t="s">
         <v>154</v>
       </c>
@@ -4527,7 +4601,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3">
       <c r="B107" s="14" t="s">
         <v>158</v>
       </c>
@@ -4535,7 +4609,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3">
       <c r="B108" s="14" t="s">
         <v>163</v>
       </c>
@@ -4543,7 +4617,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3">
       <c r="B109" s="14" t="s">
         <v>165</v>
       </c>
@@ -4551,7 +4625,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3">
       <c r="B110" s="14" t="s">
         <v>166</v>
       </c>
@@ -4559,7 +4633,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3">
       <c r="B111" s="14" t="s">
         <v>170</v>
       </c>
@@ -4567,7 +4641,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3">
       <c r="B112" s="14" t="s">
         <v>168</v>
       </c>
@@ -4575,7 +4649,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3">
       <c r="B113" s="14" t="s">
         <v>172</v>
       </c>
@@ -4583,7 +4657,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3">
       <c r="B114" s="14" t="s">
         <v>176</v>
       </c>
@@ -4591,7 +4665,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3">
       <c r="B115" s="14" t="s">
         <v>177</v>
       </c>
@@ -4599,7 +4673,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3">
       <c r="B116" s="14" t="s">
         <v>178</v>
       </c>
@@ -4607,7 +4681,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3">
       <c r="B117" s="14" t="s">
         <v>174</v>
       </c>
@@ -4615,7 +4689,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3">
       <c r="B118" s="14" t="s">
         <v>180</v>
       </c>
@@ -4623,7 +4697,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3">
       <c r="B119" s="14" t="s">
         <v>470</v>
       </c>
@@ -4631,7 +4705,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3">
       <c r="B120" s="14" t="s">
         <v>183</v>
       </c>
@@ -4639,7 +4713,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3">
       <c r="B121" s="14" t="s">
         <v>188</v>
       </c>
@@ -4647,7 +4721,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3">
       <c r="B122" s="14" t="s">
         <v>184</v>
       </c>
@@ -4655,7 +4729,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3">
       <c r="B123" s="14" t="s">
         <v>185</v>
       </c>
@@ -4663,7 +4737,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3">
       <c r="B124" s="14" t="s">
         <v>182</v>
       </c>
@@ -4671,7 +4745,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3">
       <c r="B125" s="14" t="s">
         <v>189</v>
       </c>
@@ -4679,7 +4753,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3">
       <c r="B126" s="14" t="s">
         <v>191</v>
       </c>
@@ -4687,7 +4761,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3">
       <c r="B127" s="14" t="s">
         <v>187</v>
       </c>
@@ -4695,7 +4769,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3">
       <c r="B128" s="14" t="s">
         <v>193</v>
       </c>
@@ -4703,7 +4777,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3">
       <c r="B129" s="14" t="s">
         <v>194</v>
       </c>
@@ -4711,7 +4785,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3">
       <c r="B130" s="14" t="s">
         <v>201</v>
       </c>
@@ -4719,7 +4793,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3">
       <c r="B131" s="14" t="s">
         <v>206</v>
       </c>
@@ -4727,7 +4801,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3">
       <c r="B132" s="14" t="s">
         <v>207</v>
       </c>
@@ -4735,7 +4809,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3">
       <c r="B133" s="14" t="s">
         <v>198</v>
       </c>
@@ -4743,7 +4817,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3">
       <c r="B134" s="14" t="s">
         <v>196</v>
       </c>
@@ -4751,7 +4825,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3">
       <c r="B135" s="14" t="s">
         <v>209</v>
       </c>
@@ -4759,7 +4833,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3">
       <c r="B136" s="14" t="s">
         <v>210</v>
       </c>
@@ -4767,7 +4841,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3">
       <c r="B137" s="14" t="s">
         <v>203</v>
       </c>
@@ -4775,7 +4849,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3">
       <c r="B138" s="14" t="s">
         <v>204</v>
       </c>
@@ -4783,7 +4857,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3">
       <c r="B139" s="14" t="s">
         <v>195</v>
       </c>
@@ -4791,7 +4865,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3">
       <c r="B140" s="14" t="s">
         <v>208</v>
       </c>
@@ -4799,7 +4873,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:3">
       <c r="B141" s="14" t="s">
         <v>211</v>
       </c>
@@ -4807,7 +4881,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:3">
       <c r="B142" s="14" t="s">
         <v>212</v>
       </c>
@@ -4815,7 +4889,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:3">
       <c r="B143" s="14" t="s">
         <v>219</v>
       </c>
@@ -4823,7 +4897,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:3">
       <c r="B144" s="14" t="s">
         <v>213</v>
       </c>
@@ -4831,7 +4905,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3">
       <c r="B145" s="14" t="s">
         <v>217</v>
       </c>
@@ -4839,7 +4913,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3">
       <c r="B146" s="14" t="s">
         <v>215</v>
       </c>
@@ -4847,7 +4921,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3">
       <c r="B147" s="14" t="s">
         <v>220</v>
       </c>
@@ -4855,7 +4929,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3">
       <c r="B148" s="14" t="s">
         <v>222</v>
       </c>
@@ -4863,7 +4937,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3">
       <c r="B149" s="14" t="s">
         <v>622</v>
       </c>
@@ -4871,7 +4945,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3">
       <c r="B150" s="14" t="s">
         <v>224</v>
       </c>
@@ -4879,7 +4953,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3">
       <c r="B151" s="14" t="s">
         <v>239</v>
       </c>
@@ -4887,7 +4961,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3">
       <c r="B152" s="14" t="s">
         <v>261</v>
       </c>
@@ -4895,7 +4969,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3">
       <c r="B153" s="14" t="s">
         <v>263</v>
       </c>
@@ -4903,7 +4977,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:3">
       <c r="B154" s="14" t="s">
         <v>225</v>
       </c>
@@ -4911,7 +4985,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:3">
       <c r="B155" s="14" t="s">
         <v>247</v>
       </c>
@@ -4919,7 +4993,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:3">
       <c r="B156" s="14" t="s">
         <v>231</v>
       </c>
@@ -4927,7 +5001,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:3">
       <c r="B157" s="14" t="s">
         <v>232</v>
       </c>
@@ -4935,7 +5009,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:3">
       <c r="B158" s="14" t="s">
         <v>241</v>
       </c>
@@ -4943,7 +5017,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:3">
       <c r="B159" s="14" t="s">
         <v>246</v>
       </c>
@@ -4951,7 +5025,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:3">
       <c r="B160" s="14" t="s">
         <v>471</v>
       </c>
@@ -4959,7 +5033,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:3">
       <c r="B161" s="14" t="s">
         <v>257</v>
       </c>
@@ -4967,7 +5041,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:3">
       <c r="B162" s="14" t="s">
         <v>237</v>
       </c>
@@ -4975,7 +5049,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:3">
       <c r="B163" s="14" t="s">
         <v>249</v>
       </c>
@@ -4983,7 +5057,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:3">
       <c r="B164" s="14" t="s">
         <v>243</v>
       </c>
@@ -4991,7 +5065,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:3">
       <c r="B165" s="14" t="s">
         <v>252</v>
       </c>
@@ -4999,7 +5073,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:3">
       <c r="B166" s="14" t="s">
         <v>255</v>
       </c>
@@ -5007,7 +5081,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:3">
       <c r="B167" s="14" t="s">
         <v>235</v>
       </c>
@@ -5015,7 +5089,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:3">
       <c r="B168" s="14" t="s">
         <v>245</v>
       </c>
@@ -5023,7 +5097,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:3">
       <c r="B169" s="14" t="s">
         <v>253</v>
       </c>
@@ -5031,7 +5105,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:3">
       <c r="B170" s="14" t="s">
         <v>248</v>
       </c>
@@ -5039,7 +5113,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:3">
       <c r="B171" s="14" t="s">
         <v>229</v>
       </c>
@@ -5047,7 +5121,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:3">
       <c r="B172" s="14" t="s">
         <v>230</v>
       </c>
@@ -5055,7 +5129,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:3">
       <c r="B173" s="14" t="s">
         <v>259</v>
       </c>
@@ -5063,7 +5137,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:3">
       <c r="B174" s="14" t="s">
         <v>227</v>
       </c>
@@ -5071,7 +5145,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:3">
       <c r="B175" s="14" t="s">
         <v>226</v>
       </c>
@@ -5079,7 +5153,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:3">
       <c r="B176" s="14" t="s">
         <v>240</v>
       </c>
@@ -5087,7 +5161,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:3">
       <c r="B177" s="14" t="s">
         <v>270</v>
       </c>
@@ -5095,7 +5169,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:3">
       <c r="B178" s="14" t="s">
         <v>275</v>
       </c>
@@ -5103,7 +5177,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:3">
       <c r="B179" s="14" t="s">
         <v>268</v>
       </c>
@@ -5111,7 +5185,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:3">
       <c r="B180" s="14" t="s">
         <v>267</v>
       </c>
@@ -5119,7 +5193,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:3">
       <c r="B181" s="14" t="s">
         <v>271</v>
       </c>
@@ -5127,7 +5201,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:3">
       <c r="B182" s="14" t="s">
         <v>272</v>
       </c>
@@ -5135,7 +5209,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:3">
       <c r="B183" s="14" t="s">
         <v>277</v>
       </c>
@@ -5143,7 +5217,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:3">
       <c r="B184" s="14" t="s">
         <v>284</v>
       </c>
@@ -5151,7 +5225,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:3">
       <c r="B185" s="14" t="s">
         <v>285</v>
       </c>
@@ -5159,592 +5233,592 @@
         <v>621</v>
       </c>
     </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:3">
       <c r="B186" s="14" t="s">
         <v>273</v>
       </c>
       <c r="C186"/>
     </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="187" spans="2:3">
       <c r="B187" s="14" t="s">
         <v>278</v>
       </c>
       <c r="C187"/>
     </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="188" spans="2:3">
       <c r="B188" s="14" t="s">
         <v>280</v>
       </c>
       <c r="C188"/>
     </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="189" spans="2:3">
       <c r="B189" s="14" t="s">
         <v>283</v>
       </c>
       <c r="C189"/>
     </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="190" spans="2:3">
       <c r="B190" s="14" t="s">
         <v>274</v>
       </c>
       <c r="C190"/>
     </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="191" spans="2:3">
       <c r="B191" s="14" t="s">
         <v>266</v>
       </c>
       <c r="C191"/>
     </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="192" spans="2:3">
       <c r="B192" s="14" t="s">
         <v>287</v>
       </c>
       <c r="C192"/>
     </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="193" spans="2:3">
       <c r="B193" s="14" t="s">
         <v>286</v>
       </c>
       <c r="C193"/>
     </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="194" spans="2:3">
       <c r="B194" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C194"/>
     </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="195" spans="2:3">
       <c r="B195" s="14" t="s">
         <v>289</v>
       </c>
       <c r="C195"/>
     </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="196" spans="2:3">
       <c r="B196" s="14" t="s">
         <v>288</v>
       </c>
       <c r="C196"/>
     </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="197" spans="2:3">
       <c r="B197" s="14" t="s">
         <v>302</v>
       </c>
       <c r="C197"/>
     </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="198" spans="2:3">
       <c r="B198" s="14" t="s">
         <v>291</v>
       </c>
       <c r="C198"/>
     </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="199" spans="2:3">
       <c r="B199" s="14" t="s">
         <v>296</v>
       </c>
       <c r="C199"/>
     </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="200" spans="2:3">
       <c r="B200" s="14" t="s">
         <v>305</v>
       </c>
       <c r="C200"/>
     </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="201" spans="2:3">
       <c r="B201" s="14" t="s">
         <v>293</v>
       </c>
       <c r="C201"/>
     </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="202" spans="2:3">
       <c r="B202" s="14" t="s">
         <v>298</v>
       </c>
       <c r="C202"/>
     </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="203" spans="2:3">
       <c r="B203" s="14" t="s">
         <v>290</v>
       </c>
       <c r="C203"/>
     </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="204" spans="2:3">
       <c r="B204" s="14" t="s">
         <v>299</v>
       </c>
       <c r="C204"/>
     </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="205" spans="2:3">
       <c r="B205" s="14" t="s">
         <v>300</v>
       </c>
       <c r="C205"/>
     </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="206" spans="2:3">
       <c r="B206" s="14" t="s">
         <v>292</v>
       </c>
       <c r="C206"/>
     </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="207" spans="2:3">
       <c r="B207" s="14" t="s">
         <v>308</v>
       </c>
       <c r="C207"/>
     </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="208" spans="2:3">
       <c r="B208" s="14" t="s">
         <v>309</v>
       </c>
       <c r="C208"/>
     </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="209" spans="2:3">
       <c r="B209" s="14" t="s">
         <v>311</v>
       </c>
       <c r="C209"/>
     </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="210" spans="2:3">
       <c r="B210" s="14" t="s">
         <v>307</v>
       </c>
       <c r="C210"/>
     </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="211" spans="2:3">
       <c r="B211" s="14" t="s">
         <v>294</v>
       </c>
       <c r="C211"/>
     </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="212" spans="2:3">
       <c r="B212" s="14" t="s">
         <v>304</v>
       </c>
       <c r="C212"/>
     </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="213" spans="2:3">
       <c r="B213" s="14" t="s">
         <v>313</v>
       </c>
       <c r="C213"/>
     </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="214" spans="2:3">
       <c r="B214" s="14" t="s">
         <v>312</v>
       </c>
       <c r="C214"/>
     </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="215" spans="2:3">
       <c r="B215" s="14" t="s">
         <v>315</v>
       </c>
       <c r="C215"/>
     </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="216" spans="2:3">
       <c r="B216" s="14" t="s">
         <v>316</v>
       </c>
       <c r="C216"/>
     </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="217" spans="2:3">
       <c r="B217" s="14" t="s">
         <v>314</v>
       </c>
       <c r="C217"/>
     </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="218" spans="2:3">
       <c r="B218" s="14" t="s">
         <v>317</v>
       </c>
       <c r="C218"/>
     </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="219" spans="2:3">
       <c r="B219" s="14" t="s">
         <v>318</v>
       </c>
       <c r="C219"/>
     </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="220" spans="2:3">
       <c r="B220" s="14" t="s">
         <v>319</v>
       </c>
       <c r="C220"/>
     </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="221" spans="2:3">
       <c r="B221" s="14" t="s">
         <v>320</v>
       </c>
       <c r="C221"/>
     </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="222" spans="2:3">
       <c r="B222" s="14" t="s">
         <v>323</v>
       </c>
       <c r="C222"/>
     </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="223" spans="2:3">
       <c r="B223" s="14" t="s">
         <v>322</v>
       </c>
       <c r="C223"/>
     </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="224" spans="2:3">
       <c r="B224" s="14" t="s">
         <v>331</v>
       </c>
       <c r="C224"/>
     </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="225" spans="2:3">
       <c r="B225" s="14" t="s">
         <v>329</v>
       </c>
       <c r="C225"/>
     </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="226" spans="2:3">
       <c r="B226" s="14" t="s">
         <v>328</v>
       </c>
       <c r="C226"/>
     </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="227" spans="2:3">
       <c r="B227" s="14" t="s">
         <v>326</v>
       </c>
       <c r="C227"/>
     </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="228" spans="2:3">
       <c r="B228" s="14" t="s">
         <v>324</v>
       </c>
       <c r="C228"/>
     </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="229" spans="2:3">
       <c r="B229" s="14" t="s">
         <v>325</v>
       </c>
       <c r="C229"/>
     </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="230" spans="2:3">
       <c r="B230" s="14" t="s">
         <v>327</v>
       </c>
       <c r="C230"/>
     </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="231" spans="2:3">
       <c r="B231" s="14" t="s">
         <v>330</v>
       </c>
       <c r="C231"/>
     </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="232" spans="2:3">
       <c r="B232" s="14" t="s">
         <v>332</v>
       </c>
       <c r="C232"/>
     </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="233" spans="2:3">
       <c r="B233" s="14" t="s">
         <v>333</v>
       </c>
       <c r="C233"/>
     </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="234" spans="2:3">
       <c r="C234"/>
     </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="235" spans="2:3">
       <c r="C235"/>
     </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="236" spans="2:3">
       <c r="C236"/>
     </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:3">
       <c r="C237"/>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:3">
       <c r="C238"/>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:3">
       <c r="C239"/>
     </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:3">
       <c r="C240"/>
     </row>
-    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3">
       <c r="C241"/>
     </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3">
       <c r="C242"/>
     </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3">
       <c r="C243"/>
     </row>
-    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:3">
       <c r="C244"/>
     </row>
-    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:3">
       <c r="C245"/>
     </row>
-    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:3">
       <c r="C246"/>
     </row>
-    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:3">
       <c r="C247"/>
     </row>
-    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:3">
       <c r="C248"/>
     </row>
-    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:3">
       <c r="C249"/>
     </row>
-    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:3">
       <c r="C250"/>
     </row>
-    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:3">
       <c r="C251"/>
     </row>
-    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:3">
       <c r="C252"/>
     </row>
-    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:3">
       <c r="C253"/>
     </row>
-    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:3">
       <c r="C254"/>
     </row>
-    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:3">
       <c r="C255"/>
     </row>
-    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:3">
       <c r="C256"/>
     </row>
-    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:3">
       <c r="C257"/>
     </row>
-    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:3">
       <c r="C258"/>
     </row>
-    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:3">
       <c r="C259"/>
     </row>
-    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:3">
       <c r="C260"/>
     </row>
-    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:3">
       <c r="C261"/>
     </row>
-    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:3">
       <c r="C262"/>
     </row>
-    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:3">
       <c r="C263"/>
     </row>
-    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:3">
       <c r="C264"/>
     </row>
-    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:3">
       <c r="C265"/>
     </row>
-    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:3">
       <c r="C266"/>
     </row>
-    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:3">
       <c r="C267"/>
     </row>
-    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:3">
       <c r="C268"/>
     </row>
-    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:3">
       <c r="C269"/>
     </row>
-    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:3">
       <c r="C270"/>
     </row>
-    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:3">
       <c r="C271"/>
     </row>
-    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:3">
       <c r="C272"/>
     </row>
-    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:3">
       <c r="C273"/>
     </row>
-    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:3">
       <c r="C274"/>
     </row>
-    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:3">
       <c r="C275"/>
     </row>
-    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:3">
       <c r="C276"/>
     </row>
-    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:3">
       <c r="C277"/>
     </row>
-    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:3">
       <c r="C278"/>
     </row>
-    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:3">
       <c r="C279"/>
     </row>
-    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:3">
       <c r="C280"/>
     </row>
-    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:3">
       <c r="C281"/>
     </row>
-    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:3">
       <c r="C282"/>
     </row>
-    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:3">
       <c r="C283"/>
     </row>
-    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:3">
       <c r="C284"/>
     </row>
-    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:3">
       <c r="C285"/>
     </row>
-    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:3">
       <c r="C286"/>
     </row>
-    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:3">
       <c r="C287"/>
     </row>
-    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:3">
       <c r="C288"/>
     </row>
-    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:3">
       <c r="C289"/>
     </row>
-    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:3">
       <c r="C290"/>
     </row>
-    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:3">
       <c r="C291"/>
     </row>
-    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:3">
       <c r="C292"/>
     </row>
-    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:3">
       <c r="C293"/>
     </row>
-    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:3">
       <c r="C294"/>
     </row>
-    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:3">
       <c r="C295"/>
     </row>
-    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:3">
       <c r="C296"/>
     </row>
-    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:3">
       <c r="C297"/>
     </row>
-    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:3">
       <c r="C298"/>
     </row>
-    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:3">
       <c r="C299"/>
     </row>
-    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:3">
       <c r="C300"/>
     </row>
-    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:3">
       <c r="C301"/>
     </row>
-    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:3">
       <c r="C302"/>
     </row>
-    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:3">
       <c r="C303"/>
     </row>
-    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:3">
       <c r="C304"/>
     </row>
-    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:3">
       <c r="C305"/>
     </row>
-    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:3">
       <c r="C306"/>
     </row>
-    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:3">
       <c r="C307"/>
     </row>
-    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:3">
       <c r="C308"/>
     </row>
-    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:3">
       <c r="C309"/>
     </row>
-    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:3">
       <c r="C310"/>
     </row>
-    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:3">
       <c r="C311"/>
     </row>
-    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:3">
       <c r="C312"/>
     </row>
-    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:3">
       <c r="C313"/>
     </row>
-    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:3">
       <c r="C314"/>
     </row>
-    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:3">
       <c r="C315"/>
     </row>
-    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:3">
       <c r="C316"/>
     </row>
-    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:3">
       <c r="C317"/>
     </row>
-    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:3">
       <c r="C318"/>
     </row>
-    <row r="319" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:3">
       <c r="C319"/>
     </row>
-    <row r="320" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:3">
       <c r="C320"/>
     </row>
-    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:3">
       <c r="C321"/>
     </row>
-    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:3">
       <c r="C322"/>
     </row>
-    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:3">
       <c r="C323"/>
     </row>
-    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:3">
       <c r="C324"/>
     </row>
-    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:3">
       <c r="C325"/>
     </row>
-    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:3">
       <c r="C326"/>
     </row>
-    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:3">
       <c r="C327"/>
     </row>
-    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:3">
       <c r="C328"/>
     </row>
-    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:3">
       <c r="C329"/>
     </row>
-    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:3">
       <c r="C330"/>
     </row>
-    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:3">
       <c r="C331"/>
     </row>
-    <row r="332" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:3">
       <c r="C332"/>
     </row>
-    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:3">
       <c r="C333"/>
     </row>
   </sheetData>
@@ -5752,7 +5826,12 @@
     <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5760,22 +5839,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="24" style="7" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
+    <col min="3" max="3" width="30.83203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="15.1640625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="38.5" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" s="4" t="s">
         <v>486</v>
       </c>
@@ -5791,8 +5871,11 @@
       <c r="E1" s="6" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="14" t="s">
+        <v>633</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6">
       <c r="A2" s="7" t="s">
         <v>485</v>
       </c>
@@ -5808,8 +5891,11 @@
       <c r="E2" s="7" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="11" t="s">
+        <v>634</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="7" t="s">
         <v>526</v>
       </c>
@@ -5825,8 +5911,11 @@
       <c r="E3" s="7" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="11" t="s">
+        <v>635</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4" s="2" t="s">
         <v>527</v>
       </c>
@@ -5842,8 +5931,11 @@
       <c r="E4" s="7" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="11" t="s">
+        <v>636</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="B5" s="8" t="s">
         <v>367</v>
       </c>
@@ -5856,8 +5948,11 @@
       <c r="E5" s="7" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="12" t="s">
+        <v>637</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="B6" s="8" t="s">
         <v>370</v>
       </c>
@@ -5867,8 +5962,11 @@
       <c r="D6" s="7" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="18" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="B7" s="8" t="s">
         <v>373</v>
       </c>
@@ -5878,8 +5976,11 @@
       <c r="D7" s="7" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7" s="21" t="s">
+        <v>639</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="B8" s="8" t="s">
         <v>375</v>
       </c>
@@ -5889,8 +5990,11 @@
       <c r="D8" s="7" t="s">
         <v>374</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8" s="11" t="s">
+        <v>640</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="B9" s="8" t="s">
         <v>378</v>
       </c>
@@ -5900,8 +6004,11 @@
       <c r="D9" s="7" t="s">
         <v>377</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9" s="12" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="B10" s="8" t="s">
         <v>381</v>
       </c>
@@ -5911,8 +6018,11 @@
       <c r="D10" s="7" t="s">
         <v>380</v>
       </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F10" s="12" t="s">
+        <v>642</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="B11" s="8" t="s">
         <v>384</v>
       </c>
@@ -5922,8 +6032,11 @@
       <c r="D11" s="7" t="s">
         <v>383</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11" s="21" t="s">
+        <v>643</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="B12" s="8" t="s">
         <v>387</v>
       </c>
@@ -5933,8 +6046,11 @@
       <c r="D12" s="7" t="s">
         <v>386</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12" s="11" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
       <c r="B13" s="8" t="s">
         <v>390</v>
       </c>
@@ -5944,8 +6060,11 @@
       <c r="D13" s="7" t="s">
         <v>389</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13" s="12" t="s">
+        <v>645</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6">
       <c r="B14" s="8" t="s">
         <v>392</v>
       </c>
@@ -5955,8 +6074,11 @@
       <c r="D14" s="7" t="s">
         <v>391</v>
       </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F14" s="12" t="s">
+        <v>646</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="B15" s="8" t="s">
         <v>393</v>
       </c>
@@ -5966,24 +6088,33 @@
       <c r="D15" s="7" t="s">
         <v>358</v>
       </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F15" s="21" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
       <c r="B16" s="8" t="s">
         <v>395</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>394</v>
       </c>
-    </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F16" s="11" t="s">
+        <v>648</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6">
       <c r="B17" s="8" t="s">
         <v>397</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="F17" s="12" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6">
       <c r="B18" s="8" t="s">
         <v>399</v>
       </c>
@@ -5991,7 +6122,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:6">
       <c r="B19" s="8" t="s">
         <v>401</v>
       </c>
@@ -5999,7 +6130,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:6">
       <c r="B20" s="8" t="s">
         <v>403</v>
       </c>
@@ -6007,7 +6138,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:6">
       <c r="B21" s="8" t="s">
         <v>405</v>
       </c>
@@ -6015,211 +6146,216 @@
         <v>404</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:6">
       <c r="D22" s="7" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:6">
       <c r="D23" s="7" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:6">
       <c r="D24" s="7" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:6">
       <c r="D25" s="7" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:6">
       <c r="D26" s="7" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:6">
       <c r="D27" s="7" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:6">
       <c r="D28" s="7" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:6">
       <c r="D29" s="7" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:6">
       <c r="D30" s="7" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:6">
       <c r="D31" s="7" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:6">
       <c r="D32" s="7" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="7" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="7" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="7" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="7" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="7" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="7" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="7" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="7" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="7" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="7" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="7" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="7" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="7" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="7" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="7" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="7" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="7" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4">
       <c r="D50" s="7" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4">
       <c r="D51" s="7" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4">
       <c r="D52" s="7" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4">
       <c r="D53" s="7" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4">
       <c r="D54" s="7" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4">
       <c r="D55" s="7" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4">
       <c r="D56" s="7" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4">
       <c r="D57" s="7" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4">
       <c r="D58" s="7" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4">
       <c r="D59" s="7" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4">
       <c r="D60" s="7" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4">
       <c r="D61" s="9"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4">
       <c r="D62" s="9"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4">
       <c r="D63" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Utilized values in --Select a Subject:[type]-- of the template for subject type validation. DM-136
</commit_message>
<xml_diff>
--- a/WebContent/files/xls_standard_input_template.xlsx
+++ b/WebContent/files/xls_standard_input_template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
-  <workbookPr autoCompressPictures="0"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MSD\DOMM\Excel standard input\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28780" windowHeight="16700" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
     <sheet name="Select-a-header values" sheetId="14" r:id="rId2"/>
     <sheet name="CV values" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="140001" concurrentCalc="0"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
-      <mx:ArchID Flags="2"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="152511" concurrentCalc="0"/>
 </workbook>
 </file>
 
@@ -26,7 +26,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0">
+    <comment ref="G1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0">
+    <comment ref="M1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0">
+    <comment ref="N1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0">
+    <comment ref="O1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0">
+    <comment ref="P1" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="664" uniqueCount="650">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="633">
   <si>
     <t>text</t>
   </si>
@@ -2060,64 +2060,13 @@
   </si>
   <si>
     <t>Note:related publications</t>
-  </si>
-  <si>
-    <t>subject type</t>
-  </si>
-  <si>
-    <t>anatomy</t>
-  </si>
-  <si>
-    <t>common name</t>
-  </si>
-  <si>
-    <t>conference name</t>
-  </si>
-  <si>
-    <t>corporate name</t>
-  </si>
-  <si>
-    <t>cruise</t>
-  </si>
-  <si>
-    <t>culturalContext</t>
-  </si>
-  <si>
-    <t>family name</t>
-  </si>
-  <si>
-    <t>genre</t>
-  </si>
-  <si>
-    <t>geographic</t>
-  </si>
-  <si>
-    <t>lithology</t>
-  </si>
-  <si>
-    <t>occupation</t>
-  </si>
-  <si>
-    <t>personal name</t>
-  </si>
-  <si>
-    <t>scientific name</t>
-  </si>
-  <si>
-    <t>series</t>
-  </si>
-  <si>
-    <t>temporal</t>
-  </si>
-  <si>
-    <t>topic</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="35" x14ac:knownFonts="1">
+  <fonts count="33" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2343,22 +2292,6 @@
     <font>
       <sz val="11"/>
       <color theme="5" tint="-0.249977111117893"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -2705,7 +2638,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="53">
+  <cellStyleXfs count="51">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
@@ -2757,8 +2690,6 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="34" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -2806,7 +2737,7 @@
     <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="53">
+  <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
     <cellStyle name="20% - Accent2" xfId="23" builtinId="34" customBuiltin="1"/>
     <cellStyle name="20% - Accent3" xfId="27" builtinId="38" customBuiltin="1"/>
@@ -2835,13 +2766,11 @@
     <cellStyle name="Calculation" xfId="11" builtinId="22" customBuiltin="1"/>
     <cellStyle name="Check Cell" xfId="13" builtinId="23" customBuiltin="1"/>
     <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
-    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Good" xfId="6" builtinId="26" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
     <cellStyle name="Heading 2" xfId="3" builtinId="17" customBuiltin="1"/>
     <cellStyle name="Heading 3" xfId="4" builtinId="18" customBuiltin="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" customBuiltin="1"/>
-    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink 2" xfId="48"/>
     <cellStyle name="Input" xfId="9" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Linked Cell" xfId="12" builtinId="24" customBuiltin="1"/>
@@ -2963,7 +2892,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -2998,7 +2927,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3213,30 +3142,30 @@
       <selection activeCell="G25" sqref="G25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="21" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.5" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.5" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.6640625" style="3" customWidth="1"/>
-    <col min="5" max="5" width="45.33203125" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.6640625" style="3" customWidth="1"/>
-    <col min="7" max="7" width="23.83203125" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5703125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.5703125" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.7109375" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.28515625" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.7109375" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.85546875" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" style="3" customWidth="1"/>
-    <col min="10" max="10" width="51.5" style="3" customWidth="1"/>
-    <col min="11" max="12" width="45.1640625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="45.5" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.83203125" style="3" customWidth="1"/>
-    <col min="15" max="15" width="15.1640625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="19.83203125" style="3" customWidth="1"/>
-    <col min="17" max="18" width="39.1640625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="42.83203125" style="3" customWidth="1"/>
-    <col min="20" max="20" width="44.5" style="3" customWidth="1"/>
-    <col min="21" max="21" width="84.33203125" style="3" customWidth="1"/>
+    <col min="10" max="10" width="51.5703125" style="3" customWidth="1"/>
+    <col min="11" max="12" width="45.140625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="45.5703125" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14.85546875" style="3" customWidth="1"/>
+    <col min="15" max="15" width="15.140625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="19.85546875" style="3" customWidth="1"/>
+    <col min="17" max="18" width="39.140625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="42.85546875" style="3" customWidth="1"/>
+    <col min="20" max="20" width="44.5703125" style="3" customWidth="1"/>
+    <col min="21" max="21" width="84.28515625" style="3" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="22.5" customHeight="1">
+    <row r="1" spans="1:21" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3324,8 +3253,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="I1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait"/>
-  <legacyDrawing r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
@@ -3409,9 +3338,6 @@
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
   </extLst>
 </worksheet>
 </file>
@@ -3420,21 +3346,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R333"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="G1" sqref="G1:G1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="38.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultColWidth="38.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21.1640625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="41.33203125" style="14" customWidth="1"/>
-    <col min="4" max="4" width="26.33203125" style="14" customWidth="1"/>
-    <col min="5" max="5" width="43.6640625" style="14" customWidth="1"/>
-    <col min="6" max="18" width="38.5" style="14"/>
-    <col min="19" max="16384" width="38.5" style="11"/>
+    <col min="1" max="1" width="21.140625" style="14" customWidth="1"/>
+    <col min="2" max="3" width="41.28515625" style="14" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="14" customWidth="1"/>
+    <col min="5" max="5" width="43.7109375" style="14" customWidth="1"/>
+    <col min="6" max="18" width="38.5703125" style="14"/>
+    <col min="19" max="16384" width="38.5703125" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>517</v>
       </c>
@@ -3463,7 +3389,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -3492,7 +3418,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="14" t="s">
         <v>445</v>
       </c>
@@ -3521,7 +3447,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>447</v>
       </c>
@@ -3550,7 +3476,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="5" spans="1:9">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>449</v>
       </c>
@@ -3579,7 +3505,7 @@
         <v>478</v>
       </c>
     </row>
-    <row r="6" spans="1:9" ht="15">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>453</v>
       </c>
@@ -3608,7 +3534,7 @@
         <v>479</v>
       </c>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="14" t="s">
         <v>457</v>
       </c>
@@ -3634,7 +3560,7 @@
         <v>514</v>
       </c>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B8" s="14" t="s">
         <v>27</v>
       </c>
@@ -3655,7 +3581,7 @@
         <v>480</v>
       </c>
     </row>
-    <row r="9" spans="1:9">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B9" s="14" t="s">
         <v>30</v>
       </c>
@@ -3676,7 +3602,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="10" spans="1:9">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B10" s="14" t="s">
         <v>32</v>
       </c>
@@ -3697,7 +3623,7 @@
         <v>482</v>
       </c>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B11" s="14" t="s">
         <v>34</v>
       </c>
@@ -3718,7 +3644,7 @@
         <v>483</v>
       </c>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B12" s="14" t="s">
         <v>20</v>
       </c>
@@ -3739,7 +3665,7 @@
         <v>515</v>
       </c>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B13" s="14" t="s">
         <v>22</v>
       </c>
@@ -3758,7 +3684,7 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B14" s="14" t="s">
         <v>35</v>
       </c>
@@ -3775,7 +3701,7 @@
         <v>512</v>
       </c>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B15" s="14" t="s">
         <v>33</v>
       </c>
@@ -3792,7 +3718,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B16" s="14" t="s">
         <v>36</v>
       </c>
@@ -3809,7 +3735,7 @@
         <v>334</v>
       </c>
     </row>
-    <row r="17" spans="2:7">
+    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B17" s="14" t="s">
         <v>37</v>
       </c>
@@ -3826,7 +3752,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="18" spans="2:7">
+    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
         <v>40</v>
       </c>
@@ -3840,7 +3766,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="19" spans="2:7">
+    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>41</v>
       </c>
@@ -3854,7 +3780,7 @@
         <v>504</v>
       </c>
     </row>
-    <row r="20" spans="2:7">
+    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>45</v>
       </c>
@@ -3868,7 +3794,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="21" spans="2:7">
+    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
         <v>31</v>
       </c>
@@ -3879,7 +3805,7 @@
         <v>484</v>
       </c>
     </row>
-    <row r="22" spans="2:7">
+    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
         <v>24</v>
       </c>
@@ -3890,7 +3816,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="23" spans="2:7">
+    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
         <v>42</v>
       </c>
@@ -3901,7 +3827,7 @@
         <v>342</v>
       </c>
     </row>
-    <row r="24" spans="2:7">
+    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
         <v>43</v>
       </c>
@@ -3912,7 +3838,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="2:7">
+    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
         <v>39</v>
       </c>
@@ -3923,7 +3849,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="2:7">
+    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
         <v>28</v>
       </c>
@@ -3934,7 +3860,7 @@
         <v>632</v>
       </c>
     </row>
-    <row r="27" spans="2:7">
+    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
         <v>55</v>
       </c>
@@ -3945,7 +3871,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="28" spans="2:7">
+    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
         <v>46</v>
       </c>
@@ -3956,7 +3882,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="29" spans="2:7">
+    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
         <v>54</v>
       </c>
@@ -3967,7 +3893,7 @@
         <v>629</v>
       </c>
     </row>
-    <row r="30" spans="2:7">
+    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
         <v>50</v>
       </c>
@@ -3978,7 +3904,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="31" spans="2:7">
+    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
         <v>52</v>
       </c>
@@ -3989,7 +3915,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="32" spans="2:7">
+    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
         <v>48</v>
       </c>
@@ -4000,7 +3926,7 @@
         <v>509</v>
       </c>
     </row>
-    <row r="33" spans="2:5">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
         <v>57</v>
       </c>
@@ -4011,7 +3937,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="34" spans="2:5">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
         <v>61</v>
       </c>
@@ -4022,7 +3948,7 @@
         <v>466</v>
       </c>
     </row>
-    <row r="35" spans="2:5">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
         <v>60</v>
       </c>
@@ -4030,7 +3956,7 @@
         <v>547</v>
       </c>
     </row>
-    <row r="36" spans="2:5">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
         <v>68</v>
       </c>
@@ -4039,7 +3965,7 @@
       </c>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="2:5">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
         <v>106</v>
       </c>
@@ -4048,7 +3974,7 @@
       </c>
       <c r="E37" s="18"/>
     </row>
-    <row r="38" spans="2:5">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
         <v>63</v>
       </c>
@@ -4057,7 +3983,7 @@
       </c>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="2:5">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
         <v>76</v>
       </c>
@@ -4065,7 +3991,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="2:5">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
         <v>65</v>
       </c>
@@ -4073,7 +3999,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:5">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
         <v>75</v>
       </c>
@@ -4081,7 +4007,7 @@
         <v>550</v>
       </c>
     </row>
-    <row r="42" spans="2:5">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
         <v>66</v>
       </c>
@@ -4089,7 +4015,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="43" spans="2:5">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
         <v>83</v>
       </c>
@@ -4097,7 +4023,7 @@
         <v>552</v>
       </c>
     </row>
-    <row r="44" spans="2:5">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B44" s="14" t="s">
         <v>79</v>
       </c>
@@ -4105,7 +4031,7 @@
         <v>553</v>
       </c>
     </row>
-    <row r="45" spans="2:5">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
         <v>70</v>
       </c>
@@ -4113,7 +4039,7 @@
         <v>554</v>
       </c>
     </row>
-    <row r="46" spans="2:5">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
         <v>69</v>
       </c>
@@ -4121,7 +4047,7 @@
         <v>555</v>
       </c>
     </row>
-    <row r="47" spans="2:5">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
         <v>71</v>
       </c>
@@ -4129,7 +4055,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="2:5">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
         <v>110</v>
       </c>
@@ -4137,7 +4063,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="2:3">
+    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
         <v>81</v>
       </c>
@@ -4145,7 +4071,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="2:3">
+    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="14" t="s">
         <v>72</v>
       </c>
@@ -4153,7 +4079,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="2:3">
+    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
         <v>73</v>
       </c>
@@ -4161,7 +4087,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="2:3">
+    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="14" t="s">
         <v>64</v>
       </c>
@@ -4169,7 +4095,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:3">
+    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
         <v>74</v>
       </c>
@@ -4177,7 +4103,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="2:3">
+    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="14" t="s">
         <v>82</v>
       </c>
@@ -4185,7 +4111,7 @@
         <v>556</v>
       </c>
     </row>
-    <row r="55" spans="2:3">
+    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
         <v>101</v>
       </c>
@@ -4193,7 +4119,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="2:3">
+    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="14" t="s">
         <v>102</v>
       </c>
@@ -4201,7 +4127,7 @@
         <v>557</v>
       </c>
     </row>
-    <row r="57" spans="2:3">
+    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
         <v>107</v>
       </c>
@@ -4209,7 +4135,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="2:3">
+    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="14" t="s">
         <v>104</v>
       </c>
@@ -4217,7 +4143,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="59" spans="2:3">
+    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
         <v>467</v>
       </c>
@@ -4225,7 +4151,7 @@
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="2:3">
+    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
         <v>90</v>
       </c>
@@ -4233,7 +4159,7 @@
         <v>558</v>
       </c>
     </row>
-    <row r="61" spans="2:3">
+    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
         <v>92</v>
       </c>
@@ -4241,7 +4167,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="2:3">
+    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
         <v>99</v>
       </c>
@@ -4249,7 +4175,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="2:3">
+    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="14" t="s">
         <v>98</v>
       </c>
@@ -4257,7 +4183,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="2:3">
+    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="14" t="s">
         <v>103</v>
       </c>
@@ -4265,7 +4191,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="2:3">
+    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
         <v>87</v>
       </c>
@@ -4273,7 +4199,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="2:3">
+    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="14" t="s">
         <v>100</v>
       </c>
@@ -4281,7 +4207,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="2:3">
+    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="14" t="s">
         <v>89</v>
       </c>
@@ -4289,7 +4215,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="68" spans="2:3">
+    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="14" t="s">
         <v>96</v>
       </c>
@@ -4297,7 +4223,7 @@
         <v>560</v>
       </c>
     </row>
-    <row r="69" spans="2:3">
+    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="14" t="s">
         <v>109</v>
       </c>
@@ -4305,7 +4231,7 @@
         <v>561</v>
       </c>
     </row>
-    <row r="70" spans="2:3">
+    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="14" t="s">
         <v>117</v>
       </c>
@@ -4313,7 +4239,7 @@
         <v>562</v>
       </c>
     </row>
-    <row r="71" spans="2:3">
+    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="14" t="s">
         <v>129</v>
       </c>
@@ -4321,7 +4247,7 @@
         <v>563</v>
       </c>
     </row>
-    <row r="72" spans="2:3">
+    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="14" t="s">
         <v>132</v>
       </c>
@@ -4329,7 +4255,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="2:3">
+    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="14" t="s">
         <v>131</v>
       </c>
@@ -4337,7 +4263,7 @@
         <v>564</v>
       </c>
     </row>
-    <row r="74" spans="2:3">
+    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
         <v>133</v>
       </c>
@@ -4345,7 +4271,7 @@
         <v>565</v>
       </c>
     </row>
-    <row r="75" spans="2:3">
+    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="14" t="s">
         <v>114</v>
       </c>
@@ -4353,7 +4279,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="76" spans="2:3">
+    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="14" t="s">
         <v>116</v>
       </c>
@@ -4361,7 +4287,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="77" spans="2:3">
+    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="14" t="s">
         <v>120</v>
       </c>
@@ -4369,7 +4295,7 @@
         <v>567</v>
       </c>
     </row>
-    <row r="78" spans="2:3">
+    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="14" t="s">
         <v>121</v>
       </c>
@@ -4377,7 +4303,7 @@
         <v>568</v>
       </c>
     </row>
-    <row r="79" spans="2:3">
+    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="14" t="s">
         <v>125</v>
       </c>
@@ -4385,7 +4311,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="2:3">
+    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
         <v>124</v>
       </c>
@@ -4393,7 +4319,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="2:3">
+    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="14" t="s">
         <v>115</v>
       </c>
@@ -4401,7 +4327,7 @@
         <v>569</v>
       </c>
     </row>
-    <row r="82" spans="2:3">
+    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="14" t="s">
         <v>127</v>
       </c>
@@ -4409,7 +4335,7 @@
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="2:3">
+    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="14" t="s">
         <v>118</v>
       </c>
@@ -4417,7 +4343,7 @@
         <v>155</v>
       </c>
     </row>
-    <row r="84" spans="2:3">
+    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
         <v>123</v>
       </c>
@@ -4425,7 +4351,7 @@
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="2:3">
+    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
         <v>134</v>
       </c>
@@ -4433,7 +4359,7 @@
         <v>570</v>
       </c>
     </row>
-    <row r="86" spans="2:3">
+    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="14" t="s">
         <v>137</v>
       </c>
@@ -4441,7 +4367,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="2:3">
+    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="14" t="s">
         <v>135</v>
       </c>
@@ -4449,7 +4375,7 @@
         <v>164</v>
       </c>
     </row>
-    <row r="88" spans="2:3">
+    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="14" t="s">
         <v>136</v>
       </c>
@@ -4457,7 +4383,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="2:3">
+    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
         <v>139</v>
       </c>
@@ -4465,7 +4391,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="2:3">
+    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="14" t="s">
         <v>140</v>
       </c>
@@ -4473,7 +4399,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="2:3">
+    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="14" t="s">
         <v>142</v>
       </c>
@@ -4481,7 +4407,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="92" spans="2:3">
+    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="14" t="s">
         <v>141</v>
       </c>
@@ -4489,7 +4415,7 @@
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="2:3">
+    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
         <v>138</v>
       </c>
@@ -4497,7 +4423,7 @@
         <v>179</v>
       </c>
     </row>
-    <row r="94" spans="2:3">
+    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="14" t="s">
         <v>144</v>
       </c>
@@ -4505,7 +4431,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="95" spans="2:3">
+    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="14" t="s">
         <v>146</v>
       </c>
@@ -4513,7 +4439,7 @@
         <v>572</v>
       </c>
     </row>
-    <row r="96" spans="2:3">
+    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="14" t="s">
         <v>147</v>
       </c>
@@ -4521,7 +4447,7 @@
         <v>573</v>
       </c>
     </row>
-    <row r="97" spans="2:3">
+    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="14" t="s">
         <v>469</v>
       </c>
@@ -4529,7 +4455,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="2:3">
+    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="14" t="s">
         <v>150</v>
       </c>
@@ -4537,7 +4463,7 @@
         <v>574</v>
       </c>
     </row>
-    <row r="99" spans="2:3">
+    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="14" t="s">
         <v>152</v>
       </c>
@@ -4545,7 +4471,7 @@
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="2:3">
+    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="14" t="s">
         <v>148</v>
       </c>
@@ -4553,7 +4479,7 @@
         <v>192</v>
       </c>
     </row>
-    <row r="101" spans="2:3">
+    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="14" t="s">
         <v>151</v>
       </c>
@@ -4561,7 +4487,7 @@
         <v>575</v>
       </c>
     </row>
-    <row r="102" spans="2:3">
+    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="14" t="s">
         <v>156</v>
       </c>
@@ -4569,7 +4495,7 @@
         <v>576</v>
       </c>
     </row>
-    <row r="103" spans="2:3">
+    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="14" t="s">
         <v>153</v>
       </c>
@@ -4577,7 +4503,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="104" spans="2:3">
+    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="14" t="s">
         <v>160</v>
       </c>
@@ -4585,7 +4511,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="2:3">
+    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="14" t="s">
         <v>162</v>
       </c>
@@ -4593,7 +4519,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="2:3">
+    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="14" t="s">
         <v>154</v>
       </c>
@@ -4601,7 +4527,7 @@
         <v>578</v>
       </c>
     </row>
-    <row r="107" spans="2:3">
+    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="14" t="s">
         <v>158</v>
       </c>
@@ -4609,7 +4535,7 @@
         <v>199</v>
       </c>
     </row>
-    <row r="108" spans="2:3">
+    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="14" t="s">
         <v>163</v>
       </c>
@@ -4617,7 +4543,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="2:3">
+    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="14" t="s">
         <v>165</v>
       </c>
@@ -4625,7 +4551,7 @@
         <v>579</v>
       </c>
     </row>
-    <row r="110" spans="2:3">
+    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="14" t="s">
         <v>166</v>
       </c>
@@ -4633,7 +4559,7 @@
         <v>205</v>
       </c>
     </row>
-    <row r="111" spans="2:3">
+    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="14" t="s">
         <v>170</v>
       </c>
@@ -4641,7 +4567,7 @@
         <v>580</v>
       </c>
     </row>
-    <row r="112" spans="2:3">
+    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="14" t="s">
         <v>168</v>
       </c>
@@ -4649,7 +4575,7 @@
         <v>581</v>
       </c>
     </row>
-    <row r="113" spans="2:3">
+    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="14" t="s">
         <v>172</v>
       </c>
@@ -4657,7 +4583,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="114" spans="2:3">
+    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="14" t="s">
         <v>176</v>
       </c>
@@ -4665,7 +4591,7 @@
         <v>218</v>
       </c>
     </row>
-    <row r="115" spans="2:3">
+    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="14" t="s">
         <v>177</v>
       </c>
@@ -4673,7 +4599,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="116" spans="2:3">
+    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="14" t="s">
         <v>178</v>
       </c>
@@ -4681,7 +4607,7 @@
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="2:3">
+    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="14" t="s">
         <v>174</v>
       </c>
@@ -4689,7 +4615,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="2:3">
+    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="14" t="s">
         <v>180</v>
       </c>
@@ -4697,7 +4623,7 @@
         <v>582</v>
       </c>
     </row>
-    <row r="119" spans="2:3">
+    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="14" t="s">
         <v>470</v>
       </c>
@@ -4705,7 +4631,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="120" spans="2:3">
+    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="14" t="s">
         <v>183</v>
       </c>
@@ -4713,7 +4639,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="121" spans="2:3">
+    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="14" t="s">
         <v>188</v>
       </c>
@@ -4721,7 +4647,7 @@
         <v>583</v>
       </c>
     </row>
-    <row r="122" spans="2:3">
+    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="14" t="s">
         <v>184</v>
       </c>
@@ -4729,7 +4655,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="123" spans="2:3">
+    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="14" t="s">
         <v>185</v>
       </c>
@@ -4737,7 +4663,7 @@
         <v>234</v>
       </c>
     </row>
-    <row r="124" spans="2:3">
+    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="14" t="s">
         <v>182</v>
       </c>
@@ -4745,7 +4671,7 @@
         <v>585</v>
       </c>
     </row>
-    <row r="125" spans="2:3">
+    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="14" t="s">
         <v>189</v>
       </c>
@@ -4753,7 +4679,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="126" spans="2:3">
+    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="14" t="s">
         <v>191</v>
       </c>
@@ -4761,7 +4687,7 @@
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="2:3">
+    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="14" t="s">
         <v>187</v>
       </c>
@@ -4769,7 +4695,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="128" spans="2:3">
+    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="14" t="s">
         <v>193</v>
       </c>
@@ -4777,7 +4703,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="129" spans="2:3">
+    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="14" t="s">
         <v>194</v>
       </c>
@@ -4785,7 +4711,7 @@
         <v>250</v>
       </c>
     </row>
-    <row r="130" spans="2:3">
+    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="14" t="s">
         <v>201</v>
       </c>
@@ -4793,7 +4719,7 @@
         <v>244</v>
       </c>
     </row>
-    <row r="131" spans="2:3">
+    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="14" t="s">
         <v>206</v>
       </c>
@@ -4801,7 +4727,7 @@
         <v>586</v>
       </c>
     </row>
-    <row r="132" spans="2:3">
+    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="14" t="s">
         <v>207</v>
       </c>
@@ -4809,7 +4735,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="133" spans="2:3">
+    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="14" t="s">
         <v>198</v>
       </c>
@@ -4817,7 +4743,7 @@
         <v>256</v>
       </c>
     </row>
-    <row r="134" spans="2:3">
+    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="14" t="s">
         <v>196</v>
       </c>
@@ -4825,7 +4751,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="135" spans="2:3">
+    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="14" t="s">
         <v>209</v>
       </c>
@@ -4833,7 +4759,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="136" spans="2:3">
+    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="14" t="s">
         <v>210</v>
       </c>
@@ -4841,7 +4767,7 @@
         <v>587</v>
       </c>
     </row>
-    <row r="137" spans="2:3">
+    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="14" t="s">
         <v>203</v>
       </c>
@@ -4849,7 +4775,7 @@
         <v>588</v>
       </c>
     </row>
-    <row r="138" spans="2:3">
+    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="14" t="s">
         <v>204</v>
       </c>
@@ -4857,7 +4783,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="139" spans="2:3">
+    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="14" t="s">
         <v>195</v>
       </c>
@@ -4865,7 +4791,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="140" spans="2:3">
+    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="14" t="s">
         <v>208</v>
       </c>
@@ -4873,7 +4799,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="141" spans="2:3">
+    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="14" t="s">
         <v>211</v>
       </c>
@@ -4881,7 +4807,7 @@
         <v>589</v>
       </c>
     </row>
-    <row r="142" spans="2:3">
+    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" s="14" t="s">
         <v>212</v>
       </c>
@@ -4889,7 +4815,7 @@
         <v>590</v>
       </c>
     </row>
-    <row r="143" spans="2:3">
+    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="14" t="s">
         <v>219</v>
       </c>
@@ -4897,7 +4823,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="144" spans="2:3">
+    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="14" t="s">
         <v>213</v>
       </c>
@@ -4905,7 +4831,7 @@
         <v>592</v>
       </c>
     </row>
-    <row r="145" spans="2:3">
+    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="14" t="s">
         <v>217</v>
       </c>
@@ -4913,7 +4839,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="2:3">
+    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="14" t="s">
         <v>215</v>
       </c>
@@ -4921,7 +4847,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="147" spans="2:3">
+    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" s="14" t="s">
         <v>220</v>
       </c>
@@ -4929,7 +4855,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="148" spans="2:3">
+    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" s="14" t="s">
         <v>222</v>
       </c>
@@ -4937,7 +4863,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="149" spans="2:3">
+    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="14" t="s">
         <v>622</v>
       </c>
@@ -4945,7 +4871,7 @@
         <v>593</v>
       </c>
     </row>
-    <row r="150" spans="2:3">
+    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" s="14" t="s">
         <v>224</v>
       </c>
@@ -4953,7 +4879,7 @@
         <v>594</v>
       </c>
     </row>
-    <row r="151" spans="2:3">
+    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" s="14" t="s">
         <v>239</v>
       </c>
@@ -4961,7 +4887,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="152" spans="2:3">
+    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="14" t="s">
         <v>261</v>
       </c>
@@ -4969,7 +4895,7 @@
         <v>596</v>
       </c>
     </row>
-    <row r="153" spans="2:3">
+    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" s="14" t="s">
         <v>263</v>
       </c>
@@ -4977,7 +4903,7 @@
         <v>597</v>
       </c>
     </row>
-    <row r="154" spans="2:3">
+    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" s="14" t="s">
         <v>225</v>
       </c>
@@ -4985,7 +4911,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="155" spans="2:3">
+    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" s="14" t="s">
         <v>247</v>
       </c>
@@ -4993,7 +4919,7 @@
         <v>303</v>
       </c>
     </row>
-    <row r="156" spans="2:3">
+    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="14" t="s">
         <v>231</v>
       </c>
@@ -5001,7 +4927,7 @@
         <v>297</v>
       </c>
     </row>
-    <row r="157" spans="2:3">
+    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" s="14" t="s">
         <v>232</v>
       </c>
@@ -5009,7 +4935,7 @@
         <v>599</v>
       </c>
     </row>
-    <row r="158" spans="2:3">
+    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" s="14" t="s">
         <v>241</v>
       </c>
@@ -5017,7 +4943,7 @@
         <v>306</v>
       </c>
     </row>
-    <row r="159" spans="2:3">
+    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" s="14" t="s">
         <v>246</v>
       </c>
@@ -5025,7 +4951,7 @@
         <v>600</v>
       </c>
     </row>
-    <row r="160" spans="2:3">
+    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" s="14" t="s">
         <v>471</v>
       </c>
@@ -5033,7 +4959,7 @@
         <v>601</v>
       </c>
     </row>
-    <row r="161" spans="2:3">
+    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" s="14" t="s">
         <v>257</v>
       </c>
@@ -5041,7 +4967,7 @@
         <v>602</v>
       </c>
     </row>
-    <row r="162" spans="2:3">
+    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" s="14" t="s">
         <v>237</v>
       </c>
@@ -5049,7 +4975,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="163" spans="2:3">
+    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" s="14" t="s">
         <v>249</v>
       </c>
@@ -5057,7 +4983,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="164" spans="2:3">
+    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" s="14" t="s">
         <v>243</v>
       </c>
@@ -5065,7 +4991,7 @@
         <v>603</v>
       </c>
     </row>
-    <row r="165" spans="2:3">
+    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" s="14" t="s">
         <v>252</v>
       </c>
@@ -5073,7 +4999,7 @@
         <v>295</v>
       </c>
     </row>
-    <row r="166" spans="2:3">
+    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" s="14" t="s">
         <v>255</v>
       </c>
@@ -5081,7 +5007,7 @@
         <v>604</v>
       </c>
     </row>
-    <row r="167" spans="2:3">
+    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" s="14" t="s">
         <v>235</v>
       </c>
@@ -5089,7 +5015,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="168" spans="2:3">
+    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" s="14" t="s">
         <v>245</v>
       </c>
@@ -5097,7 +5023,7 @@
         <v>606</v>
       </c>
     </row>
-    <row r="169" spans="2:3">
+    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" s="14" t="s">
         <v>253</v>
       </c>
@@ -5105,7 +5031,7 @@
         <v>607</v>
       </c>
     </row>
-    <row r="170" spans="2:3">
+    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" s="14" t="s">
         <v>248</v>
       </c>
@@ -5113,7 +5039,7 @@
         <v>608</v>
       </c>
     </row>
-    <row r="171" spans="2:3">
+    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" s="14" t="s">
         <v>229</v>
       </c>
@@ -5121,7 +5047,7 @@
         <v>609</v>
       </c>
     </row>
-    <row r="172" spans="2:3">
+    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" s="14" t="s">
         <v>230</v>
       </c>
@@ -5129,7 +5055,7 @@
         <v>610</v>
       </c>
     </row>
-    <row r="173" spans="2:3">
+    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" s="14" t="s">
         <v>259</v>
       </c>
@@ -5137,7 +5063,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="174" spans="2:3">
+    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" s="14" t="s">
         <v>227</v>
       </c>
@@ -5145,7 +5071,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="175" spans="2:3">
+    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" s="14" t="s">
         <v>226</v>
       </c>
@@ -5153,7 +5079,7 @@
         <v>611</v>
       </c>
     </row>
-    <row r="176" spans="2:3">
+    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" s="14" t="s">
         <v>240</v>
       </c>
@@ -5161,7 +5087,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="177" spans="2:3">
+    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" s="14" t="s">
         <v>270</v>
       </c>
@@ -5169,7 +5095,7 @@
         <v>613</v>
       </c>
     </row>
-    <row r="178" spans="2:3">
+    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" s="14" t="s">
         <v>275</v>
       </c>
@@ -5177,7 +5103,7 @@
         <v>614</v>
       </c>
     </row>
-    <row r="179" spans="2:3">
+    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" s="14" t="s">
         <v>268</v>
       </c>
@@ -5185,7 +5111,7 @@
         <v>615</v>
       </c>
     </row>
-    <row r="180" spans="2:3">
+    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" s="14" t="s">
         <v>267</v>
       </c>
@@ -5193,7 +5119,7 @@
         <v>616</v>
       </c>
     </row>
-    <row r="181" spans="2:3">
+    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" s="14" t="s">
         <v>271</v>
       </c>
@@ -5201,7 +5127,7 @@
         <v>617</v>
       </c>
     </row>
-    <row r="182" spans="2:3">
+    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" s="14" t="s">
         <v>272</v>
       </c>
@@ -5209,7 +5135,7 @@
         <v>618</v>
       </c>
     </row>
-    <row r="183" spans="2:3">
+    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" s="14" t="s">
         <v>277</v>
       </c>
@@ -5217,7 +5143,7 @@
         <v>619</v>
       </c>
     </row>
-    <row r="184" spans="2:3">
+    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" s="14" t="s">
         <v>284</v>
       </c>
@@ -5225,7 +5151,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="185" spans="2:3">
+    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" s="14" t="s">
         <v>285</v>
       </c>
@@ -5233,592 +5159,592 @@
         <v>621</v>
       </c>
     </row>
-    <row r="186" spans="2:3">
+    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" s="14" t="s">
         <v>273</v>
       </c>
       <c r="C186"/>
     </row>
-    <row r="187" spans="2:3">
+    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" s="14" t="s">
         <v>278</v>
       </c>
       <c r="C187"/>
     </row>
-    <row r="188" spans="2:3">
+    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" s="14" t="s">
         <v>280</v>
       </c>
       <c r="C188"/>
     </row>
-    <row r="189" spans="2:3">
+    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" s="14" t="s">
         <v>283</v>
       </c>
       <c r="C189"/>
     </row>
-    <row r="190" spans="2:3">
+    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" s="14" t="s">
         <v>274</v>
       </c>
       <c r="C190"/>
     </row>
-    <row r="191" spans="2:3">
+    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" s="14" t="s">
         <v>266</v>
       </c>
       <c r="C191"/>
     </row>
-    <row r="192" spans="2:3">
+    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" s="14" t="s">
         <v>287</v>
       </c>
       <c r="C192"/>
     </row>
-    <row r="193" spans="2:3">
+    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" s="14" t="s">
         <v>286</v>
       </c>
       <c r="C193"/>
     </row>
-    <row r="194" spans="2:3">
+    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" s="14" t="s">
         <v>44</v>
       </c>
       <c r="C194"/>
     </row>
-    <row r="195" spans="2:3">
+    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" s="14" t="s">
         <v>289</v>
       </c>
       <c r="C195"/>
     </row>
-    <row r="196" spans="2:3">
+    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" s="14" t="s">
         <v>288</v>
       </c>
       <c r="C196"/>
     </row>
-    <row r="197" spans="2:3">
+    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" s="14" t="s">
         <v>302</v>
       </c>
       <c r="C197"/>
     </row>
-    <row r="198" spans="2:3">
+    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" s="14" t="s">
         <v>291</v>
       </c>
       <c r="C198"/>
     </row>
-    <row r="199" spans="2:3">
+    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" s="14" t="s">
         <v>296</v>
       </c>
       <c r="C199"/>
     </row>
-    <row r="200" spans="2:3">
+    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" s="14" t="s">
         <v>305</v>
       </c>
       <c r="C200"/>
     </row>
-    <row r="201" spans="2:3">
+    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" s="14" t="s">
         <v>293</v>
       </c>
       <c r="C201"/>
     </row>
-    <row r="202" spans="2:3">
+    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" s="14" t="s">
         <v>298</v>
       </c>
       <c r="C202"/>
     </row>
-    <row r="203" spans="2:3">
+    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" s="14" t="s">
         <v>290</v>
       </c>
       <c r="C203"/>
     </row>
-    <row r="204" spans="2:3">
+    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" s="14" t="s">
         <v>299</v>
       </c>
       <c r="C204"/>
     </row>
-    <row r="205" spans="2:3">
+    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" s="14" t="s">
         <v>300</v>
       </c>
       <c r="C205"/>
     </row>
-    <row r="206" spans="2:3">
+    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" s="14" t="s">
         <v>292</v>
       </c>
       <c r="C206"/>
     </row>
-    <row r="207" spans="2:3">
+    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" s="14" t="s">
         <v>308</v>
       </c>
       <c r="C207"/>
     </row>
-    <row r="208" spans="2:3">
+    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" s="14" t="s">
         <v>309</v>
       </c>
       <c r="C208"/>
     </row>
-    <row r="209" spans="2:3">
+    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" s="14" t="s">
         <v>311</v>
       </c>
       <c r="C209"/>
     </row>
-    <row r="210" spans="2:3">
+    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" s="14" t="s">
         <v>307</v>
       </c>
       <c r="C210"/>
     </row>
-    <row r="211" spans="2:3">
+    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" s="14" t="s">
         <v>294</v>
       </c>
       <c r="C211"/>
     </row>
-    <row r="212" spans="2:3">
+    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" s="14" t="s">
         <v>304</v>
       </c>
       <c r="C212"/>
     </row>
-    <row r="213" spans="2:3">
+    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" s="14" t="s">
         <v>313</v>
       </c>
       <c r="C213"/>
     </row>
-    <row r="214" spans="2:3">
+    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" s="14" t="s">
         <v>312</v>
       </c>
       <c r="C214"/>
     </row>
-    <row r="215" spans="2:3">
+    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" s="14" t="s">
         <v>315</v>
       </c>
       <c r="C215"/>
     </row>
-    <row r="216" spans="2:3">
+    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" s="14" t="s">
         <v>316</v>
       </c>
       <c r="C216"/>
     </row>
-    <row r="217" spans="2:3">
+    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" s="14" t="s">
         <v>314</v>
       </c>
       <c r="C217"/>
     </row>
-    <row r="218" spans="2:3">
+    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" s="14" t="s">
         <v>317</v>
       </c>
       <c r="C218"/>
     </row>
-    <row r="219" spans="2:3">
+    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" s="14" t="s">
         <v>318</v>
       </c>
       <c r="C219"/>
     </row>
-    <row r="220" spans="2:3">
+    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" s="14" t="s">
         <v>319</v>
       </c>
       <c r="C220"/>
     </row>
-    <row r="221" spans="2:3">
+    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" s="14" t="s">
         <v>320</v>
       </c>
       <c r="C221"/>
     </row>
-    <row r="222" spans="2:3">
+    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" s="14" t="s">
         <v>323</v>
       </c>
       <c r="C222"/>
     </row>
-    <row r="223" spans="2:3">
+    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" s="14" t="s">
         <v>322</v>
       </c>
       <c r="C223"/>
     </row>
-    <row r="224" spans="2:3">
+    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" s="14" t="s">
         <v>331</v>
       </c>
       <c r="C224"/>
     </row>
-    <row r="225" spans="2:3">
+    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" s="14" t="s">
         <v>329</v>
       </c>
       <c r="C225"/>
     </row>
-    <row r="226" spans="2:3">
+    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" s="14" t="s">
         <v>328</v>
       </c>
       <c r="C226"/>
     </row>
-    <row r="227" spans="2:3">
+    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" s="14" t="s">
         <v>326</v>
       </c>
       <c r="C227"/>
     </row>
-    <row r="228" spans="2:3">
+    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" s="14" t="s">
         <v>324</v>
       </c>
       <c r="C228"/>
     </row>
-    <row r="229" spans="2:3">
+    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229" s="14" t="s">
         <v>325</v>
       </c>
       <c r="C229"/>
     </row>
-    <row r="230" spans="2:3">
+    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" s="14" t="s">
         <v>327</v>
       </c>
       <c r="C230"/>
     </row>
-    <row r="231" spans="2:3">
+    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" s="14" t="s">
         <v>330</v>
       </c>
       <c r="C231"/>
     </row>
-    <row r="232" spans="2:3">
+    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" s="14" t="s">
         <v>332</v>
       </c>
       <c r="C232"/>
     </row>
-    <row r="233" spans="2:3">
+    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" s="14" t="s">
         <v>333</v>
       </c>
       <c r="C233"/>
     </row>
-    <row r="234" spans="2:3">
+    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C234"/>
     </row>
-    <row r="235" spans="2:3">
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C235"/>
     </row>
-    <row r="236" spans="2:3">
+    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C236"/>
     </row>
-    <row r="237" spans="2:3">
+    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C237"/>
     </row>
-    <row r="238" spans="2:3">
+    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C238"/>
     </row>
-    <row r="239" spans="2:3">
+    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C239"/>
     </row>
-    <row r="240" spans="2:3">
+    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C240"/>
     </row>
-    <row r="241" spans="3:3">
+    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C241"/>
     </row>
-    <row r="242" spans="3:3">
+    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C242"/>
     </row>
-    <row r="243" spans="3:3">
+    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C243"/>
     </row>
-    <row r="244" spans="3:3">
+    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C244"/>
     </row>
-    <row r="245" spans="3:3">
+    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C245"/>
     </row>
-    <row r="246" spans="3:3">
+    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C246"/>
     </row>
-    <row r="247" spans="3:3">
+    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C247"/>
     </row>
-    <row r="248" spans="3:3">
+    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C248"/>
     </row>
-    <row r="249" spans="3:3">
+    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C249"/>
     </row>
-    <row r="250" spans="3:3">
+    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C250"/>
     </row>
-    <row r="251" spans="3:3">
+    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C251"/>
     </row>
-    <row r="252" spans="3:3">
+    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C252"/>
     </row>
-    <row r="253" spans="3:3">
+    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C253"/>
     </row>
-    <row r="254" spans="3:3">
+    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C254"/>
     </row>
-    <row r="255" spans="3:3">
+    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C255"/>
     </row>
-    <row r="256" spans="3:3">
+    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C256"/>
     </row>
-    <row r="257" spans="3:3">
+    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C257"/>
     </row>
-    <row r="258" spans="3:3">
+    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C258"/>
     </row>
-    <row r="259" spans="3:3">
+    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C259"/>
     </row>
-    <row r="260" spans="3:3">
+    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C260"/>
     </row>
-    <row r="261" spans="3:3">
+    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C261"/>
     </row>
-    <row r="262" spans="3:3">
+    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C262"/>
     </row>
-    <row r="263" spans="3:3">
+    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C263"/>
     </row>
-    <row r="264" spans="3:3">
+    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C264"/>
     </row>
-    <row r="265" spans="3:3">
+    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C265"/>
     </row>
-    <row r="266" spans="3:3">
+    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C266"/>
     </row>
-    <row r="267" spans="3:3">
+    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C267"/>
     </row>
-    <row r="268" spans="3:3">
+    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C268"/>
     </row>
-    <row r="269" spans="3:3">
+    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C269"/>
     </row>
-    <row r="270" spans="3:3">
+    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C270"/>
     </row>
-    <row r="271" spans="3:3">
+    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C271"/>
     </row>
-    <row r="272" spans="3:3">
+    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C272"/>
     </row>
-    <row r="273" spans="3:3">
+    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C273"/>
     </row>
-    <row r="274" spans="3:3">
+    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C274"/>
     </row>
-    <row r="275" spans="3:3">
+    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C275"/>
     </row>
-    <row r="276" spans="3:3">
+    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C276"/>
     </row>
-    <row r="277" spans="3:3">
+    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C277"/>
     </row>
-    <row r="278" spans="3:3">
+    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C278"/>
     </row>
-    <row r="279" spans="3:3">
+    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C279"/>
     </row>
-    <row r="280" spans="3:3">
+    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C280"/>
     </row>
-    <row r="281" spans="3:3">
+    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C281"/>
     </row>
-    <row r="282" spans="3:3">
+    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C282"/>
     </row>
-    <row r="283" spans="3:3">
+    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C283"/>
     </row>
-    <row r="284" spans="3:3">
+    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C284"/>
     </row>
-    <row r="285" spans="3:3">
+    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C285"/>
     </row>
-    <row r="286" spans="3:3">
+    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C286"/>
     </row>
-    <row r="287" spans="3:3">
+    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C287"/>
     </row>
-    <row r="288" spans="3:3">
+    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C288"/>
     </row>
-    <row r="289" spans="3:3">
+    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C289"/>
     </row>
-    <row r="290" spans="3:3">
+    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C290"/>
     </row>
-    <row r="291" spans="3:3">
+    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C291"/>
     </row>
-    <row r="292" spans="3:3">
+    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C292"/>
     </row>
-    <row r="293" spans="3:3">
+    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C293"/>
     </row>
-    <row r="294" spans="3:3">
+    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C294"/>
     </row>
-    <row r="295" spans="3:3">
+    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C295"/>
     </row>
-    <row r="296" spans="3:3">
+    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C296"/>
     </row>
-    <row r="297" spans="3:3">
+    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C297"/>
     </row>
-    <row r="298" spans="3:3">
+    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C298"/>
     </row>
-    <row r="299" spans="3:3">
+    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C299"/>
     </row>
-    <row r="300" spans="3:3">
+    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C300"/>
     </row>
-    <row r="301" spans="3:3">
+    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C301"/>
     </row>
-    <row r="302" spans="3:3">
+    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C302"/>
     </row>
-    <row r="303" spans="3:3">
+    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C303"/>
     </row>
-    <row r="304" spans="3:3">
+    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C304"/>
     </row>
-    <row r="305" spans="3:3">
+    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C305"/>
     </row>
-    <row r="306" spans="3:3">
+    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C306"/>
     </row>
-    <row r="307" spans="3:3">
+    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C307"/>
     </row>
-    <row r="308" spans="3:3">
+    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C308"/>
     </row>
-    <row r="309" spans="3:3">
+    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C309"/>
     </row>
-    <row r="310" spans="3:3">
+    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C310"/>
     </row>
-    <row r="311" spans="3:3">
+    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C311"/>
     </row>
-    <row r="312" spans="3:3">
+    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C312"/>
     </row>
-    <row r="313" spans="3:3">
+    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C313"/>
     </row>
-    <row r="314" spans="3:3">
+    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C314"/>
     </row>
-    <row r="315" spans="3:3">
+    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C315"/>
     </row>
-    <row r="316" spans="3:3">
+    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C316"/>
     </row>
-    <row r="317" spans="3:3">
+    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C317"/>
     </row>
-    <row r="318" spans="3:3">
+    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C318"/>
     </row>
-    <row r="319" spans="3:3">
+    <row r="319" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C319"/>
     </row>
-    <row r="320" spans="3:3">
+    <row r="320" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C320"/>
     </row>
-    <row r="321" spans="3:3">
+    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C321"/>
     </row>
-    <row r="322" spans="3:3">
+    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C322"/>
     </row>
-    <row r="323" spans="3:3">
+    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C323"/>
     </row>
-    <row r="324" spans="3:3">
+    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C324"/>
     </row>
-    <row r="325" spans="3:3">
+    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C325"/>
     </row>
-    <row r="326" spans="3:3">
+    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C326"/>
     </row>
-    <row r="327" spans="3:3">
+    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C327"/>
     </row>
-    <row r="328" spans="3:3">
+    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C328"/>
     </row>
-    <row r="329" spans="3:3">
+    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C329"/>
     </row>
-    <row r="330" spans="3:3">
+    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C330"/>
     </row>
-    <row r="331" spans="3:3">
+    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C331"/>
     </row>
-    <row r="332" spans="3:3">
+    <row r="332" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C332"/>
     </row>
-    <row r="333" spans="3:3">
+    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C333"/>
     </row>
   </sheetData>
@@ -5826,12 +5752,7 @@
     <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -5839,23 +5760,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F63"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="36.5" style="7" customWidth="1"/>
+    <col min="1" max="1" width="36.42578125" style="7" customWidth="1"/>
     <col min="2" max="2" width="24" style="7" customWidth="1"/>
-    <col min="3" max="3" width="30.83203125" style="7" customWidth="1"/>
-    <col min="4" max="4" width="29.33203125" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.5" style="7" customWidth="1"/>
-    <col min="6" max="6" width="15.1640625" style="14" customWidth="1"/>
-    <col min="7" max="7" width="38.5" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="8.83203125" style="7"/>
+    <col min="3" max="3" width="30.85546875" style="7" customWidth="1"/>
+    <col min="4" max="4" width="29.28515625" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="7" customWidth="1"/>
+    <col min="7" max="7" width="38.42578125" style="7" customWidth="1"/>
+    <col min="8" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>486</v>
       </c>
@@ -5871,11 +5791,8 @@
       <c r="E1" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="F1" s="14" t="s">
-        <v>633</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>485</v>
       </c>
@@ -5891,11 +5808,8 @@
       <c r="E2" s="7" t="s">
         <v>497</v>
       </c>
-      <c r="F2" s="11" t="s">
-        <v>634</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>526</v>
       </c>
@@ -5911,11 +5825,8 @@
       <c r="E3" s="7" t="s">
         <v>499</v>
       </c>
-      <c r="F3" s="11" t="s">
-        <v>635</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>527</v>
       </c>
@@ -5931,11 +5842,8 @@
       <c r="E4" s="7" t="s">
         <v>500</v>
       </c>
-      <c r="F4" s="11" t="s">
-        <v>636</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>367</v>
       </c>
@@ -5948,11 +5856,8 @@
       <c r="E5" s="7" t="s">
         <v>498</v>
       </c>
-      <c r="F5" s="12" t="s">
-        <v>637</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>370</v>
       </c>
@@ -5962,11 +5867,8 @@
       <c r="D6" s="7" t="s">
         <v>369</v>
       </c>
-      <c r="F6" s="18" t="s">
-        <v>638</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>373</v>
       </c>
@@ -5976,11 +5878,8 @@
       <c r="D7" s="7" t="s">
         <v>372</v>
       </c>
-      <c r="F7" s="21" t="s">
-        <v>639</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>375</v>
       </c>
@@ -5990,11 +5889,8 @@
       <c r="D8" s="7" t="s">
         <v>374</v>
       </c>
-      <c r="F8" s="11" t="s">
-        <v>640</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>378</v>
       </c>
@@ -6004,11 +5900,8 @@
       <c r="D9" s="7" t="s">
         <v>377</v>
       </c>
-      <c r="F9" s="12" t="s">
-        <v>641</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>381</v>
       </c>
@@ -6018,11 +5911,8 @@
       <c r="D10" s="7" t="s">
         <v>380</v>
       </c>
-      <c r="F10" s="12" t="s">
-        <v>642</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>384</v>
       </c>
@@ -6032,11 +5922,8 @@
       <c r="D11" s="7" t="s">
         <v>383</v>
       </c>
-      <c r="F11" s="21" t="s">
-        <v>643</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>387</v>
       </c>
@@ -6046,11 +5933,8 @@
       <c r="D12" s="7" t="s">
         <v>386</v>
       </c>
-      <c r="F12" s="11" t="s">
-        <v>644</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>390</v>
       </c>
@@ -6060,11 +5944,8 @@
       <c r="D13" s="7" t="s">
         <v>389</v>
       </c>
-      <c r="F13" s="12" t="s">
-        <v>645</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>392</v>
       </c>
@@ -6074,11 +5955,8 @@
       <c r="D14" s="7" t="s">
         <v>391</v>
       </c>
-      <c r="F14" s="12" t="s">
-        <v>646</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>393</v>
       </c>
@@ -6088,33 +5966,24 @@
       <c r="D15" s="7" t="s">
         <v>358</v>
       </c>
-      <c r="F15" s="21" t="s">
-        <v>647</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>395</v>
       </c>
       <c r="D16" s="7" t="s">
         <v>394</v>
       </c>
-      <c r="F16" s="11" t="s">
-        <v>648</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6">
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="8" t="s">
         <v>397</v>
       </c>
       <c r="D17" s="7" t="s">
         <v>396</v>
       </c>
-      <c r="F17" s="12" t="s">
-        <v>649</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6">
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="8" t="s">
         <v>399</v>
       </c>
@@ -6122,7 +5991,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="19" spans="2:6">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="8" t="s">
         <v>401</v>
       </c>
@@ -6130,7 +5999,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="2:6">
+    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B20" s="8" t="s">
         <v>403</v>
       </c>
@@ -6138,7 +6007,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="21" spans="2:6">
+    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B21" s="8" t="s">
         <v>405</v>
       </c>
@@ -6146,216 +6015,211 @@
         <v>404</v>
       </c>
     </row>
-    <row r="22" spans="2:6">
+    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D22" s="7" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="23" spans="2:6">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D23" s="7" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="24" spans="2:6">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D24" s="7" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="25" spans="2:6">
+    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D25" s="7" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="26" spans="2:6">
+    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D26" s="7" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="27" spans="2:6">
+    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D27" s="7" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="28" spans="2:6">
+    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D28" s="7" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="29" spans="2:6">
+    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D29" s="7" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="30" spans="2:6">
+    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D30" s="7" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="31" spans="2:6">
+    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D31" s="7" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="32" spans="2:6">
+    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
       <c r="D32" s="7" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="33" spans="4:4">
+    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D33" s="7" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="34" spans="4:4">
+    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D34" s="7" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="35" spans="4:4">
+    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D35" s="7" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="36" spans="4:4">
+    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D36" s="7" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="37" spans="4:4">
+    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D37" s="7" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="38" spans="4:4">
+    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D38" s="7" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="39" spans="4:4">
+    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D39" s="7" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="40" spans="4:4">
+    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D40" s="7" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="41" spans="4:4">
+    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D41" s="7" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="42" spans="4:4">
+    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D42" s="7" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="43" spans="4:4">
+    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D43" s="7" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="44" spans="4:4">
+    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D44" s="7" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="45" spans="4:4">
+    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D45" s="7" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="46" spans="4:4">
+    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D46" s="7" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="4:4">
+    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D47" s="7" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="48" spans="4:4">
+    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D48" s="7" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="49" spans="4:4">
+    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D49" s="7" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="50" spans="4:4">
+    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D50" s="7" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="51" spans="4:4">
+    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D51" s="7" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="4:4">
+    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D52" s="7" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="53" spans="4:4">
+    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D53" s="7" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="54" spans="4:4">
+    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D54" s="7" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="55" spans="4:4">
+    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D55" s="7" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="56" spans="4:4">
+    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D56" s="7" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="57" spans="4:4">
+    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D57" s="7" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="58" spans="4:4">
+    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D58" s="7" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="59" spans="4:4">
+    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D59" s="7" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="60" spans="4:4">
+    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D60" s="7" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="61" spans="4:4">
+    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D61" s="9"/>
     </row>
-    <row r="62" spans="4:4">
+    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D62" s="9"/>
     </row>
-    <row r="63" spans="4:4">
+    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D63" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Added new identifier type Identifier:identifier. DM-161
</commit_message>
<xml_diff>
--- a/WebContent/files/xls_standard_input_template.xlsx
+++ b/WebContent/files/xls_standard_input_template.xlsx
@@ -5,18 +5,18 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\MSD\DOMM\Excel standard input\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/rejohnson_ucsd_edu/Documents/Workspace/Latest Excel template/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
     <sheet name="Select-a-header values" sheetId="14" r:id="rId2"/>
     <sheet name="CV values" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="647" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="634">
   <si>
     <t>text</t>
   </si>
@@ -2060,6 +2060,9 @@
   </si>
   <si>
     <t>Note:related publications</t>
+  </si>
+  <si>
+    <t>Identifier:identifier</t>
   </si>
 </sst>
 </file>
@@ -2691,7 +2694,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2736,6 +2739,7 @@
     <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3138,8 +3142,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G25" sqref="G25"/>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3302,7 +3306,7 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$G$1:$G$13</xm:f>
+            <xm:f>'Select-a-header values'!$G$1:$G$17</xm:f>
           </x14:formula1>
           <xm:sqref>S1</xm:sqref>
         </x14:dataValidation>
@@ -3326,15 +3330,15 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$F$1:$F$20</xm:f>
+            <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
-          <xm:sqref>R1</xm:sqref>
+          <xm:sqref>Q1</xm:sqref>
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$E$1:$E$29</xm:f>
+            <xm:f>'Select-a-header values'!$F$1:$F$21</xm:f>
           </x14:formula1>
-          <xm:sqref>Q1</xm:sqref>
+          <xm:sqref>R1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3346,8 +3350,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3408,7 +3412,7 @@
       <c r="F2" s="11" t="s">
         <v>491</v>
       </c>
-      <c r="G2" s="11" t="s">
+      <c r="G2" s="22" t="s">
         <v>510</v>
       </c>
       <c r="H2" s="12" t="s">
@@ -3634,7 +3638,7 @@
         <v>631</v>
       </c>
       <c r="F11" s="11" t="s">
-        <v>494</v>
+        <v>633</v>
       </c>
       <c r="G11" s="21" t="s">
         <v>626</v>
@@ -3655,7 +3659,7 @@
         <v>461</v>
       </c>
       <c r="F12" s="11" t="s">
-        <v>15</v>
+        <v>494</v>
       </c>
       <c r="G12" s="11" t="s">
         <v>335</v>
@@ -3676,7 +3680,7 @@
         <v>339</v>
       </c>
       <c r="F13" s="11" t="s">
-        <v>495</v>
+        <v>15</v>
       </c>
       <c r="G13" s="12" t="s">
         <v>459</v>
@@ -3695,7 +3699,7 @@
         <v>462</v>
       </c>
       <c r="F14" s="11" t="s">
-        <v>5</v>
+        <v>495</v>
       </c>
       <c r="G14" s="12" t="s">
         <v>512</v>
@@ -3712,7 +3716,7 @@
         <v>505</v>
       </c>
       <c r="F15" s="11" t="s">
-        <v>16</v>
+        <v>5</v>
       </c>
       <c r="G15" s="21" t="s">
         <v>627</v>
@@ -3729,7 +3733,7 @@
         <v>506</v>
       </c>
       <c r="F16" s="11" t="s">
-        <v>496</v>
+        <v>16</v>
       </c>
       <c r="G16" s="11" t="s">
         <v>334</v>
@@ -3746,7 +3750,7 @@
         <v>507</v>
       </c>
       <c r="F17" s="11" t="s">
-        <v>17</v>
+        <v>496</v>
       </c>
       <c r="G17" s="12" t="s">
         <v>460</v>
@@ -3763,7 +3767,7 @@
         <v>463</v>
       </c>
       <c r="F18" s="11" t="s">
-        <v>516</v>
+        <v>17</v>
       </c>
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
@@ -3777,7 +3781,7 @@
         <v>464</v>
       </c>
       <c r="F19" s="11" t="s">
-        <v>504</v>
+        <v>516</v>
       </c>
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
@@ -3791,7 +3795,7 @@
         <v>508</v>
       </c>
       <c r="F20" s="11" t="s">
-        <v>18</v>
+        <v>504</v>
       </c>
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
@@ -3803,6 +3807,9 @@
       </c>
       <c r="E21" s="12" t="s">
         <v>484</v>
+      </c>
+      <c r="F21" s="11" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixes #138 - Updated MARC CSV mapping for multiple roles and new note types.
</commit_message>
<xml_diff>
--- a/WebContent/files/xls_standard_input_template.xlsx
+++ b/WebContent/files/xls_standard_input_template.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://ucsdcloud-my.sharepoint.com/personal/rejohnson_ucsd_edu/Documents/Workspace/Latest Excel template/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greser\dams-metadata\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="648" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="635">
   <si>
     <t>text</t>
   </si>
@@ -2063,6 +2063,9 @@
   </si>
   <si>
     <t>Identifier:identifier</t>
+  </si>
+  <si>
+    <t>Note:work title</t>
   </si>
 </sst>
 </file>
@@ -3142,7 +3145,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:U1"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+    <sheetView topLeftCell="M1" workbookViewId="0">
       <selection activeCell="Q2" sqref="Q2"/>
     </sheetView>
   </sheetViews>
@@ -3350,8 +3353,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R333"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="F22" sqref="F22"/>
+    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
+      <selection activeCell="E35" sqref="E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3961,6 +3964,9 @@
       </c>
       <c r="C35" s="14" t="s">
         <v>547</v>
+      </c>
+      <c r="E35" s="14" t="s">
+        <v>634</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Fixes #140 - Changed MARC to CSV Mapping for code 700 12 from Note:work title to Note:work featured.
</commit_message>
<xml_diff>
--- a/WebContent/files/xls_standard_input_template.xlsx
+++ b/WebContent/files/xls_standard_input_template.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23790" windowHeight="11835" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25755" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -17,6 +17,7 @@
     <sheet name="CV values" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
+  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -2065,7 +2066,7 @@
     <t>Identifier:identifier</t>
   </si>
   <si>
-    <t>Note:work title</t>
+    <t>Note:work featured</t>
   </si>
 </sst>
 </file>
@@ -3353,8 +3354,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C7" workbookViewId="0">
-      <selection activeCell="E35" sqref="E35"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="F37" sqref="F37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Fixes #180 - Updated the Excel standard input template to add new roles.
</commit_message>
<xml_diff>
--- a/WebContent/files/xls_standard_input_template.xlsx
+++ b/WebContent/files/xls_standard_input_template.xlsx
@@ -17,7 +17,6 @@
     <sheet name="CV values" sheetId="10" r:id="rId3"/>
   </sheets>
   <calcPr calcId="152511"/>
-  <fileRecoveryPr repairLoad="1"/>
 </workbook>
 </file>
 
@@ -162,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="649" uniqueCount="635">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="655">
   <si>
     <t>text</t>
   </si>
@@ -2067,13 +2066,73 @@
   </si>
   <si>
     <t>Note:work featured</t>
+  </si>
+  <si>
+    <t>Access granted</t>
+  </si>
+  <si>
+    <t>Copyright status</t>
+  </si>
+  <si>
+    <t>Copyright holder</t>
+  </si>
+  <si>
+    <t>CC license</t>
+  </si>
+  <si>
+    <t>Library curators only</t>
+  </si>
+  <si>
+    <t>Under copyright</t>
+  </si>
+  <si>
+    <t>Attribution</t>
+  </si>
+  <si>
+    <t>UCSD IP only</t>
+  </si>
+  <si>
+    <t>Public Domain</t>
+  </si>
+  <si>
+    <t>Attribution-ShareAlike</t>
+  </si>
+  <si>
+    <t>The world - metadata and files</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>Attribution-NoDerivs</t>
+  </si>
+  <si>
+    <t>The world - metadata only</t>
+  </si>
+  <si>
+    <t>Attribution-NonCommercial</t>
+  </si>
+  <si>
+    <t>The world - cultural sensitivity click through</t>
+  </si>
+  <si>
+    <t>Attribution-NonCommercial-ShareAlike</t>
+  </si>
+  <si>
+    <t>Attribution-NonCommercial-NoDerivs</t>
+  </si>
+  <si>
+    <t>Person:Co-Director</t>
+  </si>
+  <si>
+    <t>Person:Associate Director</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="33" x14ac:knownFonts="1">
+  <fonts count="34" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2303,8 +2362,14 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="38">
+  <fills count="40">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2513,6 +2578,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="11">
     <border>
@@ -2698,7 +2775,7 @@
     <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="23">
+  <cellXfs count="30">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -2744,6 +2821,15 @@
     <xf numFmtId="49" fontId="32" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="38" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="33" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="51">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -3144,10 +3230,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:U1"/>
+  <dimension ref="A1:Y1"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" workbookViewId="0">
-      <selection activeCell="Q2" sqref="Q2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3171,9 +3257,13 @@
     <col min="19" max="19" width="42.85546875" style="3" customWidth="1"/>
     <col min="20" max="20" width="44.5703125" style="3" customWidth="1"/>
     <col min="21" max="21" width="84.28515625" style="3" customWidth="1"/>
+    <col min="22" max="22" width="43.5703125" customWidth="1"/>
+    <col min="23" max="23" width="17" customWidth="1"/>
+    <col min="24" max="24" width="30.28515625" customWidth="1"/>
+    <col min="25" max="25" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3236,6 +3326,18 @@
       </c>
       <c r="U1" s="16" t="s">
         <v>525</v>
+      </c>
+      <c r="V1" s="24" t="s">
+        <v>635</v>
+      </c>
+      <c r="W1" s="24" t="s">
+        <v>636</v>
+      </c>
+      <c r="X1" s="24" t="s">
+        <v>637</v>
+      </c>
+      <c r="Y1" s="24" t="s">
+        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -3265,7 +3367,7 @@
   <legacyDrawing r:id="rId2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="13">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid entry" error="Please choose a value from the dropdown list" prompt="Please choose a value from the dropdown list">
           <x14:formula1>
             <xm:f>'CV values'!$B$2:$B$21</xm:f>
@@ -3328,12 +3430,6 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$B$1:$B$233</xm:f>
-          </x14:formula1>
-          <xm:sqref>K1</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
-          <x14:formula1>
             <xm:f>'Select-a-header values'!$E$1:$E$34</xm:f>
           </x14:formula1>
           <xm:sqref>Q1</xm:sqref>
@@ -3343,6 +3439,30 @@
             <xm:f>'Select-a-header values'!$F$1:$F$21</xm:f>
           </x14:formula1>
           <xm:sqref>R1</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'CV values'!$F$2:$F$6</xm:f>
+          </x14:formula1>
+          <xm:sqref>V2:V1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'CV values'!$G$2:$G$4</xm:f>
+          </x14:formula1>
+          <xm:sqref>W2:W1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+          <x14:formula1>
+            <xm:f>'CV values'!$H$2:$H$7</xm:f>
+          </x14:formula1>
+          <xm:sqref>Y2:Y1048576</xm:sqref>
+        </x14:dataValidation>
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
+          <x14:formula1>
+            <xm:f>'Select-a-header values'!$B$1:$B$235</xm:f>
+          </x14:formula1>
+          <xm:sqref>K1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -3354,8 +3474,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="F37" sqref="F37"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="38.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3575,7 +3695,7 @@
       <c r="C8" s="14" t="s">
         <v>534</v>
       </c>
-      <c r="E8" s="11" t="s">
+      <c r="E8" s="27" t="s">
         <v>4</v>
       </c>
       <c r="F8" s="11" t="s">
@@ -3596,7 +3716,7 @@
       <c r="C9" s="14" t="s">
         <v>535</v>
       </c>
-      <c r="E9" s="18" t="s">
+      <c r="E9" s="28" t="s">
         <v>630</v>
       </c>
       <c r="F9" s="11" t="s">
@@ -3617,7 +3737,7 @@
       <c r="C10" s="14" t="s">
         <v>536</v>
       </c>
-      <c r="E10" s="11" t="s">
+      <c r="E10" s="27" t="s">
         <v>350</v>
       </c>
       <c r="F10" s="11" t="s">
@@ -3638,7 +3758,7 @@
       <c r="C11" s="14" t="s">
         <v>537</v>
       </c>
-      <c r="E11" s="18" t="s">
+      <c r="E11" s="28" t="s">
         <v>631</v>
       </c>
       <c r="F11" s="11" t="s">
@@ -3659,7 +3779,7 @@
       <c r="C12" s="10" t="s">
         <v>38</v>
       </c>
-      <c r="E12" s="11" t="s">
+      <c r="E12" s="27" t="s">
         <v>461</v>
       </c>
       <c r="F12" s="11" t="s">
@@ -3680,7 +3800,7 @@
       <c r="C13" s="14" t="s">
         <v>538</v>
       </c>
-      <c r="E13" s="11" t="s">
+      <c r="E13" s="27" t="s">
         <v>339</v>
       </c>
       <c r="F13" s="11" t="s">
@@ -3699,7 +3819,7 @@
       <c r="C14" s="14" t="s">
         <v>539</v>
       </c>
-      <c r="E14" s="11" t="s">
+      <c r="E14" s="27" t="s">
         <v>462</v>
       </c>
       <c r="F14" s="11" t="s">
@@ -3716,7 +3836,7 @@
       <c r="C15" s="14" t="s">
         <v>540</v>
       </c>
-      <c r="E15" s="11" t="s">
+      <c r="E15" s="27" t="s">
         <v>505</v>
       </c>
       <c r="F15" s="11" t="s">
@@ -3733,7 +3853,7 @@
       <c r="C16" s="14" t="s">
         <v>541</v>
       </c>
-      <c r="E16" s="11" t="s">
+      <c r="E16" s="27" t="s">
         <v>506</v>
       </c>
       <c r="F16" s="11" t="s">
@@ -3744,13 +3864,13 @@
       </c>
     </row>
     <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="14" t="s">
-        <v>37</v>
+      <c r="B17" s="26" t="s">
+        <v>654</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>542</v>
       </c>
-      <c r="E17" s="11" t="s">
+      <c r="E17" s="27" t="s">
         <v>507</v>
       </c>
       <c r="F17" s="11" t="s">
@@ -3762,12 +3882,12 @@
     </row>
     <row r="18" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B18" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>29</v>
       </c>
-      <c r="E18" s="11" t="s">
+      <c r="E18" s="27" t="s">
         <v>463</v>
       </c>
       <c r="F18" s="11" t="s">
@@ -3776,12 +3896,12 @@
     </row>
     <row r="19" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="E19" s="11" t="s">
+      <c r="E19" s="27" t="s">
         <v>464</v>
       </c>
       <c r="F19" s="11" t="s">
@@ -3790,12 +3910,12 @@
     </row>
     <row r="20" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="E20" s="11" t="s">
+      <c r="E20" s="27" t="s">
         <v>508</v>
       </c>
       <c r="F20" s="11" t="s">
@@ -3804,12 +3924,12 @@
     </row>
     <row r="21" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B21" s="14" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>543</v>
       </c>
-      <c r="E21" s="12" t="s">
+      <c r="E21" s="29" t="s">
         <v>484</v>
       </c>
       <c r="F21" s="11" t="s">
@@ -3818,161 +3938,161 @@
     </row>
     <row r="22" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B22" s="14" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>51</v>
       </c>
-      <c r="E22" s="11" t="s">
+      <c r="E22" s="27" t="s">
         <v>351</v>
       </c>
     </row>
     <row r="23" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>53</v>
       </c>
-      <c r="E23" s="11" t="s">
+      <c r="E23" s="27" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="24" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B24" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="E24" s="11" t="s">
+      <c r="E24" s="27" t="s">
         <v>352</v>
       </c>
     </row>
     <row r="25" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B25" s="14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="E25" s="11" t="s">
+      <c r="E25" s="27" t="s">
         <v>353</v>
       </c>
     </row>
     <row r="26" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="E26" s="18" t="s">
+      <c r="E26" s="28" t="s">
         <v>632</v>
       </c>
     </row>
     <row r="27" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B27" s="14" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="E27" s="11" t="s">
+      <c r="E27" s="27" t="s">
         <v>354</v>
       </c>
     </row>
     <row r="28" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B28" s="14" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>544</v>
       </c>
-      <c r="E28" s="11" t="s">
+      <c r="E28" s="27" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="29" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B29" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>545</v>
       </c>
-      <c r="E29" s="18" t="s">
+      <c r="E29" s="28" t="s">
         <v>629</v>
       </c>
     </row>
     <row r="30" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B30" s="14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>77</v>
       </c>
-      <c r="E30" s="11" t="s">
+      <c r="E30" s="27" t="s">
         <v>355</v>
       </c>
     </row>
     <row r="31" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B31" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="E31" s="11" t="s">
+      <c r="E31" s="27" t="s">
         <v>356</v>
       </c>
     </row>
     <row r="32" spans="2:7" x14ac:dyDescent="0.25">
       <c r="B32" s="14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>84</v>
       </c>
-      <c r="E32" s="11" t="s">
+      <c r="E32" s="27" t="s">
         <v>509</v>
       </c>
     </row>
     <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33" s="14" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>80</v>
       </c>
-      <c r="E33" s="11" t="s">
+      <c r="E33" s="27" t="s">
         <v>357</v>
       </c>
     </row>
     <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>546</v>
       </c>
-      <c r="E34" s="11" t="s">
+      <c r="E34" s="27" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>547</v>
       </c>
-      <c r="E35" s="14" t="s">
+      <c r="E35" s="28" t="s">
         <v>634</v>
       </c>
     </row>
     <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36" s="14" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>548</v>
@@ -3981,7 +4101,7 @@
     </row>
     <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B37" s="14" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>111</v>
@@ -3990,7 +4110,7 @@
     </row>
     <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B38" s="14" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>549</v>
@@ -3999,7 +4119,7 @@
     </row>
     <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B39" s="14" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>94</v>
@@ -4007,7 +4127,7 @@
     </row>
     <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B40" s="14" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>95</v>
@@ -4015,7 +4135,7 @@
     </row>
     <row r="41" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B41" s="14" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>550</v>
@@ -4023,7 +4143,7 @@
     </row>
     <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B42" s="14" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>551</v>
@@ -4031,15 +4151,15 @@
     </row>
     <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" s="14" t="s">
-        <v>83</v>
+        <v>66</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>552</v>
       </c>
     </row>
     <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="14" t="s">
-        <v>79</v>
+      <c r="B44" s="25" t="s">
+        <v>653</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>553</v>
@@ -4047,7 +4167,7 @@
     </row>
     <row r="45" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B45" s="14" t="s">
-        <v>70</v>
+        <v>83</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>554</v>
@@ -4055,7 +4175,7 @@
     </row>
     <row r="46" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B46" s="14" t="s">
-        <v>69</v>
+        <v>79</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>555</v>
@@ -4063,7 +4183,7 @@
     </row>
     <row r="47" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B47" s="14" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>85</v>
@@ -4071,7 +4191,7 @@
     </row>
     <row r="48" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B48" s="14" t="s">
-        <v>110</v>
+        <v>69</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>86</v>
@@ -4079,7 +4199,7 @@
     </row>
     <row r="49" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B49" s="14" t="s">
-        <v>81</v>
+        <v>71</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>78</v>
@@ -4087,7 +4207,7 @@
     </row>
     <row r="50" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B50" s="14" t="s">
-        <v>72</v>
+        <v>110</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>108</v>
@@ -4095,7 +4215,7 @@
     </row>
     <row r="51" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B51" s="14" t="s">
-        <v>73</v>
+        <v>81</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>105</v>
@@ -4103,7 +4223,7 @@
     </row>
     <row r="52" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B52" s="14" t="s">
-        <v>64</v>
+        <v>72</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>91</v>
@@ -4111,7 +4231,7 @@
     </row>
     <row r="53" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B53" s="14" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>93</v>
@@ -4119,7 +4239,7 @@
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B54" s="14" t="s">
-        <v>82</v>
+        <v>64</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>556</v>
@@ -4127,7 +4247,7 @@
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B55" s="14" t="s">
-        <v>101</v>
+        <v>74</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>88</v>
@@ -4135,7 +4255,7 @@
     </row>
     <row r="56" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B56" s="14" t="s">
-        <v>102</v>
+        <v>82</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>557</v>
@@ -4143,7 +4263,7 @@
     </row>
     <row r="57" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B57" s="14" t="s">
-        <v>107</v>
+        <v>101</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>97</v>
@@ -4151,7 +4271,7 @@
     </row>
     <row r="58" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B58" s="14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>468</v>
@@ -4159,7 +4279,7 @@
     </row>
     <row r="59" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B59" s="14" t="s">
-        <v>467</v>
+        <v>107</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>130</v>
@@ -4167,7 +4287,7 @@
     </row>
     <row r="60" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B60" s="14" t="s">
-        <v>90</v>
+        <v>104</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>558</v>
@@ -4175,7 +4295,7 @@
     </row>
     <row r="61" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B61" s="14" t="s">
-        <v>92</v>
+        <v>467</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>113</v>
@@ -4183,7 +4303,7 @@
     </row>
     <row r="62" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B62" s="14" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>122</v>
@@ -4191,7 +4311,7 @@
     </row>
     <row r="63" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B63" s="14" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>126</v>
@@ -4199,7 +4319,7 @@
     </row>
     <row r="64" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B64" s="14" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>112</v>
@@ -4207,7 +4327,7 @@
     </row>
     <row r="65" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B65" s="14" t="s">
-        <v>87</v>
+        <v>98</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>128</v>
@@ -4215,7 +4335,7 @@
     </row>
     <row r="66" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B66" s="14" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>119</v>
@@ -4223,7 +4343,7 @@
     </row>
     <row r="67" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B67" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>559</v>
@@ -4231,7 +4351,7 @@
     </row>
     <row r="68" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B68" s="14" t="s">
-        <v>96</v>
+        <v>100</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>560</v>
@@ -4239,7 +4359,7 @@
     </row>
     <row r="69" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B69" s="14" t="s">
-        <v>109</v>
+        <v>89</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>561</v>
@@ -4247,7 +4367,7 @@
     </row>
     <row r="70" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B70" s="14" t="s">
-        <v>117</v>
+        <v>96</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>562</v>
@@ -4255,7 +4375,7 @@
     </row>
     <row r="71" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B71" s="14" t="s">
-        <v>129</v>
+        <v>109</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>563</v>
@@ -4263,7 +4383,7 @@
     </row>
     <row r="72" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B72" s="14" t="s">
-        <v>132</v>
+        <v>117</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>143</v>
@@ -4271,7 +4391,7 @@
     </row>
     <row r="73" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B73" s="14" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>564</v>
@@ -4279,7 +4399,7 @@
     </row>
     <row r="74" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B74" s="14" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>565</v>
@@ -4287,7 +4407,7 @@
     </row>
     <row r="75" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B75" s="14" t="s">
-        <v>114</v>
+        <v>131</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>566</v>
@@ -4295,7 +4415,7 @@
     </row>
     <row r="76" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B76" s="14" t="s">
-        <v>116</v>
+        <v>133</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>145</v>
@@ -4303,7 +4423,7 @@
     </row>
     <row r="77" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B77" s="14" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>567</v>
@@ -4311,7 +4431,7 @@
     </row>
     <row r="78" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B78" s="14" t="s">
-        <v>121</v>
+        <v>116</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>568</v>
@@ -4319,7 +4439,7 @@
     </row>
     <row r="79" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B79" s="14" t="s">
-        <v>125</v>
+        <v>120</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>149</v>
@@ -4327,7 +4447,7 @@
     </row>
     <row r="80" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B80" s="14" t="s">
-        <v>124</v>
+        <v>121</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>157</v>
@@ -4335,7 +4455,7 @@
     </row>
     <row r="81" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B81" s="14" t="s">
-        <v>115</v>
+        <v>125</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>569</v>
@@ -4343,7 +4463,7 @@
     </row>
     <row r="82" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B82" s="14" t="s">
-        <v>127</v>
+        <v>124</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>161</v>
@@ -4351,7 +4471,7 @@
     </row>
     <row r="83" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B83" s="14" t="s">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>155</v>
@@ -4359,7 +4479,7 @@
     </row>
     <row r="84" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B84" s="14" t="s">
-        <v>123</v>
+        <v>127</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>159</v>
@@ -4367,7 +4487,7 @@
     </row>
     <row r="85" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B85" s="14" t="s">
-        <v>134</v>
+        <v>118</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>570</v>
@@ -4375,7 +4495,7 @@
     </row>
     <row r="86" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B86" s="14" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>167</v>
@@ -4383,7 +4503,7 @@
     </row>
     <row r="87" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B87" s="14" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>164</v>
@@ -4391,7 +4511,7 @@
     </row>
     <row r="88" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B88" s="14" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>171</v>
@@ -4399,7 +4519,7 @@
     </row>
     <row r="89" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B89" s="14" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>169</v>
@@ -4407,7 +4527,7 @@
     </row>
     <row r="90" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B90" s="14" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>173</v>
@@ -4415,7 +4535,7 @@
     </row>
     <row r="91" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B91" s="14" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>571</v>
@@ -4423,7 +4543,7 @@
     </row>
     <row r="92" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B92" s="14" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>175</v>
@@ -4431,7 +4551,7 @@
     </row>
     <row r="93" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B93" s="14" t="s">
-        <v>138</v>
+        <v>142</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>179</v>
@@ -4439,7 +4559,7 @@
     </row>
     <row r="94" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B94" s="14" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>181</v>
@@ -4447,7 +4567,7 @@
     </row>
     <row r="95" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B95" s="14" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>572</v>
@@ -4455,7 +4575,7 @@
     </row>
     <row r="96" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B96" s="14" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>573</v>
@@ -4463,7 +4583,7 @@
     </row>
     <row r="97" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B97" s="14" t="s">
-        <v>469</v>
+        <v>146</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>186</v>
@@ -4471,7 +4591,7 @@
     </row>
     <row r="98" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B98" s="14" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C98" s="14" t="s">
         <v>574</v>
@@ -4479,7 +4599,7 @@
     </row>
     <row r="99" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B99" s="14" t="s">
-        <v>152</v>
+        <v>469</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>190</v>
@@ -4487,7 +4607,7 @@
     </row>
     <row r="100" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B100" s="14" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>192</v>
@@ -4495,7 +4615,7 @@
     </row>
     <row r="101" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B101" s="14" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="C101" s="14" t="s">
         <v>575</v>
@@ -4503,7 +4623,7 @@
     </row>
     <row r="102" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B102" s="14" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="C102" s="14" t="s">
         <v>576</v>
@@ -4511,7 +4631,7 @@
     </row>
     <row r="103" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B103" s="14" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C103" s="14" t="s">
         <v>577</v>
@@ -4519,7 +4639,7 @@
     </row>
     <row r="104" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B104" s="14" t="s">
-        <v>160</v>
+        <v>156</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>200</v>
@@ -4527,7 +4647,7 @@
     </row>
     <row r="105" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B105" s="14" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>202</v>
@@ -4535,7 +4655,7 @@
     </row>
     <row r="106" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B106" s="14" t="s">
-        <v>154</v>
+        <v>160</v>
       </c>
       <c r="C106" s="14" t="s">
         <v>578</v>
@@ -4543,7 +4663,7 @@
     </row>
     <row r="107" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B107" s="14" t="s">
-        <v>158</v>
+        <v>162</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>199</v>
@@ -4551,7 +4671,7 @@
     </row>
     <row r="108" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B108" s="14" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>197</v>
@@ -4559,7 +4679,7 @@
     </row>
     <row r="109" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B109" s="14" t="s">
-        <v>165</v>
+        <v>158</v>
       </c>
       <c r="C109" s="14" t="s">
         <v>579</v>
@@ -4567,7 +4687,7 @@
     </row>
     <row r="110" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B110" s="14" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>205</v>
@@ -4575,7 +4695,7 @@
     </row>
     <row r="111" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B111" s="14" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="C111" s="14" t="s">
         <v>580</v>
@@ -4583,7 +4703,7 @@
     </row>
     <row r="112" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B112" s="14" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="C112" s="14" t="s">
         <v>581</v>
@@ -4591,7 +4711,7 @@
     </row>
     <row r="113" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B113" s="14" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="C113" s="10" t="s">
         <v>214</v>
@@ -4599,7 +4719,7 @@
     </row>
     <row r="114" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B114" s="14" t="s">
-        <v>176</v>
+        <v>168</v>
       </c>
       <c r="C114" s="10" t="s">
         <v>218</v>
@@ -4607,7 +4727,7 @@
     </row>
     <row r="115" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B115" s="14" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="C115" s="10" t="s">
         <v>216</v>
@@ -4615,7 +4735,7 @@
     </row>
     <row r="116" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B116" s="14" t="s">
-        <v>178</v>
+        <v>176</v>
       </c>
       <c r="C116" s="10" t="s">
         <v>221</v>
@@ -4623,7 +4743,7 @@
     </row>
     <row r="117" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B117" s="14" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="C117" s="10" t="s">
         <v>223</v>
@@ -4631,7 +4751,7 @@
     </row>
     <row r="118" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B118" s="14" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
       <c r="C118" s="14" t="s">
         <v>582</v>
@@ -4639,7 +4759,7 @@
     </row>
     <row r="119" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B119" s="14" t="s">
-        <v>470</v>
+        <v>174</v>
       </c>
       <c r="C119" s="10" t="s">
         <v>262</v>
@@ -4647,7 +4767,7 @@
     </row>
     <row r="120" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B120" s="14" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="C120" s="10" t="s">
         <v>264</v>
@@ -4655,7 +4775,7 @@
     </row>
     <row r="121" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B121" s="14" t="s">
-        <v>188</v>
+        <v>470</v>
       </c>
       <c r="C121" s="14" t="s">
         <v>583</v>
@@ -4663,7 +4783,7 @@
     </row>
     <row r="122" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B122" s="14" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="C122" s="14" t="s">
         <v>584</v>
@@ -4671,7 +4791,7 @@
     </row>
     <row r="123" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B123" s="14" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="C123" s="10" t="s">
         <v>234</v>
@@ -4679,7 +4799,7 @@
     </row>
     <row r="124" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B124" s="14" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="C124" s="14" t="s">
         <v>585</v>
@@ -4687,7 +4807,7 @@
     </row>
     <row r="125" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B125" s="14" t="s">
-        <v>189</v>
+        <v>185</v>
       </c>
       <c r="C125" s="10" t="s">
         <v>233</v>
@@ -4695,7 +4815,7 @@
     </row>
     <row r="126" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B126" s="14" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="C126" s="10" t="s">
         <v>242</v>
@@ -4703,7 +4823,7 @@
     </row>
     <row r="127" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B127" s="14" t="s">
-        <v>187</v>
+        <v>189</v>
       </c>
       <c r="C127" s="10" t="s">
         <v>258</v>
@@ -4711,7 +4831,7 @@
     </row>
     <row r="128" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B128" s="14" t="s">
-        <v>193</v>
+        <v>191</v>
       </c>
       <c r="C128" s="10" t="s">
         <v>238</v>
@@ -4719,7 +4839,7 @@
     </row>
     <row r="129" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B129" s="14" t="s">
-        <v>194</v>
+        <v>187</v>
       </c>
       <c r="C129" s="10" t="s">
         <v>250</v>
@@ -4727,7 +4847,7 @@
     </row>
     <row r="130" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B130" s="14" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="C130" s="10" t="s">
         <v>244</v>
@@ -4735,7 +4855,7 @@
     </row>
     <row r="131" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B131" s="14" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="C131" s="14" t="s">
         <v>586</v>
@@ -4743,7 +4863,7 @@
     </row>
     <row r="132" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B132" s="14" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="C132" s="10" t="s">
         <v>251</v>
@@ -4751,7 +4871,7 @@
     </row>
     <row r="133" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B133" s="14" t="s">
-        <v>198</v>
+        <v>206</v>
       </c>
       <c r="C133" s="10" t="s">
         <v>256</v>
@@ -4759,7 +4879,7 @@
     </row>
     <row r="134" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B134" s="14" t="s">
-        <v>196</v>
+        <v>207</v>
       </c>
       <c r="C134" s="10" t="s">
         <v>236</v>
@@ -4767,7 +4887,7 @@
     </row>
     <row r="135" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B135" s="14" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C135" s="10" t="s">
         <v>254</v>
@@ -4775,7 +4895,7 @@
     </row>
     <row r="136" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B136" s="14" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="C136" s="14" t="s">
         <v>587</v>
@@ -4783,7 +4903,7 @@
     </row>
     <row r="137" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B137" s="14" t="s">
-        <v>203</v>
+        <v>209</v>
       </c>
       <c r="C137" s="14" t="s">
         <v>588</v>
@@ -4791,7 +4911,7 @@
     </row>
     <row r="138" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B138" s="14" t="s">
-        <v>204</v>
+        <v>210</v>
       </c>
       <c r="C138" s="14" t="s">
         <v>260</v>
@@ -4799,7 +4919,7 @@
     </row>
     <row r="139" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B139" s="14" t="s">
-        <v>195</v>
+        <v>203</v>
       </c>
       <c r="C139" s="10" t="s">
         <v>265</v>
@@ -4807,7 +4927,7 @@
     </row>
     <row r="140" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B140" s="14" t="s">
-        <v>208</v>
+        <v>204</v>
       </c>
       <c r="C140" s="10" t="s">
         <v>228</v>
@@ -4815,7 +4935,7 @@
     </row>
     <row r="141" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B141" s="14" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="C141" s="14" t="s">
         <v>589</v>
@@ -4823,7 +4943,7 @@
     </row>
     <row r="142" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B142" s="14" t="s">
-        <v>212</v>
+        <v>208</v>
       </c>
       <c r="C142" s="14" t="s">
         <v>590</v>
@@ -4831,7 +4951,7 @@
     </row>
     <row r="143" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B143" s="14" t="s">
-        <v>219</v>
+        <v>211</v>
       </c>
       <c r="C143" s="14" t="s">
         <v>591</v>
@@ -4839,7 +4959,7 @@
     </row>
     <row r="144" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B144" s="14" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C144" s="14" t="s">
         <v>592</v>
@@ -4847,7 +4967,7 @@
     </row>
     <row r="145" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B145" s="14" t="s">
-        <v>217</v>
+        <v>219</v>
       </c>
       <c r="C145" s="10" t="s">
         <v>276</v>
@@ -4855,7 +4975,7 @@
     </row>
     <row r="146" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B146" s="14" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C146" s="10" t="s">
         <v>282</v>
@@ -4863,7 +4983,7 @@
     </row>
     <row r="147" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B147" s="14" t="s">
-        <v>220</v>
+        <v>217</v>
       </c>
       <c r="C147" s="10" t="s">
         <v>279</v>
@@ -4871,7 +4991,7 @@
     </row>
     <row r="148" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B148" s="14" t="s">
-        <v>222</v>
+        <v>215</v>
       </c>
       <c r="C148" s="10" t="s">
         <v>281</v>
@@ -4879,7 +4999,7 @@
     </row>
     <row r="149" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B149" s="14" t="s">
-        <v>622</v>
+        <v>220</v>
       </c>
       <c r="C149" s="14" t="s">
         <v>593</v>
@@ -4887,7 +5007,7 @@
     </row>
     <row r="150" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B150" s="14" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
       <c r="C150" s="14" t="s">
         <v>594</v>
@@ -4895,7 +5015,7 @@
     </row>
     <row r="151" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B151" s="14" t="s">
-        <v>239</v>
+        <v>622</v>
       </c>
       <c r="C151" s="14" t="s">
         <v>595</v>
@@ -4903,7 +5023,7 @@
     </row>
     <row r="152" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B152" s="14" t="s">
-        <v>261</v>
+        <v>224</v>
       </c>
       <c r="C152" s="14" t="s">
         <v>596</v>
@@ -4911,7 +5031,7 @@
     </row>
     <row r="153" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B153" s="14" t="s">
-        <v>263</v>
+        <v>239</v>
       </c>
       <c r="C153" s="14" t="s">
         <v>597</v>
@@ -4919,7 +5039,7 @@
     </row>
     <row r="154" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B154" s="14" t="s">
-        <v>225</v>
+        <v>261</v>
       </c>
       <c r="C154" s="14" t="s">
         <v>598</v>
@@ -4927,7 +5047,7 @@
     </row>
     <row r="155" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B155" s="14" t="s">
-        <v>247</v>
+        <v>263</v>
       </c>
       <c r="C155" s="10" t="s">
         <v>303</v>
@@ -4935,7 +5055,7 @@
     </row>
     <row r="156" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B156" s="14" t="s">
-        <v>231</v>
+        <v>225</v>
       </c>
       <c r="C156" s="10" t="s">
         <v>297</v>
@@ -4943,7 +5063,7 @@
     </row>
     <row r="157" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B157" s="14" t="s">
-        <v>232</v>
+        <v>247</v>
       </c>
       <c r="C157" s="14" t="s">
         <v>599</v>
@@ -4951,7 +5071,7 @@
     </row>
     <row r="158" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B158" s="14" t="s">
-        <v>241</v>
+        <v>231</v>
       </c>
       <c r="C158" s="10" t="s">
         <v>306</v>
@@ -4959,7 +5079,7 @@
     </row>
     <row r="159" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B159" s="14" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="C159" s="14" t="s">
         <v>600</v>
@@ -4967,7 +5087,7 @@
     </row>
     <row r="160" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B160" s="14" t="s">
-        <v>471</v>
+        <v>241</v>
       </c>
       <c r="C160" s="14" t="s">
         <v>601</v>
@@ -4975,7 +5095,7 @@
     </row>
     <row r="161" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B161" s="14" t="s">
-        <v>257</v>
+        <v>246</v>
       </c>
       <c r="C161" s="14" t="s">
         <v>602</v>
@@ -4983,7 +5103,7 @@
     </row>
     <row r="162" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B162" s="14" t="s">
-        <v>237</v>
+        <v>471</v>
       </c>
       <c r="C162" s="10" t="s">
         <v>301</v>
@@ -4991,7 +5111,7 @@
     </row>
     <row r="163" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B163" s="14" t="s">
-        <v>249</v>
+        <v>257</v>
       </c>
       <c r="C163" s="14" t="s">
         <v>310</v>
@@ -4999,7 +5119,7 @@
     </row>
     <row r="164" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B164" s="14" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="C164" s="14" t="s">
         <v>603</v>
@@ -5007,7 +5127,7 @@
     </row>
     <row r="165" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B165" s="14" t="s">
-        <v>252</v>
+        <v>249</v>
       </c>
       <c r="C165" s="14" t="s">
         <v>295</v>
@@ -5015,7 +5135,7 @@
     </row>
     <row r="166" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B166" s="14" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="C166" s="14" t="s">
         <v>604</v>
@@ -5023,7 +5143,7 @@
     </row>
     <row r="167" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B167" s="14" t="s">
-        <v>235</v>
+        <v>252</v>
       </c>
       <c r="C167" s="14" t="s">
         <v>605</v>
@@ -5031,7 +5151,7 @@
     </row>
     <row r="168" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B168" s="14" t="s">
-        <v>245</v>
+        <v>255</v>
       </c>
       <c r="C168" s="14" t="s">
         <v>606</v>
@@ -5039,7 +5159,7 @@
     </row>
     <row r="169" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B169" s="14" t="s">
-        <v>253</v>
+        <v>235</v>
       </c>
       <c r="C169" s="14" t="s">
         <v>607</v>
@@ -5047,7 +5167,7 @@
     </row>
     <row r="170" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B170" s="14" t="s">
-        <v>248</v>
+        <v>245</v>
       </c>
       <c r="C170" s="14" t="s">
         <v>608</v>
@@ -5055,7 +5175,7 @@
     </row>
     <row r="171" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B171" s="14" t="s">
-        <v>229</v>
+        <v>253</v>
       </c>
       <c r="C171" s="14" t="s">
         <v>609</v>
@@ -5063,7 +5183,7 @@
     </row>
     <row r="172" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B172" s="14" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="C172" s="14" t="s">
         <v>610</v>
@@ -5071,7 +5191,7 @@
     </row>
     <row r="173" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B173" s="14" t="s">
-        <v>259</v>
+        <v>229</v>
       </c>
       <c r="C173" s="10" t="s">
         <v>321</v>
@@ -5079,7 +5199,7 @@
     </row>
     <row r="174" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B174" s="14" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="C174" s="10" t="s">
         <v>472</v>
@@ -5087,7 +5207,7 @@
     </row>
     <row r="175" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B175" s="14" t="s">
-        <v>226</v>
+        <v>259</v>
       </c>
       <c r="C175" s="14" t="s">
         <v>611</v>
@@ -5095,7 +5215,7 @@
     </row>
     <row r="176" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B176" s="14" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C176" s="14" t="s">
         <v>612</v>
@@ -5103,7 +5223,7 @@
     </row>
     <row r="177" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B177" s="14" t="s">
-        <v>270</v>
+        <v>226</v>
       </c>
       <c r="C177" s="14" t="s">
         <v>613</v>
@@ -5111,7 +5231,7 @@
     </row>
     <row r="178" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B178" s="14" t="s">
-        <v>275</v>
+        <v>240</v>
       </c>
       <c r="C178" s="14" t="s">
         <v>614</v>
@@ -5119,7 +5239,7 @@
     </row>
     <row r="179" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B179" s="14" t="s">
-        <v>268</v>
+        <v>270</v>
       </c>
       <c r="C179" s="14" t="s">
         <v>615</v>
@@ -5127,7 +5247,7 @@
     </row>
     <row r="180" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B180" s="14" t="s">
-        <v>267</v>
+        <v>275</v>
       </c>
       <c r="C180" s="14" t="s">
         <v>616</v>
@@ -5135,7 +5255,7 @@
     </row>
     <row r="181" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B181" s="14" t="s">
-        <v>271</v>
+        <v>268</v>
       </c>
       <c r="C181" s="14" t="s">
         <v>617</v>
@@ -5143,7 +5263,7 @@
     </row>
     <row r="182" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B182" s="14" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="C182" s="14" t="s">
         <v>618</v>
@@ -5151,7 +5271,7 @@
     </row>
     <row r="183" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B183" s="14" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="C183" s="14" t="s">
         <v>619</v>
@@ -5159,7 +5279,7 @@
     </row>
     <row r="184" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B184" s="14" t="s">
-        <v>284</v>
+        <v>272</v>
       </c>
       <c r="C184" s="14" t="s">
         <v>620</v>
@@ -5167,7 +5287,7 @@
     </row>
     <row r="185" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B185" s="14" t="s">
-        <v>285</v>
+        <v>277</v>
       </c>
       <c r="C185" s="14" t="s">
         <v>621</v>
@@ -5175,296 +5295,302 @@
     </row>
     <row r="186" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B186" s="14" t="s">
-        <v>273</v>
+        <v>284</v>
       </c>
       <c r="C186"/>
     </row>
     <row r="187" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B187" s="14" t="s">
-        <v>278</v>
+        <v>285</v>
       </c>
       <c r="C187"/>
     </row>
     <row r="188" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B188" s="14" t="s">
-        <v>280</v>
+        <v>273</v>
       </c>
       <c r="C188"/>
     </row>
     <row r="189" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B189" s="14" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="C189"/>
     </row>
     <row r="190" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B190" s="14" t="s">
-        <v>274</v>
+        <v>280</v>
       </c>
       <c r="C190"/>
     </row>
     <row r="191" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B191" s="14" t="s">
-        <v>266</v>
+        <v>283</v>
       </c>
       <c r="C191"/>
     </row>
     <row r="192" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B192" s="14" t="s">
-        <v>287</v>
+        <v>274</v>
       </c>
       <c r="C192"/>
     </row>
     <row r="193" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B193" s="14" t="s">
-        <v>286</v>
+        <v>266</v>
       </c>
       <c r="C193"/>
     </row>
     <row r="194" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B194" s="14" t="s">
-        <v>44</v>
+        <v>287</v>
       </c>
       <c r="C194"/>
     </row>
     <row r="195" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B195" s="14" t="s">
-        <v>289</v>
+        <v>286</v>
       </c>
       <c r="C195"/>
     </row>
     <row r="196" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B196" s="14" t="s">
-        <v>288</v>
+        <v>44</v>
       </c>
       <c r="C196"/>
     </row>
     <row r="197" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B197" s="14" t="s">
-        <v>302</v>
+        <v>289</v>
       </c>
       <c r="C197"/>
     </row>
     <row r="198" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B198" s="14" t="s">
-        <v>291</v>
+        <v>288</v>
       </c>
       <c r="C198"/>
     </row>
     <row r="199" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B199" s="14" t="s">
-        <v>296</v>
+        <v>302</v>
       </c>
       <c r="C199"/>
     </row>
     <row r="200" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B200" s="14" t="s">
-        <v>305</v>
+        <v>291</v>
       </c>
       <c r="C200"/>
     </row>
     <row r="201" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B201" s="14" t="s">
-        <v>293</v>
+        <v>296</v>
       </c>
       <c r="C201"/>
     </row>
     <row r="202" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B202" s="14" t="s">
-        <v>298</v>
+        <v>305</v>
       </c>
       <c r="C202"/>
     </row>
     <row r="203" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B203" s="14" t="s">
-        <v>290</v>
+        <v>293</v>
       </c>
       <c r="C203"/>
     </row>
     <row r="204" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B204" s="14" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
       <c r="C204"/>
     </row>
     <row r="205" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B205" s="14" t="s">
-        <v>300</v>
+        <v>290</v>
       </c>
       <c r="C205"/>
     </row>
     <row r="206" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B206" s="14" t="s">
-        <v>292</v>
+        <v>299</v>
       </c>
       <c r="C206"/>
     </row>
     <row r="207" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B207" s="14" t="s">
-        <v>308</v>
+        <v>300</v>
       </c>
       <c r="C207"/>
     </row>
     <row r="208" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B208" s="14" t="s">
-        <v>309</v>
+        <v>292</v>
       </c>
       <c r="C208"/>
     </row>
     <row r="209" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B209" s="14" t="s">
-        <v>311</v>
+        <v>308</v>
       </c>
       <c r="C209"/>
     </row>
     <row r="210" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B210" s="14" t="s">
-        <v>307</v>
+        <v>309</v>
       </c>
       <c r="C210"/>
     </row>
     <row r="211" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B211" s="14" t="s">
-        <v>294</v>
+        <v>311</v>
       </c>
       <c r="C211"/>
     </row>
     <row r="212" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B212" s="14" t="s">
-        <v>304</v>
+        <v>307</v>
       </c>
       <c r="C212"/>
     </row>
     <row r="213" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B213" s="14" t="s">
-        <v>313</v>
+        <v>294</v>
       </c>
       <c r="C213"/>
     </row>
     <row r="214" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B214" s="14" t="s">
-        <v>312</v>
+        <v>304</v>
       </c>
       <c r="C214"/>
     </row>
     <row r="215" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B215" s="14" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C215"/>
     </row>
     <row r="216" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B216" s="14" t="s">
-        <v>316</v>
+        <v>312</v>
       </c>
       <c r="C216"/>
     </row>
     <row r="217" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B217" s="14" t="s">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="C217"/>
     </row>
     <row r="218" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B218" s="14" t="s">
-        <v>317</v>
+        <v>316</v>
       </c>
       <c r="C218"/>
     </row>
     <row r="219" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B219" s="14" t="s">
-        <v>318</v>
+        <v>314</v>
       </c>
       <c r="C219"/>
     </row>
     <row r="220" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B220" s="14" t="s">
-        <v>319</v>
+        <v>317</v>
       </c>
       <c r="C220"/>
     </row>
     <row r="221" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B221" s="14" t="s">
-        <v>320</v>
+        <v>318</v>
       </c>
       <c r="C221"/>
     </row>
     <row r="222" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B222" s="14" t="s">
-        <v>323</v>
+        <v>319</v>
       </c>
       <c r="C222"/>
     </row>
     <row r="223" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B223" s="14" t="s">
-        <v>322</v>
+        <v>320</v>
       </c>
       <c r="C223"/>
     </row>
     <row r="224" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B224" s="14" t="s">
-        <v>331</v>
+        <v>323</v>
       </c>
       <c r="C224"/>
     </row>
     <row r="225" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B225" s="14" t="s">
-        <v>329</v>
+        <v>322</v>
       </c>
       <c r="C225"/>
     </row>
     <row r="226" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B226" s="14" t="s">
-        <v>328</v>
+        <v>331</v>
       </c>
       <c r="C226"/>
     </row>
     <row r="227" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B227" s="14" t="s">
-        <v>326</v>
+        <v>329</v>
       </c>
       <c r="C227"/>
     </row>
     <row r="228" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B228" s="14" t="s">
-        <v>324</v>
+        <v>328</v>
       </c>
       <c r="C228"/>
     </row>
     <row r="229" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B229" s="14" t="s">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="C229"/>
     </row>
     <row r="230" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B230" s="14" t="s">
-        <v>327</v>
+        <v>324</v>
       </c>
       <c r="C230"/>
     </row>
     <row r="231" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B231" s="14" t="s">
-        <v>330</v>
+        <v>325</v>
       </c>
       <c r="C231"/>
     </row>
     <row r="232" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B232" s="14" t="s">
-        <v>332</v>
+        <v>327</v>
       </c>
       <c r="C232"/>
     </row>
     <row r="233" spans="2:3" x14ac:dyDescent="0.25">
       <c r="B233" s="14" t="s">
+        <v>330</v>
+      </c>
+      <c r="C233"/>
+    </row>
+    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B234" s="14" t="s">
+        <v>332</v>
+      </c>
+      <c r="C234"/>
+    </row>
+    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B235" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="C233"/>
-    </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="C234"/>
-    </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C235"/>
     </row>
     <row r="236" spans="2:3" x14ac:dyDescent="0.25">
@@ -5772,10 +5898,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F63"/>
+  <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5785,11 +5911,13 @@
     <col min="3" max="3" width="30.85546875" style="7" customWidth="1"/>
     <col min="4" max="4" width="29.28515625" style="7" customWidth="1"/>
     <col min="5" max="5" width="25.5703125" style="7" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" style="7" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="7"/>
+    <col min="6" max="6" width="42.85546875" customWidth="1"/>
+    <col min="7" max="7" width="19.28515625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="41.140625" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="9.140625" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>486</v>
       </c>
@@ -5805,8 +5933,17 @@
       <c r="E1" s="6" t="s">
         <v>349</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="6" t="s">
+        <v>635</v>
+      </c>
+      <c r="G1" s="6" t="s">
+        <v>636</v>
+      </c>
+      <c r="H1" s="6" t="s">
+        <v>638</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="7" t="s">
         <v>485</v>
       </c>
@@ -5822,8 +5959,17 @@
       <c r="E2" s="7" t="s">
         <v>497</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>639</v>
+      </c>
+      <c r="G2" t="s">
+        <v>640</v>
+      </c>
+      <c r="H2" s="23" t="s">
+        <v>641</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
         <v>526</v>
       </c>
@@ -5839,8 +5985,17 @@
       <c r="E3" s="7" t="s">
         <v>499</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" t="s">
+        <v>642</v>
+      </c>
+      <c r="G3" t="s">
+        <v>643</v>
+      </c>
+      <c r="H3" s="23" t="s">
+        <v>644</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>527</v>
       </c>
@@ -5856,8 +6011,17 @@
       <c r="E4" s="7" t="s">
         <v>500</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" t="s">
+        <v>645</v>
+      </c>
+      <c r="G4" t="s">
+        <v>646</v>
+      </c>
+      <c r="H4" s="23" t="s">
+        <v>647</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B5" s="8" t="s">
         <v>367</v>
       </c>
@@ -5870,8 +6034,15 @@
       <c r="E5" s="7" t="s">
         <v>498</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" t="s">
+        <v>648</v>
+      </c>
+      <c r="G5"/>
+      <c r="H5" s="23" t="s">
+        <v>649</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B6" s="8" t="s">
         <v>370</v>
       </c>
@@ -5881,8 +6052,15 @@
       <c r="D6" s="7" t="s">
         <v>369</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>650</v>
+      </c>
+      <c r="G6"/>
+      <c r="H6" s="23" t="s">
+        <v>651</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B7" s="8" t="s">
         <v>373</v>
       </c>
@@ -5892,8 +6070,12 @@
       <c r="D7" s="7" t="s">
         <v>372</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="G7"/>
+      <c r="H7" s="23" t="s">
+        <v>652</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B8" s="8" t="s">
         <v>375</v>
       </c>
@@ -5904,7 +6086,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B9" s="8" t="s">
         <v>378</v>
       </c>
@@ -5915,7 +6097,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B10" s="8" t="s">
         <v>381</v>
       </c>
@@ -5926,7 +6108,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B11" s="8" t="s">
         <v>384</v>
       </c>
@@ -5937,7 +6119,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B12" s="8" t="s">
         <v>387</v>
       </c>
@@ -5948,7 +6130,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B13" s="8" t="s">
         <v>390</v>
       </c>
@@ -5959,7 +6141,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B14" s="8" t="s">
         <v>392</v>
       </c>
@@ -5970,7 +6152,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B15" s="8" t="s">
         <v>393</v>
       </c>
@@ -5981,7 +6163,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="B16" s="8" t="s">
         <v>395</v>
       </c>
@@ -6235,5 +6417,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes #307 - Add Person:Advisor to Excel Standard InputStream.
</commit_message>
<xml_diff>
--- a/WebContent/files/xls_standard_input_template.xlsx
+++ b/WebContent/files/xls_standard_input_template.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="124226"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\greser\dams-metadata\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
+  <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25755" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25760" windowHeight="11640" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
     <sheet name="Select-a-header values" sheetId="14" r:id="rId2"/>
     <sheet name="CV values" sheetId="10" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -26,7 +26,7 @@
     <author>Windows User</author>
   </authors>
   <commentList>
-    <comment ref="G1" authorId="0" shapeId="0">
+    <comment ref="G1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -40,7 +40,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="M1" authorId="0" shapeId="0">
+    <comment ref="M1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -72,7 +72,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="N1" authorId="0" shapeId="0">
+    <comment ref="N1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -107,7 +107,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="O1" authorId="0" shapeId="0">
+    <comment ref="O1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -142,7 +142,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="P1" authorId="0" shapeId="0">
+    <comment ref="P1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -161,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="672" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="673" uniqueCount="656">
   <si>
     <t>text</t>
   </si>
@@ -2126,6 +2126,9 @@
   </si>
   <si>
     <t>Person:Associate Director</t>
+  </si>
+  <si>
+    <t>Person:Advisor</t>
   </si>
 </sst>
 </file>
@@ -2986,7 +2989,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3021,7 +3024,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -3236,34 +3239,34 @@
       <selection activeCell="E29" sqref="E29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="1" width="21" style="3" customWidth="1"/>
-    <col min="2" max="2" width="23.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="34.5703125" style="3" customWidth="1"/>
-    <col min="4" max="4" width="19.7109375" style="3" customWidth="1"/>
-    <col min="5" max="5" width="45.28515625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="19.7109375" style="3" customWidth="1"/>
-    <col min="7" max="7" width="23.85546875" style="3" customWidth="1"/>
-    <col min="8" max="8" width="16.28515625" style="3" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="23.5" style="3" customWidth="1"/>
+    <col min="3" max="3" width="34.5" style="3" customWidth="1"/>
+    <col min="4" max="4" width="19.6640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="45.33203125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="19.6640625" style="3" customWidth="1"/>
+    <col min="7" max="7" width="23.83203125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="16.33203125" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="22" style="3" customWidth="1"/>
-    <col min="10" max="10" width="51.5703125" style="3" customWidth="1"/>
-    <col min="11" max="12" width="45.140625" style="3" customWidth="1"/>
-    <col min="13" max="13" width="45.5703125" style="3" customWidth="1"/>
-    <col min="14" max="14" width="14.85546875" style="3" customWidth="1"/>
-    <col min="15" max="15" width="15.140625" style="3" customWidth="1"/>
-    <col min="16" max="16" width="19.85546875" style="3" customWidth="1"/>
-    <col min="17" max="18" width="39.140625" style="3" customWidth="1"/>
-    <col min="19" max="19" width="42.85546875" style="3" customWidth="1"/>
-    <col min="20" max="20" width="44.5703125" style="3" customWidth="1"/>
-    <col min="21" max="21" width="84.28515625" style="3" customWidth="1"/>
-    <col min="22" max="22" width="43.5703125" customWidth="1"/>
+    <col min="10" max="10" width="51.5" style="3" customWidth="1"/>
+    <col min="11" max="12" width="45.1640625" style="3" customWidth="1"/>
+    <col min="13" max="13" width="45.5" style="3" customWidth="1"/>
+    <col min="14" max="14" width="14.83203125" style="3" customWidth="1"/>
+    <col min="15" max="15" width="15.1640625" style="3" customWidth="1"/>
+    <col min="16" max="16" width="19.83203125" style="3" customWidth="1"/>
+    <col min="17" max="18" width="39.1640625" style="3" customWidth="1"/>
+    <col min="19" max="19" width="42.83203125" style="3" customWidth="1"/>
+    <col min="20" max="20" width="44.5" style="3" customWidth="1"/>
+    <col min="21" max="21" width="84.33203125" style="3" customWidth="1"/>
+    <col min="22" max="22" width="43.5" customWidth="1"/>
     <col min="23" max="23" width="17" customWidth="1"/>
-    <col min="24" max="24" width="30.28515625" customWidth="1"/>
+    <col min="24" max="24" width="30.33203125" customWidth="1"/>
     <col min="25" max="25" width="34" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:25" s="1" customFormat="1" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" s="1" customFormat="1" ht="22.5" customHeight="1">
       <c r="A1" s="15" t="s">
         <v>338</v>
       </c>
@@ -3363,8 +3366,8 @@
     <dataValidation allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Please select a value from the drop-down list" prompt="Please select a header from the drop-down list" sqref="I1"/>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
-  <legacyDrawing r:id="rId2"/>
+  <pageSetup orientation="portrait"/>
+  <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="16">
@@ -3460,11 +3463,14 @@
         </x14:dataValidation>
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid header" error="Please select a header from the drop-down list" prompt="Please select a header from the drop-down list">
           <x14:formula1>
-            <xm:f>'Select-a-header values'!$B$1:$B$235</xm:f>
+            <xm:f>'Select-a-header values'!$B$1:$B$236</xm:f>
           </x14:formula1>
           <xm:sqref>K1</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
+    </ext>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
     </ext>
   </extLst>
 </worksheet>
@@ -3474,21 +3480,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R333"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="38.5703125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="38.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="21.140625" style="14" customWidth="1"/>
-    <col min="2" max="3" width="41.28515625" style="14" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="14" customWidth="1"/>
-    <col min="5" max="5" width="43.7109375" style="14" customWidth="1"/>
-    <col min="6" max="18" width="38.5703125" style="14"/>
-    <col min="19" max="16384" width="38.5703125" style="11"/>
+    <col min="1" max="1" width="21.1640625" style="14" customWidth="1"/>
+    <col min="2" max="3" width="41.33203125" style="14" customWidth="1"/>
+    <col min="4" max="4" width="26.33203125" style="14" customWidth="1"/>
+    <col min="5" max="5" width="43.6640625" style="14" customWidth="1"/>
+    <col min="6" max="18" width="38.5" style="14"/>
+    <col min="19" max="16384" width="38.5" style="11"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9">
       <c r="A1" s="14" t="s">
         <v>517</v>
       </c>
@@ -3517,7 +3523,7 @@
         <v>525</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9">
       <c r="A2" s="14" t="s">
         <v>1</v>
       </c>
@@ -3546,7 +3552,7 @@
         <v>513</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9">
       <c r="A3" s="14" t="s">
         <v>445</v>
       </c>
@@ -3575,7 +3581,7 @@
         <v>476</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9">
       <c r="A4" s="14" t="s">
         <v>447</v>
       </c>
@@ -3604,7 +3610,7 @@
         <v>477</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9">
       <c r="A5" s="14" t="s">
         <v>449</v>
       </c>
@@ -3633,12 +3639,12 @@
         <v>478</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" ht="15">
       <c r="A6" s="14" t="s">
         <v>453</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>25</v>
+        <v>655</v>
       </c>
       <c r="C6" s="14" t="s">
         <v>532</v>
@@ -3662,12 +3668,12 @@
         <v>479</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9">
       <c r="A7" s="14" t="s">
         <v>457</v>
       </c>
       <c r="B7" s="14" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
         <v>533</v>
@@ -3688,9 +3694,9 @@
         <v>514</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9">
       <c r="B8" s="14" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C8" s="14" t="s">
         <v>534</v>
@@ -3709,9 +3715,9 @@
         <v>480</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9">
       <c r="B9" s="14" t="s">
-        <v>30</v>
+        <v>27</v>
       </c>
       <c r="C9" s="14" t="s">
         <v>535</v>
@@ -3730,9 +3736,9 @@
         <v>481</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9">
       <c r="B10" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C10" s="14" t="s">
         <v>536</v>
@@ -3751,9 +3757,9 @@
         <v>482</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9">
       <c r="B11" s="14" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="C11" s="14" t="s">
         <v>537</v>
@@ -3772,9 +3778,9 @@
         <v>483</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9">
       <c r="B12" s="14" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
       <c r="C12" s="10" t="s">
         <v>38</v>
@@ -3793,9 +3799,9 @@
         <v>515</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9">
       <c r="B13" s="14" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="C13" s="14" t="s">
         <v>538</v>
@@ -3812,9 +3818,9 @@
       <c r="H13" s="11"/>
       <c r="I13" s="11"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9">
       <c r="B14" s="14" t="s">
-        <v>35</v>
+        <v>22</v>
       </c>
       <c r="C14" s="14" t="s">
         <v>539</v>
@@ -3829,9 +3835,9 @@
         <v>512</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9">
       <c r="B15" s="14" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="C15" s="14" t="s">
         <v>540</v>
@@ -3846,9 +3852,9 @@
         <v>627</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9">
       <c r="B16" s="14" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C16" s="14" t="s">
         <v>541</v>
@@ -3863,9 +3869,9 @@
         <v>334</v>
       </c>
     </row>
-    <row r="17" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B17" s="26" t="s">
-        <v>654</v>
+    <row r="17" spans="2:7">
+      <c r="B17" s="14" t="s">
+        <v>36</v>
       </c>
       <c r="C17" s="14" t="s">
         <v>542</v>
@@ -3880,9 +3886,9 @@
         <v>460</v>
       </c>
     </row>
-    <row r="18" spans="2:7" x14ac:dyDescent="0.25">
-      <c r="B18" s="14" t="s">
-        <v>37</v>
+    <row r="18" spans="2:7">
+      <c r="B18" s="26" t="s">
+        <v>654</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>29</v>
@@ -3894,9 +3900,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="19" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:7">
       <c r="B19" s="14" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="C19" s="10" t="s">
         <v>56</v>
@@ -3908,9 +3914,9 @@
         <v>516</v>
       </c>
     </row>
-    <row r="20" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:7">
       <c r="B20" s="14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C20" s="10" t="s">
         <v>47</v>
@@ -3922,9 +3928,9 @@
         <v>504</v>
       </c>
     </row>
-    <row r="21" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:7">
       <c r="B21" s="14" t="s">
-        <v>45</v>
+        <v>41</v>
       </c>
       <c r="C21" s="14" t="s">
         <v>543</v>
@@ -3936,9 +3942,9 @@
         <v>18</v>
       </c>
     </row>
-    <row r="22" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:7">
       <c r="B22" s="14" t="s">
-        <v>31</v>
+        <v>45</v>
       </c>
       <c r="C22" s="10" t="s">
         <v>51</v>
@@ -3947,9 +3953,9 @@
         <v>351</v>
       </c>
     </row>
-    <row r="23" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:7">
       <c r="B23" s="14" t="s">
-        <v>24</v>
+        <v>31</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>53</v>
@@ -3958,9 +3964,9 @@
         <v>342</v>
       </c>
     </row>
-    <row r="24" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:7">
       <c r="B24" s="14" t="s">
-        <v>42</v>
+        <v>24</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>49</v>
@@ -3969,9 +3975,9 @@
         <v>352</v>
       </c>
     </row>
-    <row r="25" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:7">
       <c r="B25" s="14" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>58</v>
@@ -3980,9 +3986,9 @@
         <v>353</v>
       </c>
     </row>
-    <row r="26" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:7">
       <c r="B26" s="14" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C26" s="10" t="s">
         <v>62</v>
@@ -3991,9 +3997,9 @@
         <v>632</v>
       </c>
     </row>
-    <row r="27" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:7">
       <c r="B27" s="14" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="C27" s="10" t="s">
         <v>59</v>
@@ -4002,9 +4008,9 @@
         <v>354</v>
       </c>
     </row>
-    <row r="28" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:7">
       <c r="B28" s="14" t="s">
-        <v>55</v>
+        <v>28</v>
       </c>
       <c r="C28" s="14" t="s">
         <v>544</v>
@@ -4013,9 +4019,9 @@
         <v>465</v>
       </c>
     </row>
-    <row r="29" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:7">
       <c r="B29" s="14" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="C29" s="14" t="s">
         <v>545</v>
@@ -4024,9 +4030,9 @@
         <v>629</v>
       </c>
     </row>
-    <row r="30" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:7">
       <c r="B30" s="14" t="s">
-        <v>54</v>
+        <v>46</v>
       </c>
       <c r="C30" s="10" t="s">
         <v>77</v>
@@ -4035,9 +4041,9 @@
         <v>355</v>
       </c>
     </row>
-    <row r="31" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:7">
       <c r="B31" s="14" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C31" s="10" t="s">
         <v>67</v>
@@ -4046,9 +4052,9 @@
         <v>356</v>
       </c>
     </row>
-    <row r="32" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:7">
       <c r="B32" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>84</v>
@@ -4057,9 +4063,9 @@
         <v>509</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:5">
       <c r="B33" s="14" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C33" s="10" t="s">
         <v>80</v>
@@ -4068,9 +4074,9 @@
         <v>357</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:5">
       <c r="B34" s="14" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="C34" s="14" t="s">
         <v>546</v>
@@ -4079,9 +4085,9 @@
         <v>466</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:5">
       <c r="B35" s="14" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="C35" s="14" t="s">
         <v>547</v>
@@ -4090,1801 +4096,1804 @@
         <v>634</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:5">
       <c r="B36" s="14" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C36" s="14" t="s">
         <v>548</v>
       </c>
       <c r="E36" s="20"/>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:5">
       <c r="B37" s="14" t="s">
-        <v>68</v>
+        <v>60</v>
       </c>
       <c r="C37" s="10" t="s">
         <v>111</v>
       </c>
       <c r="E37" s="18"/>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:5">
       <c r="B38" s="14" t="s">
-        <v>106</v>
+        <v>68</v>
       </c>
       <c r="C38" s="14" t="s">
         <v>549</v>
       </c>
       <c r="E38" s="19"/>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:5">
       <c r="B39" s="14" t="s">
-        <v>63</v>
+        <v>106</v>
       </c>
       <c r="C39" s="10" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:5">
       <c r="B40" s="14" t="s">
-        <v>76</v>
+        <v>63</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:5">
       <c r="B41" s="14" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="C41" s="14" t="s">
         <v>550</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:5">
       <c r="B42" s="14" t="s">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="C42" s="14" t="s">
         <v>551</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:5">
       <c r="B43" s="14" t="s">
-        <v>66</v>
+        <v>75</v>
       </c>
       <c r="C43" s="14" t="s">
         <v>552</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B44" s="25" t="s">
-        <v>653</v>
+    <row r="44" spans="2:5">
+      <c r="B44" s="14" t="s">
+        <v>66</v>
       </c>
       <c r="C44" s="14" t="s">
         <v>553</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.25">
-      <c r="B45" s="14" t="s">
-        <v>83</v>
+    <row r="45" spans="2:5">
+      <c r="B45" s="25" t="s">
+        <v>653</v>
       </c>
       <c r="C45" s="14" t="s">
         <v>554</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:5">
       <c r="B46" s="14" t="s">
-        <v>79</v>
+        <v>83</v>
       </c>
       <c r="C46" s="14" t="s">
         <v>555</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:5">
       <c r="B47" s="14" t="s">
-        <v>70</v>
+        <v>79</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:5">
       <c r="B48" s="14" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="49" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:3">
       <c r="B49" s="14" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="50" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:3">
       <c r="B50" s="14" t="s">
-        <v>110</v>
+        <v>71</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="51" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:3">
       <c r="B51" s="14" t="s">
-        <v>81</v>
+        <v>110</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="52" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:3">
       <c r="B52" s="14" t="s">
-        <v>72</v>
+        <v>81</v>
       </c>
       <c r="C52" s="10" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="53" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:3">
       <c r="B53" s="14" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C53" s="10" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="54" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:3">
       <c r="B54" s="14" t="s">
-        <v>64</v>
+        <v>73</v>
       </c>
       <c r="C54" s="14" t="s">
         <v>556</v>
       </c>
     </row>
-    <row r="55" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:3">
       <c r="B55" s="14" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
       <c r="C55" s="10" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="56" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:3">
       <c r="B56" s="14" t="s">
-        <v>82</v>
+        <v>74</v>
       </c>
       <c r="C56" s="14" t="s">
         <v>557</v>
       </c>
     </row>
-    <row r="57" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:3">
       <c r="B57" s="14" t="s">
-        <v>101</v>
+        <v>82</v>
       </c>
       <c r="C57" s="10" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="58" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:3">
       <c r="B58" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C58" s="10" t="s">
         <v>468</v>
       </c>
     </row>
-    <row r="59" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:3">
       <c r="B59" s="14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="C59" s="10" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="60" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:3">
       <c r="B60" s="14" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="C60" s="14" t="s">
         <v>558</v>
       </c>
     </row>
-    <row r="61" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:3">
       <c r="B61" s="14" t="s">
-        <v>467</v>
+        <v>104</v>
       </c>
       <c r="C61" s="10" t="s">
         <v>113</v>
       </c>
     </row>
-    <row r="62" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:3">
       <c r="B62" s="14" t="s">
-        <v>90</v>
+        <v>467</v>
       </c>
       <c r="C62" s="10" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="63" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:3">
       <c r="B63" s="14" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>126</v>
       </c>
     </row>
-    <row r="64" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:3">
       <c r="B64" s="14" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>112</v>
       </c>
     </row>
-    <row r="65" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:3">
       <c r="B65" s="14" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>128</v>
       </c>
     </row>
-    <row r="66" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:3">
       <c r="B66" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>119</v>
       </c>
     </row>
-    <row r="67" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:3">
       <c r="B67" s="14" t="s">
-        <v>87</v>
+        <v>103</v>
       </c>
       <c r="C67" s="14" t="s">
         <v>559</v>
       </c>
     </row>
-    <row r="68" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:3">
       <c r="B68" s="14" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
       <c r="C68" s="14" t="s">
         <v>560</v>
       </c>
     </row>
-    <row r="69" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:3">
       <c r="B69" s="14" t="s">
-        <v>89</v>
+        <v>100</v>
       </c>
       <c r="C69" s="14" t="s">
         <v>561</v>
       </c>
     </row>
-    <row r="70" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:3">
       <c r="B70" s="14" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C70" s="14" t="s">
         <v>562</v>
       </c>
     </row>
-    <row r="71" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:3">
       <c r="B71" s="14" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
       <c r="C71" s="14" t="s">
         <v>563</v>
       </c>
     </row>
-    <row r="72" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:3">
       <c r="B72" s="14" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>143</v>
       </c>
     </row>
-    <row r="73" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:3">
       <c r="B73" s="14" t="s">
-        <v>129</v>
+        <v>117</v>
       </c>
       <c r="C73" s="14" t="s">
         <v>564</v>
       </c>
     </row>
-    <row r="74" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:3">
       <c r="B74" s="14" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C74" s="14" t="s">
         <v>565</v>
       </c>
     </row>
-    <row r="75" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:3">
       <c r="B75" s="14" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="C75" s="14" t="s">
         <v>566</v>
       </c>
     </row>
-    <row r="76" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:3">
       <c r="B76" s="14" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>145</v>
       </c>
     </row>
-    <row r="77" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:3">
       <c r="B77" s="14" t="s">
-        <v>114</v>
+        <v>133</v>
       </c>
       <c r="C77" s="14" t="s">
         <v>567</v>
       </c>
     </row>
-    <row r="78" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:3">
       <c r="B78" s="14" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C78" s="14" t="s">
         <v>568</v>
       </c>
     </row>
-    <row r="79" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:3">
       <c r="B79" s="14" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>149</v>
       </c>
     </row>
-    <row r="80" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:3">
       <c r="B80" s="14" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>157</v>
       </c>
     </row>
-    <row r="81" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:3">
       <c r="B81" s="14" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="C81" s="14" t="s">
         <v>569</v>
       </c>
     </row>
-    <row r="82" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:3">
       <c r="B82" s="14" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>161</v>
       </c>
     </row>
-    <row r="83" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:3">
       <c r="B83" s="14" t="s">
-        <v>115</v>
+        <v>124</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>155</v>
       </c>
     </row>
-    <row r="84" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:3">
       <c r="B84" s="14" t="s">
-        <v>127</v>
+        <v>115</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>159</v>
       </c>
     </row>
-    <row r="85" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:3">
       <c r="B85" s="14" t="s">
-        <v>118</v>
+        <v>127</v>
       </c>
       <c r="C85" s="14" t="s">
         <v>570</v>
       </c>
     </row>
-    <row r="86" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:3">
       <c r="B86" s="14" t="s">
-        <v>123</v>
+        <v>118</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>167</v>
       </c>
     </row>
-    <row r="87" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:3">
       <c r="B87" s="14" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="C87" s="10" t="s">
         <v>164</v>
       </c>
     </row>
-    <row r="88" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:3">
       <c r="B88" s="14" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="C88" s="14" t="s">
         <v>171</v>
       </c>
     </row>
-    <row r="89" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:3">
       <c r="B89" s="14" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="C89" s="10" t="s">
         <v>169</v>
       </c>
     </row>
-    <row r="90" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:3">
       <c r="B90" s="14" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>173</v>
       </c>
     </row>
-    <row r="91" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:3">
       <c r="B91" s="14" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C91" s="14" t="s">
         <v>571</v>
       </c>
     </row>
-    <row r="92" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:3">
       <c r="B92" s="14" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="93" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:3">
       <c r="B93" s="14" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>179</v>
       </c>
     </row>
-    <row r="94" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:3">
       <c r="B94" s="14" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>181</v>
       </c>
     </row>
-    <row r="95" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:3">
       <c r="B95" s="14" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="C95" s="14" t="s">
         <v>572</v>
       </c>
     </row>
-    <row r="96" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:3">
       <c r="B96" s="14" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C96" s="14" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:3">
       <c r="B97" s="14" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C97" s="10" t="s">
         <v>186</v>
       </c>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:3">
       <c r="B98" s="14" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C98" s="14" t="s">
         <v>574</v>
       </c>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:3">
       <c r="B99" s="14" t="s">
-        <v>469</v>
+        <v>147</v>
       </c>
       <c r="C99" s="10" t="s">
         <v>190</v>
       </c>
     </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:3">
       <c r="B100" s="14" t="s">
-        <v>150</v>
+        <v>469</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>192</v>
       </c>
     </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:3">
       <c r="B101" s="14" t="s">
-        <v>152</v>
+        <v>150</v>
       </c>
       <c r="C101" s="14" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:3">
       <c r="B102" s="14" t="s">
-        <v>148</v>
+        <v>152</v>
       </c>
       <c r="C102" s="14" t="s">
         <v>576</v>
       </c>
     </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:3">
       <c r="B103" s="14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C103" s="14" t="s">
         <v>577</v>
       </c>
     </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:3">
       <c r="B104" s="14" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>200</v>
       </c>
     </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:3">
       <c r="B105" s="14" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>202</v>
       </c>
     </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:3">
       <c r="B106" s="14" t="s">
-        <v>160</v>
+        <v>153</v>
       </c>
       <c r="C106" s="14" t="s">
         <v>578</v>
       </c>
     </row>
-    <row r="107" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:3">
       <c r="B107" s="14" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="108" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:3">
       <c r="B108" s="14" t="s">
-        <v>154</v>
+        <v>162</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="109" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:3">
       <c r="B109" s="14" t="s">
-        <v>158</v>
+        <v>154</v>
       </c>
       <c r="C109" s="14" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="110" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:3">
       <c r="B110" s="14" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>205</v>
       </c>
     </row>
-    <row r="111" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:3">
       <c r="B111" s="14" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C111" s="14" t="s">
         <v>580</v>
       </c>
     </row>
-    <row r="112" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:3">
       <c r="B112" s="14" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C112" s="14" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="113" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:3">
       <c r="B113" s="14" t="s">
-        <v>170</v>
+        <v>166</v>
       </c>
       <c r="C113" s="10" t="s">
         <v>214</v>
       </c>
     </row>
-    <row r="114" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:3">
       <c r="B114" s="14" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="C114" s="10" t="s">
         <v>218</v>
       </c>
     </row>
-    <row r="115" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:3">
       <c r="B115" s="14" t="s">
-        <v>172</v>
+        <v>168</v>
       </c>
       <c r="C115" s="10" t="s">
         <v>216</v>
       </c>
     </row>
-    <row r="116" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:3">
       <c r="B116" s="14" t="s">
-        <v>176</v>
+        <v>172</v>
       </c>
       <c r="C116" s="10" t="s">
         <v>221</v>
       </c>
     </row>
-    <row r="117" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:3">
       <c r="B117" s="14" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C117" s="10" t="s">
         <v>223</v>
       </c>
     </row>
-    <row r="118" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:3">
       <c r="B118" s="14" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="C118" s="14" t="s">
         <v>582</v>
       </c>
     </row>
-    <row r="119" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:3">
       <c r="B119" s="14" t="s">
-        <v>174</v>
+        <v>178</v>
       </c>
       <c r="C119" s="10" t="s">
         <v>262</v>
       </c>
     </row>
-    <row r="120" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:3">
       <c r="B120" s="14" t="s">
-        <v>180</v>
+        <v>174</v>
       </c>
       <c r="C120" s="10" t="s">
         <v>264</v>
       </c>
     </row>
-    <row r="121" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:3">
       <c r="B121" s="14" t="s">
-        <v>470</v>
+        <v>180</v>
       </c>
       <c r="C121" s="14" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="122" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:3">
       <c r="B122" s="14" t="s">
-        <v>183</v>
+        <v>470</v>
       </c>
       <c r="C122" s="14" t="s">
         <v>584</v>
       </c>
     </row>
-    <row r="123" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:3">
       <c r="B123" s="14" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="C123" s="10" t="s">
         <v>234</v>
       </c>
     </row>
-    <row r="124" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:3">
       <c r="B124" s="14" t="s">
-        <v>184</v>
+        <v>188</v>
       </c>
       <c r="C124" s="14" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="125" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:3">
       <c r="B125" s="14" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="C125" s="10" t="s">
         <v>233</v>
       </c>
     </row>
-    <row r="126" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:3">
       <c r="B126" s="14" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="C126" s="10" t="s">
         <v>242</v>
       </c>
     </row>
-    <row r="127" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:3">
       <c r="B127" s="14" t="s">
-        <v>189</v>
+        <v>182</v>
       </c>
       <c r="C127" s="10" t="s">
         <v>258</v>
       </c>
     </row>
-    <row r="128" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:3">
       <c r="B128" s="14" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C128" s="10" t="s">
         <v>238</v>
       </c>
     </row>
-    <row r="129" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:3">
       <c r="B129" s="14" t="s">
-        <v>187</v>
+        <v>191</v>
       </c>
       <c r="C129" s="10" t="s">
         <v>250</v>
       </c>
     </row>
-    <row r="130" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:3">
       <c r="B130" s="14" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
       <c r="C130" s="10" t="s">
         <v>244</v>
       </c>
     </row>
-    <row r="131" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:3">
       <c r="B131" s="14" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C131" s="14" t="s">
         <v>586</v>
       </c>
     </row>
-    <row r="132" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:3">
       <c r="B132" s="14" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="C132" s="10" t="s">
         <v>251</v>
       </c>
     </row>
-    <row r="133" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:3">
       <c r="B133" s="14" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="C133" s="10" t="s">
         <v>256</v>
       </c>
     </row>
-    <row r="134" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:3">
       <c r="B134" s="14" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C134" s="10" t="s">
         <v>236</v>
       </c>
     </row>
-    <row r="135" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:3">
       <c r="B135" s="14" t="s">
-        <v>198</v>
+        <v>207</v>
       </c>
       <c r="C135" s="10" t="s">
         <v>254</v>
       </c>
     </row>
-    <row r="136" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:3">
       <c r="B136" s="14" t="s">
-        <v>196</v>
+        <v>198</v>
       </c>
       <c r="C136" s="14" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="137" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:3">
       <c r="B137" s="14" t="s">
-        <v>209</v>
+        <v>196</v>
       </c>
       <c r="C137" s="14" t="s">
         <v>588</v>
       </c>
     </row>
-    <row r="138" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:3">
       <c r="B138" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C138" s="14" t="s">
         <v>260</v>
       </c>
     </row>
-    <row r="139" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:3">
       <c r="B139" s="14" t="s">
-        <v>203</v>
+        <v>210</v>
       </c>
       <c r="C139" s="10" t="s">
         <v>265</v>
       </c>
     </row>
-    <row r="140" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:3">
       <c r="B140" s="14" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C140" s="10" t="s">
         <v>228</v>
       </c>
     </row>
-    <row r="141" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:3">
       <c r="B141" s="14" t="s">
-        <v>195</v>
+        <v>204</v>
       </c>
       <c r="C141" s="14" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="142" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:3">
       <c r="B142" s="14" t="s">
-        <v>208</v>
+        <v>195</v>
       </c>
       <c r="C142" s="14" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="143" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:3">
       <c r="B143" s="14" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="C143" s="14" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="144" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:3">
       <c r="B144" s="14" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C144" s="14" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="145" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="145" spans="2:3">
       <c r="B145" s="14" t="s">
-        <v>219</v>
+        <v>212</v>
       </c>
       <c r="C145" s="10" t="s">
         <v>276</v>
       </c>
     </row>
-    <row r="146" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="146" spans="2:3">
       <c r="B146" s="14" t="s">
-        <v>213</v>
+        <v>219</v>
       </c>
       <c r="C146" s="10" t="s">
         <v>282</v>
       </c>
     </row>
-    <row r="147" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="147" spans="2:3">
       <c r="B147" s="14" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C147" s="10" t="s">
         <v>279</v>
       </c>
     </row>
-    <row r="148" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="148" spans="2:3">
       <c r="B148" s="14" t="s">
-        <v>215</v>
+        <v>217</v>
       </c>
       <c r="C148" s="10" t="s">
         <v>281</v>
       </c>
     </row>
-    <row r="149" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="149" spans="2:3">
       <c r="B149" s="14" t="s">
-        <v>220</v>
+        <v>215</v>
       </c>
       <c r="C149" s="14" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="150" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="150" spans="2:3">
       <c r="B150" s="14" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
       <c r="C150" s="14" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="151" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="151" spans="2:3">
       <c r="B151" s="14" t="s">
-        <v>622</v>
+        <v>222</v>
       </c>
       <c r="C151" s="14" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="152" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="152" spans="2:3">
       <c r="B152" s="14" t="s">
-        <v>224</v>
+        <v>622</v>
       </c>
       <c r="C152" s="14" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="153" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="153" spans="2:3">
       <c r="B153" s="14" t="s">
-        <v>239</v>
+        <v>224</v>
       </c>
       <c r="C153" s="14" t="s">
         <v>597</v>
       </c>
     </row>
-    <row r="154" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="154" spans="2:3">
       <c r="B154" s="14" t="s">
-        <v>261</v>
+        <v>239</v>
       </c>
       <c r="C154" s="14" t="s">
         <v>598</v>
       </c>
     </row>
-    <row r="155" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="155" spans="2:3">
       <c r="B155" s="14" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C155" s="10" t="s">
         <v>303</v>
       </c>
     </row>
-    <row r="156" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="156" spans="2:3">
       <c r="B156" s="14" t="s">
-        <v>225</v>
+        <v>263</v>
       </c>
       <c r="C156" s="10" t="s">
         <v>297</v>
       </c>
     </row>
-    <row r="157" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="157" spans="2:3">
       <c r="B157" s="14" t="s">
-        <v>247</v>
+        <v>225</v>
       </c>
       <c r="C157" s="14" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="158" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="158" spans="2:3">
       <c r="B158" s="14" t="s">
-        <v>231</v>
+        <v>247</v>
       </c>
       <c r="C158" s="10" t="s">
         <v>306</v>
       </c>
     </row>
-    <row r="159" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="159" spans="2:3">
       <c r="B159" s="14" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C159" s="14" t="s">
         <v>600</v>
       </c>
     </row>
-    <row r="160" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="160" spans="2:3">
       <c r="B160" s="14" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
       <c r="C160" s="14" t="s">
         <v>601</v>
       </c>
     </row>
-    <row r="161" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="161" spans="2:3">
       <c r="B161" s="14" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="C161" s="14" t="s">
         <v>602</v>
       </c>
     </row>
-    <row r="162" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="162" spans="2:3">
       <c r="B162" s="14" t="s">
-        <v>471</v>
+        <v>246</v>
       </c>
       <c r="C162" s="10" t="s">
         <v>301</v>
       </c>
     </row>
-    <row r="163" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="163" spans="2:3">
       <c r="B163" s="14" t="s">
-        <v>257</v>
+        <v>471</v>
       </c>
       <c r="C163" s="14" t="s">
         <v>310</v>
       </c>
     </row>
-    <row r="164" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="164" spans="2:3">
       <c r="B164" s="14" t="s">
-        <v>237</v>
+        <v>257</v>
       </c>
       <c r="C164" s="14" t="s">
         <v>603</v>
       </c>
     </row>
-    <row r="165" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="165" spans="2:3">
       <c r="B165" s="14" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="C165" s="14" t="s">
         <v>295</v>
       </c>
     </row>
-    <row r="166" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="166" spans="2:3">
       <c r="B166" s="14" t="s">
-        <v>243</v>
+        <v>249</v>
       </c>
       <c r="C166" s="14" t="s">
         <v>604</v>
       </c>
     </row>
-    <row r="167" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="167" spans="2:3">
       <c r="B167" s="14" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
       <c r="C167" s="14" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="168" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="168" spans="2:3">
       <c r="B168" s="14" t="s">
-        <v>255</v>
+        <v>252</v>
       </c>
       <c r="C168" s="14" t="s">
         <v>606</v>
       </c>
     </row>
-    <row r="169" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="169" spans="2:3">
       <c r="B169" s="14" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="C169" s="14" t="s">
         <v>607</v>
       </c>
     </row>
-    <row r="170" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="170" spans="2:3">
       <c r="B170" s="14" t="s">
-        <v>245</v>
+        <v>235</v>
       </c>
       <c r="C170" s="14" t="s">
         <v>608</v>
       </c>
     </row>
-    <row r="171" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="171" spans="2:3">
       <c r="B171" s="14" t="s">
-        <v>253</v>
+        <v>245</v>
       </c>
       <c r="C171" s="14" t="s">
         <v>609</v>
       </c>
     </row>
-    <row r="172" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="172" spans="2:3">
       <c r="B172" s="14" t="s">
-        <v>248</v>
+        <v>253</v>
       </c>
       <c r="C172" s="14" t="s">
         <v>610</v>
       </c>
     </row>
-    <row r="173" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="173" spans="2:3">
       <c r="B173" s="14" t="s">
-        <v>229</v>
+        <v>248</v>
       </c>
       <c r="C173" s="10" t="s">
         <v>321</v>
       </c>
     </row>
-    <row r="174" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="174" spans="2:3">
       <c r="B174" s="14" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C174" s="10" t="s">
         <v>472</v>
       </c>
     </row>
-    <row r="175" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="175" spans="2:3">
       <c r="B175" s="14" t="s">
-        <v>259</v>
+        <v>230</v>
       </c>
       <c r="C175" s="14" t="s">
         <v>611</v>
       </c>
     </row>
-    <row r="176" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="176" spans="2:3">
       <c r="B176" s="14" t="s">
-        <v>227</v>
+        <v>259</v>
       </c>
       <c r="C176" s="14" t="s">
         <v>612</v>
       </c>
     </row>
-    <row r="177" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="177" spans="2:3">
       <c r="B177" s="14" t="s">
-        <v>226</v>
+        <v>227</v>
       </c>
       <c r="C177" s="14" t="s">
         <v>613</v>
       </c>
     </row>
-    <row r="178" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="178" spans="2:3">
       <c r="B178" s="14" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="C178" s="14" t="s">
         <v>614</v>
       </c>
     </row>
-    <row r="179" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="179" spans="2:3">
       <c r="B179" s="14" t="s">
-        <v>270</v>
+        <v>240</v>
       </c>
       <c r="C179" s="14" t="s">
         <v>615</v>
       </c>
     </row>
-    <row r="180" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="180" spans="2:3">
       <c r="B180" s="14" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="C180" s="14" t="s">
         <v>616</v>
       </c>
     </row>
-    <row r="181" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="181" spans="2:3">
       <c r="B181" s="14" t="s">
-        <v>268</v>
+        <v>275</v>
       </c>
       <c r="C181" s="14" t="s">
         <v>617</v>
       </c>
     </row>
-    <row r="182" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="182" spans="2:3">
       <c r="B182" s="14" t="s">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="C182" s="14" t="s">
         <v>618</v>
       </c>
     </row>
-    <row r="183" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="183" spans="2:3">
       <c r="B183" s="14" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="C183" s="14" t="s">
         <v>619</v>
       </c>
     </row>
-    <row r="184" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="184" spans="2:3">
       <c r="B184" s="14" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="C184" s="14" t="s">
         <v>620</v>
       </c>
     </row>
-    <row r="185" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="185" spans="2:3">
       <c r="B185" s="14" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="C185" s="14" t="s">
         <v>621</v>
       </c>
     </row>
-    <row r="186" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="186" spans="2:3">
       <c r="B186" s="14" t="s">
+        <v>277</v>
+      </c>
+      <c r="C186"/>
+    </row>
+    <row r="187" spans="2:3">
+      <c r="B187" s="14" t="s">
         <v>284</v>
       </c>
-      <c r="C186"/>
-    </row>
-    <row r="187" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B187" s="14" t="s">
+      <c r="C187"/>
+    </row>
+    <row r="188" spans="2:3">
+      <c r="B188" s="14" t="s">
         <v>285</v>
       </c>
-      <c r="C187"/>
-    </row>
-    <row r="188" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B188" s="14" t="s">
+      <c r="C188"/>
+    </row>
+    <row r="189" spans="2:3">
+      <c r="B189" s="14" t="s">
         <v>273</v>
       </c>
-      <c r="C188"/>
-    </row>
-    <row r="189" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B189" s="14" t="s">
+      <c r="C189"/>
+    </row>
+    <row r="190" spans="2:3">
+      <c r="B190" s="14" t="s">
         <v>278</v>
       </c>
-      <c r="C189"/>
-    </row>
-    <row r="190" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B190" s="14" t="s">
+      <c r="C190"/>
+    </row>
+    <row r="191" spans="2:3">
+      <c r="B191" s="14" t="s">
         <v>280</v>
       </c>
-      <c r="C190"/>
-    </row>
-    <row r="191" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B191" s="14" t="s">
+      <c r="C191"/>
+    </row>
+    <row r="192" spans="2:3">
+      <c r="B192" s="14" t="s">
         <v>283</v>
       </c>
-      <c r="C191"/>
-    </row>
-    <row r="192" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B192" s="14" t="s">
+      <c r="C192"/>
+    </row>
+    <row r="193" spans="2:3">
+      <c r="B193" s="14" t="s">
         <v>274</v>
       </c>
-      <c r="C192"/>
-    </row>
-    <row r="193" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B193" s="14" t="s">
+      <c r="C193"/>
+    </row>
+    <row r="194" spans="2:3">
+      <c r="B194" s="14" t="s">
         <v>266</v>
       </c>
-      <c r="C193"/>
-    </row>
-    <row r="194" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B194" s="14" t="s">
+      <c r="C194"/>
+    </row>
+    <row r="195" spans="2:3">
+      <c r="B195" s="14" t="s">
         <v>287</v>
       </c>
-      <c r="C194"/>
-    </row>
-    <row r="195" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B195" s="14" t="s">
+      <c r="C195"/>
+    </row>
+    <row r="196" spans="2:3">
+      <c r="B196" s="14" t="s">
         <v>286</v>
       </c>
-      <c r="C195"/>
-    </row>
-    <row r="196" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B196" s="14" t="s">
+      <c r="C196"/>
+    </row>
+    <row r="197" spans="2:3">
+      <c r="B197" s="14" t="s">
         <v>44</v>
       </c>
-      <c r="C196"/>
-    </row>
-    <row r="197" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B197" s="14" t="s">
+      <c r="C197"/>
+    </row>
+    <row r="198" spans="2:3">
+      <c r="B198" s="14" t="s">
         <v>289</v>
       </c>
-      <c r="C197"/>
-    </row>
-    <row r="198" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B198" s="14" t="s">
+      <c r="C198"/>
+    </row>
+    <row r="199" spans="2:3">
+      <c r="B199" s="14" t="s">
         <v>288</v>
       </c>
-      <c r="C198"/>
-    </row>
-    <row r="199" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B199" s="14" t="s">
+      <c r="C199"/>
+    </row>
+    <row r="200" spans="2:3">
+      <c r="B200" s="14" t="s">
         <v>302</v>
       </c>
-      <c r="C199"/>
-    </row>
-    <row r="200" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B200" s="14" t="s">
+      <c r="C200"/>
+    </row>
+    <row r="201" spans="2:3">
+      <c r="B201" s="14" t="s">
         <v>291</v>
       </c>
-      <c r="C200"/>
-    </row>
-    <row r="201" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B201" s="14" t="s">
+      <c r="C201"/>
+    </row>
+    <row r="202" spans="2:3">
+      <c r="B202" s="14" t="s">
         <v>296</v>
       </c>
-      <c r="C201"/>
-    </row>
-    <row r="202" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B202" s="14" t="s">
+      <c r="C202"/>
+    </row>
+    <row r="203" spans="2:3">
+      <c r="B203" s="14" t="s">
         <v>305</v>
       </c>
-      <c r="C202"/>
-    </row>
-    <row r="203" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B203" s="14" t="s">
+      <c r="C203"/>
+    </row>
+    <row r="204" spans="2:3">
+      <c r="B204" s="14" t="s">
         <v>293</v>
       </c>
-      <c r="C203"/>
-    </row>
-    <row r="204" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B204" s="14" t="s">
+      <c r="C204"/>
+    </row>
+    <row r="205" spans="2:3">
+      <c r="B205" s="14" t="s">
         <v>298</v>
       </c>
-      <c r="C204"/>
-    </row>
-    <row r="205" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B205" s="14" t="s">
+      <c r="C205"/>
+    </row>
+    <row r="206" spans="2:3">
+      <c r="B206" s="14" t="s">
         <v>290</v>
       </c>
-      <c r="C205"/>
-    </row>
-    <row r="206" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B206" s="14" t="s">
+      <c r="C206"/>
+    </row>
+    <row r="207" spans="2:3">
+      <c r="B207" s="14" t="s">
         <v>299</v>
       </c>
-      <c r="C206"/>
-    </row>
-    <row r="207" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B207" s="14" t="s">
+      <c r="C207"/>
+    </row>
+    <row r="208" spans="2:3">
+      <c r="B208" s="14" t="s">
         <v>300</v>
       </c>
-      <c r="C207"/>
-    </row>
-    <row r="208" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B208" s="14" t="s">
+      <c r="C208"/>
+    </row>
+    <row r="209" spans="2:3">
+      <c r="B209" s="14" t="s">
         <v>292</v>
       </c>
-      <c r="C208"/>
-    </row>
-    <row r="209" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B209" s="14" t="s">
+      <c r="C209"/>
+    </row>
+    <row r="210" spans="2:3">
+      <c r="B210" s="14" t="s">
         <v>308</v>
       </c>
-      <c r="C209"/>
-    </row>
-    <row r="210" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B210" s="14" t="s">
+      <c r="C210"/>
+    </row>
+    <row r="211" spans="2:3">
+      <c r="B211" s="14" t="s">
         <v>309</v>
       </c>
-      <c r="C210"/>
-    </row>
-    <row r="211" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B211" s="14" t="s">
+      <c r="C211"/>
+    </row>
+    <row r="212" spans="2:3">
+      <c r="B212" s="14" t="s">
         <v>311</v>
       </c>
-      <c r="C211"/>
-    </row>
-    <row r="212" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B212" s="14" t="s">
+      <c r="C212"/>
+    </row>
+    <row r="213" spans="2:3">
+      <c r="B213" s="14" t="s">
         <v>307</v>
       </c>
-      <c r="C212"/>
-    </row>
-    <row r="213" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B213" s="14" t="s">
+      <c r="C213"/>
+    </row>
+    <row r="214" spans="2:3">
+      <c r="B214" s="14" t="s">
         <v>294</v>
       </c>
-      <c r="C213"/>
-    </row>
-    <row r="214" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B214" s="14" t="s">
+      <c r="C214"/>
+    </row>
+    <row r="215" spans="2:3">
+      <c r="B215" s="14" t="s">
         <v>304</v>
       </c>
-      <c r="C214"/>
-    </row>
-    <row r="215" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B215" s="14" t="s">
+      <c r="C215"/>
+    </row>
+    <row r="216" spans="2:3">
+      <c r="B216" s="14" t="s">
         <v>313</v>
       </c>
-      <c r="C215"/>
-    </row>
-    <row r="216" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B216" s="14" t="s">
+      <c r="C216"/>
+    </row>
+    <row r="217" spans="2:3">
+      <c r="B217" s="14" t="s">
         <v>312</v>
       </c>
-      <c r="C216"/>
-    </row>
-    <row r="217" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B217" s="14" t="s">
+      <c r="C217"/>
+    </row>
+    <row r="218" spans="2:3">
+      <c r="B218" s="14" t="s">
         <v>315</v>
       </c>
-      <c r="C217"/>
-    </row>
-    <row r="218" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B218" s="14" t="s">
+      <c r="C218"/>
+    </row>
+    <row r="219" spans="2:3">
+      <c r="B219" s="14" t="s">
         <v>316</v>
       </c>
-      <c r="C218"/>
-    </row>
-    <row r="219" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B219" s="14" t="s">
+      <c r="C219"/>
+    </row>
+    <row r="220" spans="2:3">
+      <c r="B220" s="14" t="s">
         <v>314</v>
       </c>
-      <c r="C219"/>
-    </row>
-    <row r="220" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B220" s="14" t="s">
+      <c r="C220"/>
+    </row>
+    <row r="221" spans="2:3">
+      <c r="B221" s="14" t="s">
         <v>317</v>
       </c>
-      <c r="C220"/>
-    </row>
-    <row r="221" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B221" s="14" t="s">
+      <c r="C221"/>
+    </row>
+    <row r="222" spans="2:3">
+      <c r="B222" s="14" t="s">
         <v>318</v>
       </c>
-      <c r="C221"/>
-    </row>
-    <row r="222" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B222" s="14" t="s">
+      <c r="C222"/>
+    </row>
+    <row r="223" spans="2:3">
+      <c r="B223" s="14" t="s">
         <v>319</v>
       </c>
-      <c r="C222"/>
-    </row>
-    <row r="223" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B223" s="14" t="s">
+      <c r="C223"/>
+    </row>
+    <row r="224" spans="2:3">
+      <c r="B224" s="14" t="s">
         <v>320</v>
       </c>
-      <c r="C223"/>
-    </row>
-    <row r="224" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B224" s="14" t="s">
+      <c r="C224"/>
+    </row>
+    <row r="225" spans="2:3">
+      <c r="B225" s="14" t="s">
         <v>323</v>
       </c>
-      <c r="C224"/>
-    </row>
-    <row r="225" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B225" s="14" t="s">
+      <c r="C225"/>
+    </row>
+    <row r="226" spans="2:3">
+      <c r="B226" s="14" t="s">
         <v>322</v>
       </c>
-      <c r="C225"/>
-    </row>
-    <row r="226" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B226" s="14" t="s">
+      <c r="C226"/>
+    </row>
+    <row r="227" spans="2:3">
+      <c r="B227" s="14" t="s">
         <v>331</v>
       </c>
-      <c r="C226"/>
-    </row>
-    <row r="227" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B227" s="14" t="s">
+      <c r="C227"/>
+    </row>
+    <row r="228" spans="2:3">
+      <c r="B228" s="14" t="s">
         <v>329</v>
       </c>
-      <c r="C227"/>
-    </row>
-    <row r="228" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B228" s="14" t="s">
+      <c r="C228"/>
+    </row>
+    <row r="229" spans="2:3">
+      <c r="B229" s="14" t="s">
         <v>328</v>
       </c>
-      <c r="C228"/>
-    </row>
-    <row r="229" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B229" s="14" t="s">
+      <c r="C229"/>
+    </row>
+    <row r="230" spans="2:3">
+      <c r="B230" s="14" t="s">
         <v>326</v>
       </c>
-      <c r="C229"/>
-    </row>
-    <row r="230" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B230" s="14" t="s">
+      <c r="C230"/>
+    </row>
+    <row r="231" spans="2:3">
+      <c r="B231" s="14" t="s">
         <v>324</v>
       </c>
-      <c r="C230"/>
-    </row>
-    <row r="231" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B231" s="14" t="s">
+      <c r="C231"/>
+    </row>
+    <row r="232" spans="2:3">
+      <c r="B232" s="14" t="s">
         <v>325</v>
       </c>
-      <c r="C231"/>
-    </row>
-    <row r="232" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B232" s="14" t="s">
+      <c r="C232"/>
+    </row>
+    <row r="233" spans="2:3">
+      <c r="B233" s="14" t="s">
         <v>327</v>
       </c>
-      <c r="C232"/>
-    </row>
-    <row r="233" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B233" s="14" t="s">
+      <c r="C233"/>
+    </row>
+    <row r="234" spans="2:3">
+      <c r="B234" s="14" t="s">
         <v>330</v>
       </c>
-      <c r="C233"/>
-    </row>
-    <row r="234" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B234" s="14" t="s">
+      <c r="C234"/>
+    </row>
+    <row r="235" spans="2:3">
+      <c r="B235" s="14" t="s">
         <v>332</v>
       </c>
-      <c r="C234"/>
-    </row>
-    <row r="235" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B235" s="14" t="s">
+      <c r="C235"/>
+    </row>
+    <row r="236" spans="2:3">
+      <c r="B236" s="14" t="s">
         <v>333</v>
       </c>
-      <c r="C235"/>
-    </row>
-    <row r="236" spans="2:3" x14ac:dyDescent="0.25">
       <c r="C236"/>
     </row>
-    <row r="237" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="237" spans="2:3">
       <c r="C237"/>
     </row>
-    <row r="238" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="238" spans="2:3">
       <c r="C238"/>
     </row>
-    <row r="239" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="239" spans="2:3">
       <c r="C239"/>
     </row>
-    <row r="240" spans="2:3" x14ac:dyDescent="0.25">
+    <row r="240" spans="2:3">
       <c r="C240"/>
     </row>
-    <row r="241" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="241" spans="3:3">
       <c r="C241"/>
     </row>
-    <row r="242" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="242" spans="3:3">
       <c r="C242"/>
     </row>
-    <row r="243" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="243" spans="3:3">
       <c r="C243"/>
     </row>
-    <row r="244" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="244" spans="3:3">
       <c r="C244"/>
     </row>
-    <row r="245" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="245" spans="3:3">
       <c r="C245"/>
     </row>
-    <row r="246" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="246" spans="3:3">
       <c r="C246"/>
     </row>
-    <row r="247" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="247" spans="3:3">
       <c r="C247"/>
     </row>
-    <row r="248" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="248" spans="3:3">
       <c r="C248"/>
     </row>
-    <row r="249" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="249" spans="3:3">
       <c r="C249"/>
     </row>
-    <row r="250" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="250" spans="3:3">
       <c r="C250"/>
     </row>
-    <row r="251" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="251" spans="3:3">
       <c r="C251"/>
     </row>
-    <row r="252" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="252" spans="3:3">
       <c r="C252"/>
     </row>
-    <row r="253" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="253" spans="3:3">
       <c r="C253"/>
     </row>
-    <row r="254" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="254" spans="3:3">
       <c r="C254"/>
     </row>
-    <row r="255" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="255" spans="3:3">
       <c r="C255"/>
     </row>
-    <row r="256" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="256" spans="3:3">
       <c r="C256"/>
     </row>
-    <row r="257" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="257" spans="3:3">
       <c r="C257"/>
     </row>
-    <row r="258" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="258" spans="3:3">
       <c r="C258"/>
     </row>
-    <row r="259" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="259" spans="3:3">
       <c r="C259"/>
     </row>
-    <row r="260" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="260" spans="3:3">
       <c r="C260"/>
     </row>
-    <row r="261" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="261" spans="3:3">
       <c r="C261"/>
     </row>
-    <row r="262" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="262" spans="3:3">
       <c r="C262"/>
     </row>
-    <row r="263" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="263" spans="3:3">
       <c r="C263"/>
     </row>
-    <row r="264" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="264" spans="3:3">
       <c r="C264"/>
     </row>
-    <row r="265" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="265" spans="3:3">
       <c r="C265"/>
     </row>
-    <row r="266" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="266" spans="3:3">
       <c r="C266"/>
     </row>
-    <row r="267" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="267" spans="3:3">
       <c r="C267"/>
     </row>
-    <row r="268" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="268" spans="3:3">
       <c r="C268"/>
     </row>
-    <row r="269" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="269" spans="3:3">
       <c r="C269"/>
     </row>
-    <row r="270" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="270" spans="3:3">
       <c r="C270"/>
     </row>
-    <row r="271" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="271" spans="3:3">
       <c r="C271"/>
     </row>
-    <row r="272" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="272" spans="3:3">
       <c r="C272"/>
     </row>
-    <row r="273" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="273" spans="3:3">
       <c r="C273"/>
     </row>
-    <row r="274" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="274" spans="3:3">
       <c r="C274"/>
     </row>
-    <row r="275" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="275" spans="3:3">
       <c r="C275"/>
     </row>
-    <row r="276" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="276" spans="3:3">
       <c r="C276"/>
     </row>
-    <row r="277" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="277" spans="3:3">
       <c r="C277"/>
     </row>
-    <row r="278" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="278" spans="3:3">
       <c r="C278"/>
     </row>
-    <row r="279" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="279" spans="3:3">
       <c r="C279"/>
     </row>
-    <row r="280" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="280" spans="3:3">
       <c r="C280"/>
     </row>
-    <row r="281" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="281" spans="3:3">
       <c r="C281"/>
     </row>
-    <row r="282" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="282" spans="3:3">
       <c r="C282"/>
     </row>
-    <row r="283" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="283" spans="3:3">
       <c r="C283"/>
     </row>
-    <row r="284" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="284" spans="3:3">
       <c r="C284"/>
     </row>
-    <row r="285" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="285" spans="3:3">
       <c r="C285"/>
     </row>
-    <row r="286" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="286" spans="3:3">
       <c r="C286"/>
     </row>
-    <row r="287" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="287" spans="3:3">
       <c r="C287"/>
     </row>
-    <row r="288" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="288" spans="3:3">
       <c r="C288"/>
     </row>
-    <row r="289" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="289" spans="3:3">
       <c r="C289"/>
     </row>
-    <row r="290" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="290" spans="3:3">
       <c r="C290"/>
     </row>
-    <row r="291" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="291" spans="3:3">
       <c r="C291"/>
     </row>
-    <row r="292" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="292" spans="3:3">
       <c r="C292"/>
     </row>
-    <row r="293" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="293" spans="3:3">
       <c r="C293"/>
     </row>
-    <row r="294" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="294" spans="3:3">
       <c r="C294"/>
     </row>
-    <row r="295" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="295" spans="3:3">
       <c r="C295"/>
     </row>
-    <row r="296" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="296" spans="3:3">
       <c r="C296"/>
     </row>
-    <row r="297" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="297" spans="3:3">
       <c r="C297"/>
     </row>
-    <row r="298" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="298" spans="3:3">
       <c r="C298"/>
     </row>
-    <row r="299" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="299" spans="3:3">
       <c r="C299"/>
     </row>
-    <row r="300" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="300" spans="3:3">
       <c r="C300"/>
     </row>
-    <row r="301" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="301" spans="3:3">
       <c r="C301"/>
     </row>
-    <row r="302" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="302" spans="3:3">
       <c r="C302"/>
     </row>
-    <row r="303" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="303" spans="3:3">
       <c r="C303"/>
     </row>
-    <row r="304" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="304" spans="3:3">
       <c r="C304"/>
     </row>
-    <row r="305" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="305" spans="3:3">
       <c r="C305"/>
     </row>
-    <row r="306" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="306" spans="3:3">
       <c r="C306"/>
     </row>
-    <row r="307" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="307" spans="3:3">
       <c r="C307"/>
     </row>
-    <row r="308" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="308" spans="3:3">
       <c r="C308"/>
     </row>
-    <row r="309" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="309" spans="3:3">
       <c r="C309"/>
     </row>
-    <row r="310" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="310" spans="3:3">
       <c r="C310"/>
     </row>
-    <row r="311" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="311" spans="3:3">
       <c r="C311"/>
     </row>
-    <row r="312" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="312" spans="3:3">
       <c r="C312"/>
     </row>
-    <row r="313" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="313" spans="3:3">
       <c r="C313"/>
     </row>
-    <row r="314" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="314" spans="3:3">
       <c r="C314"/>
     </row>
-    <row r="315" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="315" spans="3:3">
       <c r="C315"/>
     </row>
-    <row r="316" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="316" spans="3:3">
       <c r="C316"/>
     </row>
-    <row r="317" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="317" spans="3:3">
       <c r="C317"/>
     </row>
-    <row r="318" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="318" spans="3:3">
       <c r="C318"/>
     </row>
-    <row r="319" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="319" spans="3:3">
       <c r="C319"/>
     </row>
-    <row r="320" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="320" spans="3:3">
       <c r="C320"/>
     </row>
-    <row r="321" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="321" spans="3:3">
       <c r="C321"/>
     </row>
-    <row r="322" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="322" spans="3:3">
       <c r="C322"/>
     </row>
-    <row r="323" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="323" spans="3:3">
       <c r="C323"/>
     </row>
-    <row r="324" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="324" spans="3:3">
       <c r="C324"/>
     </row>
-    <row r="325" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="325" spans="3:3">
       <c r="C325"/>
     </row>
-    <row r="326" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="326" spans="3:3">
       <c r="C326"/>
     </row>
-    <row r="327" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="327" spans="3:3">
       <c r="C327"/>
     </row>
-    <row r="328" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="328" spans="3:3">
       <c r="C328"/>
     </row>
-    <row r="329" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="329" spans="3:3">
       <c r="C329"/>
     </row>
-    <row r="330" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="330" spans="3:3">
       <c r="C330"/>
     </row>
-    <row r="331" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="331" spans="3:3">
       <c r="C331"/>
     </row>
-    <row r="332" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="332" spans="3:3">
       <c r="C332"/>
     </row>
-    <row r="333" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="333" spans="3:3">
       <c r="C333"/>
     </row>
   </sheetData>
@@ -5892,7 +5901,12 @@
     <sortCondition ref="G2"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5904,20 +5918,20 @@
       <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="36.42578125" style="7" customWidth="1"/>
+    <col min="1" max="1" width="36.5" style="7" customWidth="1"/>
     <col min="2" max="2" width="24" style="7" customWidth="1"/>
-    <col min="3" max="3" width="30.85546875" style="7" customWidth="1"/>
-    <col min="4" max="4" width="29.28515625" style="7" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="7" customWidth="1"/>
-    <col min="6" max="6" width="42.85546875" customWidth="1"/>
-    <col min="7" max="7" width="19.28515625" style="7" customWidth="1"/>
-    <col min="8" max="8" width="41.140625" style="7" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="7"/>
+    <col min="3" max="3" width="30.83203125" style="7" customWidth="1"/>
+    <col min="4" max="4" width="29.33203125" style="7" customWidth="1"/>
+    <col min="5" max="5" width="25.5" style="7" customWidth="1"/>
+    <col min="6" max="6" width="42.83203125" customWidth="1"/>
+    <col min="7" max="7" width="19.33203125" style="7" customWidth="1"/>
+    <col min="8" max="8" width="41.1640625" style="7" customWidth="1"/>
+    <col min="9" max="16384" width="8.83203125" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" s="4" t="s">
         <v>486</v>
       </c>
@@ -5943,7 +5957,7 @@
         <v>638</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2" s="7" t="s">
         <v>485</v>
       </c>
@@ -5969,7 +5983,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
         <v>526</v>
       </c>
@@ -5995,7 +6009,7 @@
         <v>644</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
         <v>527</v>
       </c>
@@ -6021,7 +6035,7 @@
         <v>647</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8">
       <c r="B5" s="8" t="s">
         <v>367</v>
       </c>
@@ -6042,7 +6056,7 @@
         <v>649</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8">
       <c r="B6" s="8" t="s">
         <v>370</v>
       </c>
@@ -6060,7 +6074,7 @@
         <v>651</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8">
       <c r="B7" s="8" t="s">
         <v>373</v>
       </c>
@@ -6075,7 +6089,7 @@
         <v>652</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8">
       <c r="B8" s="8" t="s">
         <v>375</v>
       </c>
@@ -6086,7 +6100,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8">
       <c r="B9" s="8" t="s">
         <v>378</v>
       </c>
@@ -6097,7 +6111,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8">
       <c r="B10" s="8" t="s">
         <v>381</v>
       </c>
@@ -6108,7 +6122,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8">
       <c r="B11" s="8" t="s">
         <v>384</v>
       </c>
@@ -6119,7 +6133,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:8">
       <c r="B12" s="8" t="s">
         <v>387</v>
       </c>
@@ -6130,7 +6144,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8">
       <c r="B13" s="8" t="s">
         <v>390</v>
       </c>
@@ -6141,7 +6155,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:8">
       <c r="B14" s="8" t="s">
         <v>392</v>
       </c>
@@ -6152,7 +6166,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:8">
       <c r="B15" s="8" t="s">
         <v>393</v>
       </c>
@@ -6163,7 +6177,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:8">
       <c r="B16" s="8" t="s">
         <v>395</v>
       </c>
@@ -6171,7 +6185,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4">
       <c r="B17" s="8" t="s">
         <v>397</v>
       </c>
@@ -6179,7 +6193,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4">
       <c r="B18" s="8" t="s">
         <v>399</v>
       </c>
@@ -6187,7 +6201,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4">
       <c r="B19" s="8" t="s">
         <v>401</v>
       </c>
@@ -6195,7 +6209,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="20" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:4">
       <c r="B20" s="8" t="s">
         <v>403</v>
       </c>
@@ -6203,7 +6217,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="21" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:4">
       <c r="B21" s="8" t="s">
         <v>405</v>
       </c>
@@ -6211,212 +6225,217 @@
         <v>404</v>
       </c>
     </row>
-    <row r="22" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:4">
       <c r="D22" s="7" t="s">
         <v>406</v>
       </c>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4">
       <c r="D23" s="7" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4">
       <c r="D24" s="7" t="s">
         <v>408</v>
       </c>
     </row>
-    <row r="25" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:4">
       <c r="D25" s="7" t="s">
         <v>409</v>
       </c>
     </row>
-    <row r="26" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:4">
       <c r="D26" s="7" t="s">
         <v>410</v>
       </c>
     </row>
-    <row r="27" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:4">
       <c r="D27" s="7" t="s">
         <v>411</v>
       </c>
     </row>
-    <row r="28" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:4">
       <c r="D28" s="7" t="s">
         <v>412</v>
       </c>
     </row>
-    <row r="29" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:4">
       <c r="D29" s="7" t="s">
         <v>413</v>
       </c>
     </row>
-    <row r="30" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:4">
       <c r="D30" s="7" t="s">
         <v>414</v>
       </c>
     </row>
-    <row r="31" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:4">
       <c r="D31" s="7" t="s">
         <v>415</v>
       </c>
     </row>
-    <row r="32" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:4">
       <c r="D32" s="7" t="s">
         <v>416</v>
       </c>
     </row>
-    <row r="33" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="33" spans="4:4">
       <c r="D33" s="7" t="s">
         <v>417</v>
       </c>
     </row>
-    <row r="34" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="34" spans="4:4">
       <c r="D34" s="7" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="35" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="35" spans="4:4">
       <c r="D35" s="7" t="s">
         <v>419</v>
       </c>
     </row>
-    <row r="36" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="36" spans="4:4">
       <c r="D36" s="7" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="37" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="37" spans="4:4">
       <c r="D37" s="7" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="38" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="38" spans="4:4">
       <c r="D38" s="7" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="39" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="39" spans="4:4">
       <c r="D39" s="7" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="40" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="40" spans="4:4">
       <c r="D40" s="7" t="s">
         <v>424</v>
       </c>
     </row>
-    <row r="41" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="41" spans="4:4">
       <c r="D41" s="7" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="42" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="42" spans="4:4">
       <c r="D42" s="7" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="43" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="43" spans="4:4">
       <c r="D43" s="7" t="s">
         <v>427</v>
       </c>
     </row>
-    <row r="44" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="44" spans="4:4">
       <c r="D44" s="7" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="45" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="45" spans="4:4">
       <c r="D45" s="7" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="46" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="4:4">
       <c r="D46" s="7" t="s">
         <v>430</v>
       </c>
     </row>
-    <row r="47" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="47" spans="4:4">
       <c r="D47" s="7" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="48" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="48" spans="4:4">
       <c r="D48" s="7" t="s">
         <v>432</v>
       </c>
     </row>
-    <row r="49" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="49" spans="4:4">
       <c r="D49" s="7" t="s">
         <v>433</v>
       </c>
     </row>
-    <row r="50" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="4:4">
       <c r="D50" s="7" t="s">
         <v>434</v>
       </c>
     </row>
-    <row r="51" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="51" spans="4:4">
       <c r="D51" s="7" t="s">
         <v>435</v>
       </c>
     </row>
-    <row r="52" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="52" spans="4:4">
       <c r="D52" s="7" t="s">
         <v>436</v>
       </c>
     </row>
-    <row r="53" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="53" spans="4:4">
       <c r="D53" s="7" t="s">
         <v>437</v>
       </c>
     </row>
-    <row r="54" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="54" spans="4:4">
       <c r="D54" s="7" t="s">
         <v>438</v>
       </c>
     </row>
-    <row r="55" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="55" spans="4:4">
       <c r="D55" s="7" t="s">
         <v>439</v>
       </c>
     </row>
-    <row r="56" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="56" spans="4:4">
       <c r="D56" s="7" t="s">
         <v>440</v>
       </c>
     </row>
-    <row r="57" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="57" spans="4:4">
       <c r="D57" s="7" t="s">
         <v>441</v>
       </c>
     </row>
-    <row r="58" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="58" spans="4:4">
       <c r="D58" s="7" t="s">
         <v>442</v>
       </c>
     </row>
-    <row r="59" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="59" spans="4:4">
       <c r="D59" s="7" t="s">
         <v>443</v>
       </c>
     </row>
-    <row r="60" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="60" spans="4:4">
       <c r="D60" s="7" t="s">
         <v>361</v>
       </c>
     </row>
-    <row r="61" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="61" spans="4:4">
       <c r="D61" s="9"/>
     </row>
-    <row r="62" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="62" spans="4:4">
       <c r="D62" s="9"/>
     </row>
-    <row r="63" spans="4:4" x14ac:dyDescent="0.25">
+    <row r="63" spans="4:4">
       <c r="D63" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes #307 - Update the Standard InputStream template to remove slash from component and sub-component.
</commit_message>
<xml_diff>
--- a/WebContent/files/xls_standard_input_template.xlsx
+++ b/WebContent/files/xls_standard_input_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="25203"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25760" windowHeight="11640" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25760" windowHeight="11640" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Item description" sheetId="9" r:id="rId1"/>
@@ -1741,12 +1741,6 @@
     <t>--Select a Related resource:[type]--</t>
   </si>
   <si>
-    <t xml:space="preserve">  \Component</t>
-  </si>
-  <si>
-    <t xml:space="preserve">    \Sub-component</t>
-  </si>
-  <si>
     <t>Corporate:Abridger</t>
   </si>
   <si>
@@ -2129,6 +2123,12 @@
   </si>
   <si>
     <t>Person:Advisor</t>
+  </si>
+  <si>
+    <t>Component</t>
+  </si>
+  <si>
+    <t>Sub-component</t>
   </si>
 </sst>
 </file>
@@ -3286,7 +3286,7 @@
         <v>502</v>
       </c>
       <c r="G1" s="17" t="s">
-        <v>624</v>
+        <v>622</v>
       </c>
       <c r="H1" s="15" t="s">
         <v>9</v>
@@ -3313,7 +3313,7 @@
         <v>7</v>
       </c>
       <c r="P1" s="17" t="s">
-        <v>623</v>
+        <v>621</v>
       </c>
       <c r="Q1" s="16" t="s">
         <v>521</v>
@@ -3331,16 +3331,16 @@
         <v>525</v>
       </c>
       <c r="V1" s="24" t="s">
+        <v>633</v>
+      </c>
+      <c r="W1" s="24" t="s">
+        <v>634</v>
+      </c>
+      <c r="X1" s="24" t="s">
         <v>635</v>
       </c>
-      <c r="W1" s="24" t="s">
+      <c r="Y1" s="24" t="s">
         <v>636</v>
-      </c>
-      <c r="X1" s="24" t="s">
-        <v>637</v>
-      </c>
-      <c r="Y1" s="24" t="s">
-        <v>638</v>
       </c>
     </row>
   </sheetData>
@@ -3480,8 +3480,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R333"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="38.5" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -3531,7 +3531,7 @@
         <v>19</v>
       </c>
       <c r="C2" s="14" t="s">
-        <v>528</v>
+        <v>526</v>
       </c>
       <c r="D2" s="10" t="s">
         <v>489</v>
@@ -3560,7 +3560,7 @@
         <v>21</v>
       </c>
       <c r="C3" s="14" t="s">
-        <v>529</v>
+        <v>527</v>
       </c>
       <c r="D3" s="12" t="s">
         <v>488</v>
@@ -3589,7 +3589,7 @@
         <v>23</v>
       </c>
       <c r="C4" s="14" t="s">
-        <v>530</v>
+        <v>528</v>
       </c>
       <c r="D4" s="12" t="s">
         <v>487</v>
@@ -3618,7 +3618,7 @@
         <v>269</v>
       </c>
       <c r="C5" s="14" t="s">
-        <v>531</v>
+        <v>529</v>
       </c>
       <c r="D5" s="12" t="s">
         <v>450</v>
@@ -3644,10 +3644,10 @@
         <v>453</v>
       </c>
       <c r="B6" s="14" t="s">
-        <v>655</v>
+        <v>653</v>
       </c>
       <c r="C6" s="14" t="s">
-        <v>532</v>
+        <v>530</v>
       </c>
       <c r="D6" s="13" t="s">
         <v>490</v>
@@ -3659,7 +3659,7 @@
         <v>12</v>
       </c>
       <c r="G6" s="18" t="s">
-        <v>628</v>
+        <v>626</v>
       </c>
       <c r="H6" s="12" t="s">
         <v>456</v>
@@ -3676,7 +3676,7 @@
         <v>25</v>
       </c>
       <c r="C7" s="14" t="s">
-        <v>533</v>
+        <v>531</v>
       </c>
       <c r="E7" s="11" t="s">
         <v>348</v>
@@ -3685,7 +3685,7 @@
         <v>454</v>
       </c>
       <c r="G7" s="21" t="s">
-        <v>625</v>
+        <v>623</v>
       </c>
       <c r="H7" s="12" t="s">
         <v>458</v>
@@ -3699,7 +3699,7 @@
         <v>26</v>
       </c>
       <c r="C8" s="14" t="s">
-        <v>534</v>
+        <v>532</v>
       </c>
       <c r="E8" s="27" t="s">
         <v>4</v>
@@ -3720,10 +3720,10 @@
         <v>27</v>
       </c>
       <c r="C9" s="14" t="s">
-        <v>535</v>
+        <v>533</v>
       </c>
       <c r="E9" s="28" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="F9" s="11" t="s">
         <v>503</v>
@@ -3741,7 +3741,7 @@
         <v>30</v>
       </c>
       <c r="C10" s="14" t="s">
-        <v>536</v>
+        <v>534</v>
       </c>
       <c r="E10" s="27" t="s">
         <v>350</v>
@@ -3762,16 +3762,16 @@
         <v>32</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>537</v>
+        <v>535</v>
       </c>
       <c r="E11" s="28" t="s">
+        <v>629</v>
+      </c>
+      <c r="F11" s="11" t="s">
         <v>631</v>
       </c>
-      <c r="F11" s="11" t="s">
-        <v>633</v>
-      </c>
       <c r="G11" s="21" t="s">
-        <v>626</v>
+        <v>624</v>
       </c>
       <c r="H11" s="11"/>
       <c r="I11" s="11" t="s">
@@ -3804,7 +3804,7 @@
         <v>20</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>538</v>
+        <v>536</v>
       </c>
       <c r="E13" s="27" t="s">
         <v>339</v>
@@ -3823,7 +3823,7 @@
         <v>22</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>539</v>
+        <v>537</v>
       </c>
       <c r="E14" s="27" t="s">
         <v>462</v>
@@ -3840,7 +3840,7 @@
         <v>35</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>540</v>
+        <v>538</v>
       </c>
       <c r="E15" s="27" t="s">
         <v>505</v>
@@ -3849,7 +3849,7 @@
         <v>5</v>
       </c>
       <c r="G15" s="21" t="s">
-        <v>627</v>
+        <v>625</v>
       </c>
     </row>
     <row r="16" spans="1:9">
@@ -3857,7 +3857,7 @@
         <v>33</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>541</v>
+        <v>539</v>
       </c>
       <c r="E16" s="27" t="s">
         <v>506</v>
@@ -3874,7 +3874,7 @@
         <v>36</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>542</v>
+        <v>540</v>
       </c>
       <c r="E17" s="27" t="s">
         <v>507</v>
@@ -3888,7 +3888,7 @@
     </row>
     <row r="18" spans="2:7">
       <c r="B18" s="26" t="s">
-        <v>654</v>
+        <v>652</v>
       </c>
       <c r="C18" s="10" t="s">
         <v>29</v>
@@ -3933,7 +3933,7 @@
         <v>41</v>
       </c>
       <c r="C21" s="14" t="s">
-        <v>543</v>
+        <v>541</v>
       </c>
       <c r="E21" s="29" t="s">
         <v>484</v>
@@ -3994,7 +3994,7 @@
         <v>62</v>
       </c>
       <c r="E26" s="28" t="s">
-        <v>632</v>
+        <v>630</v>
       </c>
     </row>
     <row r="27" spans="2:7">
@@ -4013,7 +4013,7 @@
         <v>28</v>
       </c>
       <c r="C28" s="14" t="s">
-        <v>544</v>
+        <v>542</v>
       </c>
       <c r="E28" s="27" t="s">
         <v>465</v>
@@ -4024,10 +4024,10 @@
         <v>55</v>
       </c>
       <c r="C29" s="14" t="s">
-        <v>545</v>
+        <v>543</v>
       </c>
       <c r="E29" s="28" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
     </row>
     <row r="30" spans="2:7">
@@ -4079,7 +4079,7 @@
         <v>48</v>
       </c>
       <c r="C34" s="14" t="s">
-        <v>546</v>
+        <v>544</v>
       </c>
       <c r="E34" s="27" t="s">
         <v>466</v>
@@ -4090,10 +4090,10 @@
         <v>57</v>
       </c>
       <c r="C35" s="14" t="s">
-        <v>547</v>
+        <v>545</v>
       </c>
       <c r="E35" s="28" t="s">
-        <v>634</v>
+        <v>632</v>
       </c>
     </row>
     <row r="36" spans="2:5">
@@ -4101,7 +4101,7 @@
         <v>61</v>
       </c>
       <c r="C36" s="14" t="s">
-        <v>548</v>
+        <v>546</v>
       </c>
       <c r="E36" s="20"/>
     </row>
@@ -4119,7 +4119,7 @@
         <v>68</v>
       </c>
       <c r="C38" s="14" t="s">
-        <v>549</v>
+        <v>547</v>
       </c>
       <c r="E38" s="19"/>
     </row>
@@ -4144,7 +4144,7 @@
         <v>76</v>
       </c>
       <c r="C41" s="14" t="s">
-        <v>550</v>
+        <v>548</v>
       </c>
     </row>
     <row r="42" spans="2:5">
@@ -4152,7 +4152,7 @@
         <v>65</v>
       </c>
       <c r="C42" s="14" t="s">
-        <v>551</v>
+        <v>549</v>
       </c>
     </row>
     <row r="43" spans="2:5">
@@ -4160,7 +4160,7 @@
         <v>75</v>
       </c>
       <c r="C43" s="14" t="s">
-        <v>552</v>
+        <v>550</v>
       </c>
     </row>
     <row r="44" spans="2:5">
@@ -4168,15 +4168,15 @@
         <v>66</v>
       </c>
       <c r="C44" s="14" t="s">
-        <v>553</v>
+        <v>551</v>
       </c>
     </row>
     <row r="45" spans="2:5">
       <c r="B45" s="25" t="s">
-        <v>653</v>
+        <v>651</v>
       </c>
       <c r="C45" s="14" t="s">
-        <v>554</v>
+        <v>552</v>
       </c>
     </row>
     <row r="46" spans="2:5">
@@ -4184,7 +4184,7 @@
         <v>83</v>
       </c>
       <c r="C46" s="14" t="s">
-        <v>555</v>
+        <v>553</v>
       </c>
     </row>
     <row r="47" spans="2:5">
@@ -4248,7 +4248,7 @@
         <v>73</v>
       </c>
       <c r="C54" s="14" t="s">
-        <v>556</v>
+        <v>554</v>
       </c>
     </row>
     <row r="55" spans="2:3">
@@ -4264,7 +4264,7 @@
         <v>74</v>
       </c>
       <c r="C56" s="14" t="s">
-        <v>557</v>
+        <v>555</v>
       </c>
     </row>
     <row r="57" spans="2:3">
@@ -4296,7 +4296,7 @@
         <v>107</v>
       </c>
       <c r="C60" s="14" t="s">
-        <v>558</v>
+        <v>556</v>
       </c>
     </row>
     <row r="61" spans="2:3">
@@ -4352,7 +4352,7 @@
         <v>103</v>
       </c>
       <c r="C67" s="14" t="s">
-        <v>559</v>
+        <v>557</v>
       </c>
     </row>
     <row r="68" spans="2:3">
@@ -4360,7 +4360,7 @@
         <v>87</v>
       </c>
       <c r="C68" s="14" t="s">
-        <v>560</v>
+        <v>558</v>
       </c>
     </row>
     <row r="69" spans="2:3">
@@ -4368,7 +4368,7 @@
         <v>100</v>
       </c>
       <c r="C69" s="14" t="s">
-        <v>561</v>
+        <v>559</v>
       </c>
     </row>
     <row r="70" spans="2:3">
@@ -4376,7 +4376,7 @@
         <v>89</v>
       </c>
       <c r="C70" s="14" t="s">
-        <v>562</v>
+        <v>560</v>
       </c>
     </row>
     <row r="71" spans="2:3">
@@ -4384,7 +4384,7 @@
         <v>96</v>
       </c>
       <c r="C71" s="14" t="s">
-        <v>563</v>
+        <v>561</v>
       </c>
     </row>
     <row r="72" spans="2:3">
@@ -4400,7 +4400,7 @@
         <v>117</v>
       </c>
       <c r="C73" s="14" t="s">
-        <v>564</v>
+        <v>562</v>
       </c>
     </row>
     <row r="74" spans="2:3">
@@ -4408,7 +4408,7 @@
         <v>129</v>
       </c>
       <c r="C74" s="14" t="s">
-        <v>565</v>
+        <v>563</v>
       </c>
     </row>
     <row r="75" spans="2:3">
@@ -4416,7 +4416,7 @@
         <v>132</v>
       </c>
       <c r="C75" s="14" t="s">
-        <v>566</v>
+        <v>564</v>
       </c>
     </row>
     <row r="76" spans="2:3">
@@ -4432,7 +4432,7 @@
         <v>133</v>
       </c>
       <c r="C77" s="14" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
     </row>
     <row r="78" spans="2:3">
@@ -4440,7 +4440,7 @@
         <v>114</v>
       </c>
       <c r="C78" s="14" t="s">
-        <v>568</v>
+        <v>566</v>
       </c>
     </row>
     <row r="79" spans="2:3">
@@ -4464,7 +4464,7 @@
         <v>121</v>
       </c>
       <c r="C81" s="14" t="s">
-        <v>569</v>
+        <v>567</v>
       </c>
     </row>
     <row r="82" spans="2:3">
@@ -4496,7 +4496,7 @@
         <v>127</v>
       </c>
       <c r="C85" s="14" t="s">
-        <v>570</v>
+        <v>568</v>
       </c>
     </row>
     <row r="86" spans="2:3">
@@ -4544,7 +4544,7 @@
         <v>136</v>
       </c>
       <c r="C91" s="14" t="s">
-        <v>571</v>
+        <v>569</v>
       </c>
     </row>
     <row r="92" spans="2:3">
@@ -4576,7 +4576,7 @@
         <v>141</v>
       </c>
       <c r="C95" s="14" t="s">
-        <v>572</v>
+        <v>570</v>
       </c>
     </row>
     <row r="96" spans="2:3">
@@ -4584,7 +4584,7 @@
         <v>138</v>
       </c>
       <c r="C96" s="14" t="s">
-        <v>573</v>
+        <v>571</v>
       </c>
     </row>
     <row r="97" spans="2:3">
@@ -4600,7 +4600,7 @@
         <v>146</v>
       </c>
       <c r="C98" s="14" t="s">
-        <v>574</v>
+        <v>572</v>
       </c>
     </row>
     <row r="99" spans="2:3">
@@ -4624,7 +4624,7 @@
         <v>150</v>
       </c>
       <c r="C101" s="14" t="s">
-        <v>575</v>
+        <v>573</v>
       </c>
     </row>
     <row r="102" spans="2:3">
@@ -4632,7 +4632,7 @@
         <v>152</v>
       </c>
       <c r="C102" s="14" t="s">
-        <v>576</v>
+        <v>574</v>
       </c>
     </row>
     <row r="103" spans="2:3">
@@ -4640,7 +4640,7 @@
         <v>148</v>
       </c>
       <c r="C103" s="14" t="s">
-        <v>577</v>
+        <v>575</v>
       </c>
     </row>
     <row r="104" spans="2:3">
@@ -4664,7 +4664,7 @@
         <v>153</v>
       </c>
       <c r="C106" s="14" t="s">
-        <v>578</v>
+        <v>576</v>
       </c>
     </row>
     <row r="107" spans="2:3">
@@ -4688,7 +4688,7 @@
         <v>154</v>
       </c>
       <c r="C109" s="14" t="s">
-        <v>579</v>
+        <v>577</v>
       </c>
     </row>
     <row r="110" spans="2:3">
@@ -4704,7 +4704,7 @@
         <v>163</v>
       </c>
       <c r="C111" s="14" t="s">
-        <v>580</v>
+        <v>578</v>
       </c>
     </row>
     <row r="112" spans="2:3">
@@ -4712,7 +4712,7 @@
         <v>165</v>
       </c>
       <c r="C112" s="14" t="s">
-        <v>581</v>
+        <v>579</v>
       </c>
     </row>
     <row r="113" spans="2:3">
@@ -4760,7 +4760,7 @@
         <v>177</v>
       </c>
       <c r="C118" s="14" t="s">
-        <v>582</v>
+        <v>580</v>
       </c>
     </row>
     <row r="119" spans="2:3">
@@ -4784,7 +4784,7 @@
         <v>180</v>
       </c>
       <c r="C121" s="14" t="s">
-        <v>583</v>
+        <v>581</v>
       </c>
     </row>
     <row r="122" spans="2:3">
@@ -4792,7 +4792,7 @@
         <v>470</v>
       </c>
       <c r="C122" s="14" t="s">
-        <v>584</v>
+        <v>582</v>
       </c>
     </row>
     <row r="123" spans="2:3">
@@ -4808,7 +4808,7 @@
         <v>188</v>
       </c>
       <c r="C124" s="14" t="s">
-        <v>585</v>
+        <v>583</v>
       </c>
     </row>
     <row r="125" spans="2:3">
@@ -4864,7 +4864,7 @@
         <v>193</v>
       </c>
       <c r="C131" s="14" t="s">
-        <v>586</v>
+        <v>584</v>
       </c>
     </row>
     <row r="132" spans="2:3">
@@ -4904,7 +4904,7 @@
         <v>198</v>
       </c>
       <c r="C136" s="14" t="s">
-        <v>587</v>
+        <v>585</v>
       </c>
     </row>
     <row r="137" spans="2:3">
@@ -4912,7 +4912,7 @@
         <v>196</v>
       </c>
       <c r="C137" s="14" t="s">
-        <v>588</v>
+        <v>586</v>
       </c>
     </row>
     <row r="138" spans="2:3">
@@ -4944,7 +4944,7 @@
         <v>204</v>
       </c>
       <c r="C141" s="14" t="s">
-        <v>589</v>
+        <v>587</v>
       </c>
     </row>
     <row r="142" spans="2:3">
@@ -4952,7 +4952,7 @@
         <v>195</v>
       </c>
       <c r="C142" s="14" t="s">
-        <v>590</v>
+        <v>588</v>
       </c>
     </row>
     <row r="143" spans="2:3">
@@ -4960,7 +4960,7 @@
         <v>208</v>
       </c>
       <c r="C143" s="14" t="s">
-        <v>591</v>
+        <v>589</v>
       </c>
     </row>
     <row r="144" spans="2:3">
@@ -4968,7 +4968,7 @@
         <v>211</v>
       </c>
       <c r="C144" s="14" t="s">
-        <v>592</v>
+        <v>590</v>
       </c>
     </row>
     <row r="145" spans="2:3">
@@ -5008,7 +5008,7 @@
         <v>215</v>
       </c>
       <c r="C149" s="14" t="s">
-        <v>593</v>
+        <v>591</v>
       </c>
     </row>
     <row r="150" spans="2:3">
@@ -5016,7 +5016,7 @@
         <v>220</v>
       </c>
       <c r="C150" s="14" t="s">
-        <v>594</v>
+        <v>592</v>
       </c>
     </row>
     <row r="151" spans="2:3">
@@ -5024,15 +5024,15 @@
         <v>222</v>
       </c>
       <c r="C151" s="14" t="s">
-        <v>595</v>
+        <v>593</v>
       </c>
     </row>
     <row r="152" spans="2:3">
       <c r="B152" s="14" t="s">
-        <v>622</v>
+        <v>620</v>
       </c>
       <c r="C152" s="14" t="s">
-        <v>596</v>
+        <v>594</v>
       </c>
     </row>
     <row r="153" spans="2:3">
@@ -5040,7 +5040,7 @@
         <v>224</v>
       </c>
       <c r="C153" s="14" t="s">
-        <v>597</v>
+        <v>595</v>
       </c>
     </row>
     <row r="154" spans="2:3">
@@ -5048,7 +5048,7 @@
         <v>239</v>
       </c>
       <c r="C154" s="14" t="s">
-        <v>598</v>
+        <v>596</v>
       </c>
     </row>
     <row r="155" spans="2:3">
@@ -5072,7 +5072,7 @@
         <v>225</v>
       </c>
       <c r="C157" s="14" t="s">
-        <v>599</v>
+        <v>597</v>
       </c>
     </row>
     <row r="158" spans="2:3">
@@ -5088,7 +5088,7 @@
         <v>231</v>
       </c>
       <c r="C159" s="14" t="s">
-        <v>600</v>
+        <v>598</v>
       </c>
     </row>
     <row r="160" spans="2:3">
@@ -5096,7 +5096,7 @@
         <v>232</v>
       </c>
       <c r="C160" s="14" t="s">
-        <v>601</v>
+        <v>599</v>
       </c>
     </row>
     <row r="161" spans="2:3">
@@ -5104,7 +5104,7 @@
         <v>241</v>
       </c>
       <c r="C161" s="14" t="s">
-        <v>602</v>
+        <v>600</v>
       </c>
     </row>
     <row r="162" spans="2:3">
@@ -5128,7 +5128,7 @@
         <v>257</v>
       </c>
       <c r="C164" s="14" t="s">
-        <v>603</v>
+        <v>601</v>
       </c>
     </row>
     <row r="165" spans="2:3">
@@ -5144,7 +5144,7 @@
         <v>249</v>
       </c>
       <c r="C166" s="14" t="s">
-        <v>604</v>
+        <v>602</v>
       </c>
     </row>
     <row r="167" spans="2:3">
@@ -5152,7 +5152,7 @@
         <v>243</v>
       </c>
       <c r="C167" s="14" t="s">
-        <v>605</v>
+        <v>603</v>
       </c>
     </row>
     <row r="168" spans="2:3">
@@ -5160,7 +5160,7 @@
         <v>252</v>
       </c>
       <c r="C168" s="14" t="s">
-        <v>606</v>
+        <v>604</v>
       </c>
     </row>
     <row r="169" spans="2:3">
@@ -5168,7 +5168,7 @@
         <v>255</v>
       </c>
       <c r="C169" s="14" t="s">
-        <v>607</v>
+        <v>605</v>
       </c>
     </row>
     <row r="170" spans="2:3">
@@ -5176,7 +5176,7 @@
         <v>235</v>
       </c>
       <c r="C170" s="14" t="s">
-        <v>608</v>
+        <v>606</v>
       </c>
     </row>
     <row r="171" spans="2:3">
@@ -5184,7 +5184,7 @@
         <v>245</v>
       </c>
       <c r="C171" s="14" t="s">
-        <v>609</v>
+        <v>607</v>
       </c>
     </row>
     <row r="172" spans="2:3">
@@ -5192,7 +5192,7 @@
         <v>253</v>
       </c>
       <c r="C172" s="14" t="s">
-        <v>610</v>
+        <v>608</v>
       </c>
     </row>
     <row r="173" spans="2:3">
@@ -5216,7 +5216,7 @@
         <v>230</v>
       </c>
       <c r="C175" s="14" t="s">
-        <v>611</v>
+        <v>609</v>
       </c>
     </row>
     <row r="176" spans="2:3">
@@ -5224,7 +5224,7 @@
         <v>259</v>
       </c>
       <c r="C176" s="14" t="s">
-        <v>612</v>
+        <v>610</v>
       </c>
     </row>
     <row r="177" spans="2:3">
@@ -5232,7 +5232,7 @@
         <v>227</v>
       </c>
       <c r="C177" s="14" t="s">
-        <v>613</v>
+        <v>611</v>
       </c>
     </row>
     <row r="178" spans="2:3">
@@ -5240,7 +5240,7 @@
         <v>226</v>
       </c>
       <c r="C178" s="14" t="s">
-        <v>614</v>
+        <v>612</v>
       </c>
     </row>
     <row r="179" spans="2:3">
@@ -5248,7 +5248,7 @@
         <v>240</v>
       </c>
       <c r="C179" s="14" t="s">
-        <v>615</v>
+        <v>613</v>
       </c>
     </row>
     <row r="180" spans="2:3">
@@ -5256,7 +5256,7 @@
         <v>270</v>
       </c>
       <c r="C180" s="14" t="s">
-        <v>616</v>
+        <v>614</v>
       </c>
     </row>
     <row r="181" spans="2:3">
@@ -5264,7 +5264,7 @@
         <v>275</v>
       </c>
       <c r="C181" s="14" t="s">
-        <v>617</v>
+        <v>615</v>
       </c>
     </row>
     <row r="182" spans="2:3">
@@ -5272,7 +5272,7 @@
         <v>268</v>
       </c>
       <c r="C182" s="14" t="s">
-        <v>618</v>
+        <v>616</v>
       </c>
     </row>
     <row r="183" spans="2:3">
@@ -5280,7 +5280,7 @@
         <v>267</v>
       </c>
       <c r="C183" s="14" t="s">
-        <v>619</v>
+        <v>617</v>
       </c>
     </row>
     <row r="184" spans="2:3">
@@ -5288,7 +5288,7 @@
         <v>271</v>
       </c>
       <c r="C184" s="14" t="s">
-        <v>620</v>
+        <v>618</v>
       </c>
     </row>
     <row r="185" spans="2:3">
@@ -5296,7 +5296,7 @@
         <v>272</v>
       </c>
       <c r="C185" s="14" t="s">
-        <v>621</v>
+        <v>619</v>
       </c>
     </row>
     <row r="186" spans="2:3">
@@ -5914,8 +5914,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H63"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -5948,13 +5948,13 @@
         <v>349</v>
       </c>
       <c r="F1" s="6" t="s">
-        <v>635</v>
+        <v>633</v>
       </c>
       <c r="G1" s="6" t="s">
+        <v>634</v>
+      </c>
+      <c r="H1" s="6" t="s">
         <v>636</v>
-      </c>
-      <c r="H1" s="6" t="s">
-        <v>638</v>
       </c>
     </row>
     <row r="2" spans="1:8">
@@ -5974,18 +5974,18 @@
         <v>497</v>
       </c>
       <c r="F2" t="s">
+        <v>637</v>
+      </c>
+      <c r="G2" t="s">
+        <v>638</v>
+      </c>
+      <c r="H2" s="23" t="s">
         <v>639</v>
-      </c>
-      <c r="G2" t="s">
-        <v>640</v>
-      </c>
-      <c r="H2" s="23" t="s">
-        <v>641</v>
       </c>
     </row>
     <row r="3" spans="1:8">
       <c r="A3" s="7" t="s">
-        <v>526</v>
+        <v>654</v>
       </c>
       <c r="B3" s="8" t="s">
         <v>340</v>
@@ -6000,18 +6000,18 @@
         <v>499</v>
       </c>
       <c r="F3" t="s">
+        <v>640</v>
+      </c>
+      <c r="G3" t="s">
+        <v>641</v>
+      </c>
+      <c r="H3" s="23" t="s">
         <v>642</v>
-      </c>
-      <c r="G3" t="s">
-        <v>643</v>
-      </c>
-      <c r="H3" s="23" t="s">
-        <v>644</v>
       </c>
     </row>
     <row r="4" spans="1:8">
       <c r="A4" s="2" t="s">
-        <v>527</v>
+        <v>655</v>
       </c>
       <c r="B4" s="8" t="s">
         <v>364</v>
@@ -6026,13 +6026,13 @@
         <v>500</v>
       </c>
       <c r="F4" t="s">
+        <v>643</v>
+      </c>
+      <c r="G4" t="s">
+        <v>644</v>
+      </c>
+      <c r="H4" s="23" t="s">
         <v>645</v>
-      </c>
-      <c r="G4" t="s">
-        <v>646</v>
-      </c>
-      <c r="H4" s="23" t="s">
-        <v>647</v>
       </c>
     </row>
     <row r="5" spans="1:8">
@@ -6049,11 +6049,11 @@
         <v>498</v>
       </c>
       <c r="F5" t="s">
-        <v>648</v>
+        <v>646</v>
       </c>
       <c r="G5"/>
       <c r="H5" s="23" t="s">
-        <v>649</v>
+        <v>647</v>
       </c>
     </row>
     <row r="6" spans="1:8">
@@ -6067,11 +6067,11 @@
         <v>369</v>
       </c>
       <c r="F6" t="s">
-        <v>650</v>
+        <v>648</v>
       </c>
       <c r="G6"/>
       <c r="H6" s="23" t="s">
-        <v>651</v>
+        <v>649</v>
       </c>
     </row>
     <row r="7" spans="1:8">
@@ -6086,7 +6086,7 @@
       </c>
       <c r="G7"/>
       <c r="H7" s="23" t="s">
-        <v>652</v>
+        <v>650</v>
       </c>
     </row>
     <row r="8" spans="1:8">

</xml_diff>